<commit_message>
Recreating NPS 2024 excel
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/NPS2024/DoD_2024_NPS.xlsx
+++ b/Output/AcqTrends/NPS2024/DoD_2024_NPS.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="1 Budg" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="1 K&amp;Ota" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t xml:space="preserve">source</t>
   </si>
@@ -157,14 +158,48 @@
   </si>
   <si>
     <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">AreaType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SimpleAreaType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTA for Production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Products and Production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract for Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTA for Prototype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R&amp;D and Prototypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract for R&amp;D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract for Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unlabeled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00,,,&quot;B&quot;"/>
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -200,9 +235,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,11 +1182,1915 @@
       <c r="AZ6" s="1" t="str">
         <f>Sum(AZ2:AZ5)</f>
       </c>
-      <c r="BA6" s="1"/>
+      <c r="BA6" s="1" t="str">
+        <f>Sum(BA2:BA5)</f>
+      </c>
       <c r="BB6" s="1"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <f>M9</f>
+      </c>
+      <c r="B9" t="str">
+        <f>N9</f>
+      </c>
+      <c r="C9" t="str">
+        <f>AS9</f>
+      </c>
+      <c r="D9" t="str">
+        <f>AU9</f>
+      </c>
+      <c r="E9" t="str">
+        <f>AV9</f>
+      </c>
+      <c r="G9" t="str">
+        <f>AU9&amp;"-"&amp;AV9</f>
+      </c>
+      <c r="H9" t="str">
+        <f>AS9&amp;"-"&amp;AV9</f>
+      </c>
+      <c r="J9" t="str">
+        <f>"Share "&amp;AV9</f>
+      </c>
+      <c r="M9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>4</v>
+      </c>
+      <c r="R9" t="s">
+        <v>5</v>
+      </c>
+      <c r="S9" t="s">
+        <v>6</v>
+      </c>
+      <c r="T9" t="s">
+        <v>7</v>
+      </c>
+      <c r="U9" t="s">
+        <v>8</v>
+      </c>
+      <c r="V9" t="s">
+        <v>9</v>
+      </c>
+      <c r="W9" t="s">
+        <v>10</v>
+      </c>
+      <c r="X9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <f>M10</f>
+      </c>
+      <c r="B10" t="str">
+        <f>N10</f>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>AS10</f>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>AU10</f>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f>AV10</f>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2" t="str">
+        <f>AV10/AU10-1</f>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f>AV10/AS10-1</f>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="str">
+        <f>AV10/Sum(AV$9:AV$13)</f>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="M10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1" t="n">
+        <v>36390869420.0532</v>
+      </c>
+      <c r="AL10" s="1" t="n">
+        <v>25896384490.0193</v>
+      </c>
+      <c r="AM10" s="1" t="n">
+        <v>19992431792.9514</v>
+      </c>
+      <c r="AN10" s="1" t="n">
+        <v>30286399449.1285</v>
+      </c>
+      <c r="AO10" s="1" t="n">
+        <v>41815605260.499</v>
+      </c>
+      <c r="AP10" s="1" t="n">
+        <v>37884999724.2074</v>
+      </c>
+      <c r="AQ10" s="1" t="n">
+        <v>41573208124.9344</v>
+      </c>
+      <c r="AR10" s="1" t="n">
+        <v>44992590026.8429</v>
+      </c>
+      <c r="AS10" s="1" t="n">
+        <v>57987138191.6318</v>
+      </c>
+      <c r="AT10" s="1" t="n">
+        <v>27730527616.1122</v>
+      </c>
+      <c r="AU10" s="1" t="n">
+        <v>40499381567.492</v>
+      </c>
+      <c r="AV10" s="1" t="n">
+        <v>65793606575.0316</v>
+      </c>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <f>M11</f>
+      </c>
+      <c r="B11" t="str">
+        <f>N11</f>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>AS11</f>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>AU11</f>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f>AV11</f>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2" t="str">
+        <f>AV11/AU11-1</f>
+      </c>
+      <c r="H11" s="2" t="str">
+        <f>AV11/AS11-1</f>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="str">
+        <f>AV11/Sum(AV$9:AV$13)</f>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="M11" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1" t="n">
+        <v>432330186054.03</v>
+      </c>
+      <c r="AL11" s="1" t="n">
+        <v>368750341721.862</v>
+      </c>
+      <c r="AM11" s="1" t="n">
+        <v>338132277217.976</v>
+      </c>
+      <c r="AN11" s="1" t="n">
+        <v>312773586648.454</v>
+      </c>
+      <c r="AO11" s="1" t="n">
+        <v>328542572360.358</v>
+      </c>
+      <c r="AP11" s="1" t="n">
+        <v>353490764546.252</v>
+      </c>
+      <c r="AQ11" s="1" t="n">
+        <v>387087885833.412</v>
+      </c>
+      <c r="AR11" s="1" t="n">
+        <v>405081653062.029</v>
+      </c>
+      <c r="AS11" s="1" t="n">
+        <v>431127980837.866</v>
+      </c>
+      <c r="AT11" s="1" t="n">
+        <v>405348242639.538</v>
+      </c>
+      <c r="AU11" s="1" t="n">
+        <v>392694446194.055</v>
+      </c>
+      <c r="AV11" s="1" t="n">
+        <v>390453368175.855</v>
+      </c>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <f>M12</f>
+      </c>
+      <c r="B12" t="str">
+        <f>N12</f>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>AS12</f>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>AU12</f>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f>AV12</f>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2" t="str">
+        <f>AV12/AU12-1</f>
+      </c>
+      <c r="H12" s="2" t="str">
+        <f>AV12/AS12-1</f>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="str">
+        <f>AV12/Sum(AV$9:AV$13)</f>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="M12" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>248917998790.874</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>271885202720.129</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>240412560734.939</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>231031479111.987</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>218250472650.085</v>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>212677633977.603</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <v>212071611328.834</v>
+      </c>
+      <c r="V12" s="1" t="n">
+        <v>204034317412.979</v>
+      </c>
+      <c r="W12" s="1" t="n">
+        <v>203216983313.484</v>
+      </c>
+      <c r="X12" s="1" t="n">
+        <v>209688280565.4</v>
+      </c>
+      <c r="Y12" s="1" t="n">
+        <v>222214954426.99</v>
+      </c>
+      <c r="Z12" s="1" t="n">
+        <v>236349380759.976</v>
+      </c>
+      <c r="AA12" s="1" t="n">
+        <v>274407867785.644</v>
+      </c>
+      <c r="AB12" s="1" t="n">
+        <v>335392180495.053</v>
+      </c>
+      <c r="AC12" s="1" t="n">
+        <v>355611032054.797</v>
+      </c>
+      <c r="AD12" s="1" t="n">
+        <v>399034409966.236</v>
+      </c>
+      <c r="AE12" s="1" t="n">
+        <v>429398322936.051</v>
+      </c>
+      <c r="AF12" s="1" t="n">
+        <v>464598647461.156</v>
+      </c>
+      <c r="AG12" s="1" t="n">
+        <v>524270052465.528</v>
+      </c>
+      <c r="AH12" s="1" t="n">
+        <v>523860817748.021</v>
+      </c>
+      <c r="AI12" s="1" t="n">
+        <v>493294382841.294</v>
+      </c>
+      <c r="AJ12" s="1" t="n">
+        <v>491810684195.121</v>
+      </c>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1" t="n">
+        <v>7816340.87652611</v>
+      </c>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <f>M13</f>
+      </c>
+      <c r="B13" t="str">
+        <f>N13</f>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>AS13</f>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>AU13</f>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f>AV13</f>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2" t="str">
+        <f>AV13/AU13-1</f>
+      </c>
+      <c r="H13" s="2" t="str">
+        <f>AV13/AS13-1</f>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="str">
+        <f>AV13/Sum(AV$9:AV$13)</f>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="M13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13" t="s">
+        <v>43</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>602606352101.694</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>620274552583.297</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>555597728301.067</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>513282174398.476</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>468197035636.694</v>
+      </c>
+      <c r="T13" s="1" t="n">
+        <v>463718246766.96</v>
+      </c>
+      <c r="U13" s="1" t="n">
+        <v>456647075846.094</v>
+      </c>
+      <c r="V13" s="1" t="n">
+        <v>447160758493.617</v>
+      </c>
+      <c r="W13" s="1" t="n">
+        <v>450201318466.152</v>
+      </c>
+      <c r="X13" s="1" t="n">
+        <v>468044833590.874</v>
+      </c>
+      <c r="Y13" s="1" t="n">
+        <v>482426154042.693</v>
+      </c>
+      <c r="Z13" s="1" t="n">
+        <v>519564848435.905</v>
+      </c>
+      <c r="AA13" s="1" t="n">
+        <v>574278428296.36</v>
+      </c>
+      <c r="AB13" s="1" t="n">
+        <v>686572797072.324</v>
+      </c>
+      <c r="AC13" s="1" t="n">
+        <v>705848454956.435</v>
+      </c>
+      <c r="AD13" s="1" t="n">
+        <v>754734162091.152</v>
+      </c>
+      <c r="AE13" s="1" t="n">
+        <v>780154010413.381</v>
+      </c>
+      <c r="AF13" s="1" t="n">
+        <v>854960044741.897</v>
+      </c>
+      <c r="AG13" s="1" t="n">
+        <v>928290961219.569</v>
+      </c>
+      <c r="AH13" s="1" t="n">
+        <v>914201464665.633</v>
+      </c>
+      <c r="AI13" s="1" t="n">
+        <v>941647271844.871</v>
+      </c>
+      <c r="AJ13" s="1" t="n">
+        <v>919517495559.997</v>
+      </c>
+      <c r="AK13" s="1" t="n">
+        <v>854893667495.288</v>
+      </c>
+      <c r="AL13" s="1" t="n">
+        <v>753547648271.248</v>
+      </c>
+      <c r="AM13" s="1" t="n">
+        <v>734730935805.295</v>
+      </c>
+      <c r="AN13" s="1" t="n">
+        <v>707449202632.779</v>
+      </c>
+      <c r="AO13" s="1" t="n">
+        <v>729860428011.978</v>
+      </c>
+      <c r="AP13" s="1" t="n">
+        <v>743756641042.876</v>
+      </c>
+      <c r="AQ13" s="1" t="n">
+        <v>803641431930.826</v>
+      </c>
+      <c r="AR13" s="1" t="n">
+        <v>812550495675.43</v>
+      </c>
+      <c r="AS13" s="1" t="n">
+        <v>839984421891.179</v>
+      </c>
+      <c r="AT13" s="1" t="n">
+        <v>795568567643.196</v>
+      </c>
+      <c r="AU13" s="1" t="n">
+        <v>804667494998.361</v>
+      </c>
+      <c r="AV13" s="1" t="n">
+        <v>853072000000</v>
+      </c>
+      <c r="AW13" s="1" t="n">
+        <v>820251376580.069</v>
+      </c>
+      <c r="AX13" s="1" t="n">
+        <v>819313863553.375</v>
+      </c>
+      <c r="AY13" s="1" t="n">
+        <v>819450662554.299</v>
+      </c>
+      <c r="AZ13" s="1" t="n">
+        <v>819548057151.466</v>
+      </c>
+      <c r="BA13" s="1" t="n">
+        <v>819669680013.5</v>
+      </c>
+      <c r="BB13" s="1"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <f>M14</f>
+      </c>
+      <c r="B14" t="str">
+        <f>N14</f>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>AS14</f>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>AU14</f>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f>AV14</f>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2" t="str">
+        <f>AV14/AU14-1</f>
+      </c>
+      <c r="H14" s="2" t="str">
+        <f>AV14/AS14-1</f>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="str">
+        <f>Sum(J$9:J$13)</f>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="M14" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="1" t="str">
+        <f>Sum(O10:O13)</f>
+      </c>
+      <c r="P14" s="1" t="str">
+        <f>Sum(P10:P13)</f>
+      </c>
+      <c r="Q14" s="1" t="str">
+        <f>Sum(Q10:Q13)</f>
+      </c>
+      <c r="R14" s="1" t="str">
+        <f>Sum(R10:R13)</f>
+      </c>
+      <c r="S14" s="1" t="str">
+        <f>Sum(S10:S13)</f>
+      </c>
+      <c r="T14" s="1" t="str">
+        <f>Sum(T10:T13)</f>
+      </c>
+      <c r="U14" s="1" t="str">
+        <f>Sum(U10:U13)</f>
+      </c>
+      <c r="V14" s="1" t="str">
+        <f>Sum(V10:V13)</f>
+      </c>
+      <c r="W14" s="1" t="str">
+        <f>Sum(W10:W13)</f>
+      </c>
+      <c r="X14" s="1" t="str">
+        <f>Sum(X10:X13)</f>
+      </c>
+      <c r="Y14" s="1" t="str">
+        <f>Sum(Y10:Y13)</f>
+      </c>
+      <c r="Z14" s="1" t="str">
+        <f>Sum(Z10:Z13)</f>
+      </c>
+      <c r="AA14" s="1" t="str">
+        <f>Sum(AA10:AA13)</f>
+      </c>
+      <c r="AB14" s="1" t="str">
+        <f>Sum(AB10:AB13)</f>
+      </c>
+      <c r="AC14" s="1" t="str">
+        <f>Sum(AC10:AC13)</f>
+      </c>
+      <c r="AD14" s="1" t="str">
+        <f>Sum(AD10:AD13)</f>
+      </c>
+      <c r="AE14" s="1" t="str">
+        <f>Sum(AE10:AE13)</f>
+      </c>
+      <c r="AF14" s="1" t="str">
+        <f>Sum(AF10:AF13)</f>
+      </c>
+      <c r="AG14" s="1" t="str">
+        <f>Sum(AG10:AG13)</f>
+      </c>
+      <c r="AH14" s="1" t="str">
+        <f>Sum(AH10:AH13)</f>
+      </c>
+      <c r="AI14" s="1" t="str">
+        <f>Sum(AI10:AI13)</f>
+      </c>
+      <c r="AJ14" s="1" t="str">
+        <f>Sum(AJ10:AJ13)</f>
+      </c>
+      <c r="AK14" s="1" t="str">
+        <f>Sum(AK10:AK13)</f>
+      </c>
+      <c r="AL14" s="1" t="str">
+        <f>Sum(AL10:AL13)</f>
+      </c>
+      <c r="AM14" s="1" t="str">
+        <f>Sum(AM10:AM13)</f>
+      </c>
+      <c r="AN14" s="1" t="str">
+        <f>Sum(AN10:AN13)</f>
+      </c>
+      <c r="AO14" s="1" t="str">
+        <f>Sum(AO10:AO13)</f>
+      </c>
+      <c r="AP14" s="1" t="str">
+        <f>Sum(AP10:AP13)</f>
+      </c>
+      <c r="AQ14" s="1" t="str">
+        <f>Sum(AQ10:AQ13)</f>
+      </c>
+      <c r="AR14" s="1" t="str">
+        <f>Sum(AR10:AR13)</f>
+      </c>
+      <c r="AS14" s="1" t="str">
+        <f>Sum(AS10:AS13)</f>
+      </c>
+      <c r="AT14" s="1" t="str">
+        <f>Sum(AT10:AT13)</f>
+      </c>
+      <c r="AU14" s="1" t="str">
+        <f>Sum(AU10:AU13)</f>
+      </c>
+      <c r="AV14" s="1" t="str">
+        <f>Sum(AV10:AV13)</f>
+      </c>
+      <c r="AW14" s="1" t="str">
+        <f>Sum(AW10:AW13)</f>
+      </c>
+      <c r="AX14" s="1" t="str">
+        <f>Sum(AX10:AX13)</f>
+      </c>
+      <c r="AY14" s="1" t="str">
+        <f>Sum(AY10:AY13)</f>
+      </c>
+      <c r="AZ14" s="1" t="str">
+        <f>Sum(AZ10:AZ13)</f>
+      </c>
+      <c r="BA14" s="1" t="str">
+        <f>Sum(BA10:BA13)</f>
+      </c>
+      <c r="BB14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" xSplit="2" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <f>M1</f>
+      </c>
+      <c r="B1" t="str">
+        <f>N1</f>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <f>M2</f>
+      </c>
+      <c r="B2" t="str">
+        <f>N2</f>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3" t="n">
+        <v>1003576.97</v>
+      </c>
+      <c r="T2" s="3" t="n">
+        <v>357061685.3</v>
+      </c>
+      <c r="U2" s="3" t="n">
+        <v>1079497813.63</v>
+      </c>
+      <c r="V2" s="3" t="n">
+        <v>1009757071.82</v>
+      </c>
+      <c r="W2" s="3" t="n">
+        <v>2082784769.7</v>
+      </c>
+      <c r="X2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <f>M3</f>
+      </c>
+      <c r="B3" t="str">
+        <f>N3</f>
+      </c>
+      <c r="M3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>129800148412.8</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>148647289683.223</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>163617709805.785</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <v>183152473080.586</v>
+      </c>
+      <c r="S3" s="3" t="n">
+        <v>192794964659.917</v>
+      </c>
+      <c r="T3" s="3" t="n">
+        <v>218384238186.164</v>
+      </c>
+      <c r="U3" s="3" t="n">
+        <v>193995037853.426</v>
+      </c>
+      <c r="V3" s="3" t="n">
+        <v>209676052547.551</v>
+      </c>
+      <c r="W3" s="3" t="n">
+        <v>225642793034.253</v>
+      </c>
+      <c r="X3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <f>M4</f>
+      </c>
+      <c r="B4" t="str">
+        <f>N4</f>
+      </c>
+      <c r="M4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>694883317.68</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>1433156330.3</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>2115488321.87</v>
+      </c>
+      <c r="R4" s="3" t="n">
+        <v>3953909229.18</v>
+      </c>
+      <c r="S4" s="3" t="n">
+        <v>7210412511.82</v>
+      </c>
+      <c r="T4" s="3" t="n">
+        <v>15977844023.82</v>
+      </c>
+      <c r="U4" s="3" t="n">
+        <v>13587248379.41</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <v>9970880441.6</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <v>13597718627.55</v>
+      </c>
+      <c r="X4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <f>M5</f>
+      </c>
+      <c r="B5" t="str">
+        <f>N5</f>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>23781261098.9443</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>24573276196.2158</v>
+      </c>
+      <c r="Q5" s="3" t="n">
+        <v>25597996648.6431</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>27242841176.5787</v>
+      </c>
+      <c r="S5" s="3" t="n">
+        <v>31029627313.4931</v>
+      </c>
+      <c r="T5" s="3" t="n">
+        <v>31730385296.1509</v>
+      </c>
+      <c r="U5" s="3" t="n">
+        <v>32848499043.4238</v>
+      </c>
+      <c r="V5" s="3" t="n">
+        <v>35326395851.8385</v>
+      </c>
+      <c r="W5" s="3" t="n">
+        <v>43247146108.6712</v>
+      </c>
+      <c r="X5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <f>M6</f>
+      </c>
+      <c r="B6" t="str">
+        <f>N6</f>
+      </c>
+      <c r="M6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="3" t="n">
+        <v>120603002254.88</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>125137638219.523</v>
+      </c>
+      <c r="Q6" s="3" t="n">
+        <v>131399208203.59</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>148574738300.029</v>
+      </c>
+      <c r="S6" s="3" t="n">
+        <v>159815344233.307</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>172402223143.601</v>
+      </c>
+      <c r="U6" s="3" t="n">
+        <v>160008849942.056</v>
+      </c>
+      <c r="V6" s="3" t="n">
+        <v>169216514631.91</v>
+      </c>
+      <c r="W6" s="3" t="n">
+        <v>187356782728.035</v>
+      </c>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <f>M7</f>
+      </c>
+      <c r="B7" t="str">
+        <f>N7</f>
+      </c>
+      <c r="M7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" s="3" t="n">
+        <v>30000</v>
+      </c>
+      <c r="P7" s="3" t="n">
+        <v>3581529.4308</v>
+      </c>
+      <c r="Q7" s="3" t="n">
+        <v>1345607</v>
+      </c>
+      <c r="R7" s="3" t="n">
+        <v>-212795.3691</v>
+      </c>
+      <c r="S7" s="3" t="n">
+        <v>465885</v>
+      </c>
+      <c r="T7" s="3" t="n">
+        <v>245000</v>
+      </c>
+      <c r="U7" s="3" t="n">
+        <v>386316</v>
+      </c>
+      <c r="V7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="X7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <f>M8</f>
+      </c>
+      <c r="B8" t="str">
+        <f>N8</f>
+      </c>
+      <c r="M8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="3" t="str">
+        <f>Sum(O2:O7)</f>
+      </c>
+      <c r="P8" s="3" t="str">
+        <f>Sum(P2:P7)</f>
+      </c>
+      <c r="Q8" s="3" t="str">
+        <f>Sum(Q2:Q7)</f>
+      </c>
+      <c r="R8" s="3" t="str">
+        <f>Sum(R2:R7)</f>
+      </c>
+      <c r="S8" s="3" t="str">
+        <f>Sum(S2:S7)</f>
+      </c>
+      <c r="T8" s="3" t="str">
+        <f>Sum(T2:T7)</f>
+      </c>
+      <c r="U8" s="3" t="str">
+        <f>Sum(U2:U7)</f>
+      </c>
+      <c r="V8" s="3" t="str">
+        <f>Sum(V2:V7)</f>
+      </c>
+      <c r="W8" s="3" t="str">
+        <f>Sum(W2:W7)</f>
+      </c>
+      <c r="X8" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <f>M11</f>
+      </c>
+      <c r="B11" t="str">
+        <f>N11</f>
+      </c>
+      <c r="C11" t="str">
+        <f>T11</f>
+      </c>
+      <c r="D11" t="str">
+        <f>V11</f>
+      </c>
+      <c r="E11" t="str">
+        <f>W11</f>
+      </c>
+      <c r="G11" t="str">
+        <f>V11&amp;"-"&amp;W11</f>
+      </c>
+      <c r="H11" t="str">
+        <f>T11&amp;"-"&amp;W11</f>
+      </c>
+      <c r="J11" t="str">
+        <f>"Share "&amp;W11</f>
+      </c>
+      <c r="M11" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" t="s">
+        <v>31</v>
+      </c>
+      <c r="T11" t="s">
+        <v>32</v>
+      </c>
+      <c r="U11" t="s">
+        <v>33</v>
+      </c>
+      <c r="V11" t="s">
+        <v>34</v>
+      </c>
+      <c r="W11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <f>M12</f>
+      </c>
+      <c r="B12" t="str">
+        <f>N12</f>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f>T12</f>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>V12</f>
+      </c>
+      <c r="E12" s="3" t="str">
+        <f>W12</f>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2" t="str">
+        <f>W12/V12-1</f>
+      </c>
+      <c r="H12" s="2" t="str">
+        <f>W12/T12-1</f>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="str">
+        <f>W12/Sum(W$11:W$17)</f>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="M12" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3" t="n">
+        <v>1176703.87838105</v>
+      </c>
+      <c r="T12" s="3" t="n">
+        <v>413259883.550845</v>
+      </c>
+      <c r="U12" s="3" t="n">
+        <v>1207830413.4704</v>
+      </c>
+      <c r="V12" s="3" t="n">
+        <v>1055950019.34882</v>
+      </c>
+      <c r="W12" s="3" t="n">
+        <v>2082784769.7</v>
+      </c>
+      <c r="X12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <f>M13</f>
+      </c>
+      <c r="B13" t="str">
+        <f>N13</f>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>T13</f>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f>V13</f>
+      </c>
+      <c r="E13" s="3" t="str">
+        <f>W13</f>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2" t="str">
+        <f>W13/V13-1</f>
+      </c>
+      <c r="H13" s="2" t="str">
+        <f>W13/T13-1</f>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="str">
+        <f>W13/Sum(W$11:W$17)</f>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="M13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="3" t="n">
+        <v>162409841292.409</v>
+      </c>
+      <c r="P13" s="3" t="n">
+        <v>184516724215.902</v>
+      </c>
+      <c r="Q13" s="3" t="n">
+        <v>199728138398.289</v>
+      </c>
+      <c r="R13" s="3" t="n">
+        <v>218718669353.533</v>
+      </c>
+      <c r="S13" s="3" t="n">
+        <v>226053994291.7</v>
+      </c>
+      <c r="T13" s="3" t="n">
+        <v>252755892210.41</v>
+      </c>
+      <c r="U13" s="3" t="n">
+        <v>217057509355.939</v>
+      </c>
+      <c r="V13" s="3" t="n">
+        <v>219268017945.646</v>
+      </c>
+      <c r="W13" s="3" t="n">
+        <v>225642793034.253</v>
+      </c>
+      <c r="X13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <f>M14</f>
+      </c>
+      <c r="B14" t="str">
+        <f>N14</f>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f>T14</f>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f>V14</f>
+      </c>
+      <c r="E14" s="3" t="str">
+        <f>W14</f>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2" t="str">
+        <f>W14/V14-1</f>
+      </c>
+      <c r="H14" s="2" t="str">
+        <f>W14/T14-1</f>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="str">
+        <f>W14/Sum(W$11:W$17)</f>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="M14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="3" t="n">
+        <v>869458862.113459</v>
+      </c>
+      <c r="P14" s="3" t="n">
+        <v>1778985085.56584</v>
+      </c>
+      <c r="Q14" s="3" t="n">
+        <v>2582376595.00278</v>
+      </c>
+      <c r="R14" s="3" t="n">
+        <v>4721714923.11983</v>
+      </c>
+      <c r="S14" s="3" t="n">
+        <v>8454279662.6609</v>
+      </c>
+      <c r="T14" s="3" t="n">
+        <v>18492608511.4107</v>
+      </c>
+      <c r="U14" s="3" t="n">
+        <v>15202524378.2965</v>
+      </c>
+      <c r="V14" s="3" t="n">
+        <v>10427014268.1498</v>
+      </c>
+      <c r="W14" s="3" t="n">
+        <v>13597718627.55</v>
+      </c>
+      <c r="X14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <f>M15</f>
+      </c>
+      <c r="B15" t="str">
+        <f>N15</f>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f>T15</f>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f>V15</f>
+      </c>
+      <c r="E15" s="3" t="str">
+        <f>W15</f>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2" t="str">
+        <f>W15/V15-1</f>
+      </c>
+      <c r="H15" s="2" t="str">
+        <f>W15/T15-1</f>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="str">
+        <f>W15/Sum(W$11:W$17)</f>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="M15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" s="3" t="n">
+        <v>29755827616.8504</v>
+      </c>
+      <c r="P15" s="3" t="n">
+        <v>30502947188.8857</v>
+      </c>
+      <c r="Q15" s="3" t="n">
+        <v>31247474515.0013</v>
+      </c>
+      <c r="R15" s="3" t="n">
+        <v>32533101362.6512</v>
+      </c>
+      <c r="S15" s="3" t="n">
+        <v>36382543537.7477</v>
+      </c>
+      <c r="T15" s="3" t="n">
+        <v>36724453707.4691</v>
+      </c>
+      <c r="U15" s="3" t="n">
+        <v>36753586418.1931</v>
+      </c>
+      <c r="V15" s="3" t="n">
+        <v>36942458165.7425</v>
+      </c>
+      <c r="W15" s="3" t="n">
+        <v>43247146108.6712</v>
+      </c>
+      <c r="X15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <f>M16</f>
+      </c>
+      <c r="B16" t="str">
+        <f>N16</f>
+      </c>
+      <c r="C16" s="3" t="str">
+        <f>T16</f>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f>V16</f>
+      </c>
+      <c r="E16" s="3" t="str">
+        <f>W16</f>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2" t="str">
+        <f>W16/V16-1</f>
+      </c>
+      <c r="H16" s="2" t="str">
+        <f>W16/T16-1</f>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="str">
+        <f>W16/Sum(W$11:W$17)</f>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="M16" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" t="s">
+        <v>57</v>
+      </c>
+      <c r="O16" s="3" t="n">
+        <v>150902095992.3</v>
+      </c>
+      <c r="P16" s="3" t="n">
+        <v>155334060443.263</v>
+      </c>
+      <c r="Q16" s="3" t="n">
+        <v>160399013484.935</v>
+      </c>
+      <c r="R16" s="3" t="n">
+        <v>177426318705.693</v>
+      </c>
+      <c r="S16" s="3" t="n">
+        <v>187385064629.507</v>
+      </c>
+      <c r="T16" s="3" t="n">
+        <v>199536734389.102</v>
+      </c>
+      <c r="U16" s="3" t="n">
+        <v>179030983615.014</v>
+      </c>
+      <c r="V16" s="3" t="n">
+        <v>176957593946.476</v>
+      </c>
+      <c r="W16" s="3" t="n">
+        <v>187356782728.035</v>
+      </c>
+      <c r="X16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <f>M17</f>
+      </c>
+      <c r="B17" t="str">
+        <f>N17</f>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f>T17</f>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f>V17</f>
+      </c>
+      <c r="E17" s="3" t="str">
+        <f>W17</f>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="2" t="str">
+        <f>W17/V17-1</f>
+      </c>
+      <c r="H17" s="2" t="str">
+        <f>W17/T17-1</f>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="str">
+        <f>W17/Sum(W$11:W$17)</f>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="M17" t="s">
+        <v>58</v>
+      </c>
+      <c r="N17" t="s">
+        <v>58</v>
+      </c>
+      <c r="O17" s="3" t="n">
+        <v>37536.9003683804</v>
+      </c>
+      <c r="P17" s="3" t="n">
+        <v>4445772.80663764</v>
+      </c>
+      <c r="Q17" s="3" t="n">
+        <v>1642582.46521554</v>
+      </c>
+      <c r="R17" s="3" t="n">
+        <v>-254117.889817779</v>
+      </c>
+      <c r="S17" s="3" t="n">
+        <v>546254.749528136</v>
+      </c>
+      <c r="T17" s="3" t="n">
+        <v>283560.728127099</v>
+      </c>
+      <c r="U17" s="3" t="n">
+        <v>432241.925938871</v>
+      </c>
+      <c r="V17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" s="3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="X17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <f>M18</f>
+      </c>
+      <c r="B18" t="str">
+        <f>N18</f>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f>T18</f>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f>V18</f>
+      </c>
+      <c r="E18" s="3" t="str">
+        <f>W18</f>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="2" t="str">
+        <f>W18/V18-1</f>
+      </c>
+      <c r="H18" s="2" t="str">
+        <f>W18/T18-1</f>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2" t="str">
+        <f>Sum(J$11:J$17)</f>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="M18" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18" t="s">
+        <v>47</v>
+      </c>
+      <c r="O18" s="3" t="str">
+        <f>Sum(O12:O17)</f>
+      </c>
+      <c r="P18" s="3" t="str">
+        <f>Sum(P12:P17)</f>
+      </c>
+      <c r="Q18" s="3" t="str">
+        <f>Sum(Q12:Q17)</f>
+      </c>
+      <c r="R18" s="3" t="str">
+        <f>Sum(R12:R17)</f>
+      </c>
+      <c r="S18" s="3" t="str">
+        <f>Sum(S12:S17)</f>
+      </c>
+      <c r="T18" s="3" t="str">
+        <f>Sum(T12:T17)</f>
+      </c>
+      <c r="U18" s="3" t="str">
+        <f>Sum(U12:U17)</f>
+      </c>
+      <c r="V18" s="3" t="str">
+        <f>Sum(V12:V17)</f>
+      </c>
+      <c r="W18" s="3" t="str">
+        <f>Sum(W12:W17)</f>
+      </c>
+      <c r="X18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010025DE50B441C283468F0A19FFD0E26C8A" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d7eaad3f2307abdda69af20ceb01590">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f" xmlns:ns3="361d4f7d-a938-4275-8fcb-42d4143832a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7531f5b5039f72b900df0adb30279836" ns2:_="" ns3:_="">
+    <xsd:import namespace="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f"/>
+    <xsd:import namespace="361d4f7d-a938-4275-8fcb-42d4143832a1"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:LastSharedByUser" minOccurs="0"/>
+                <xsd:element ref="ns2:LastSharedByTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="9" nillable="true" ma:displayName="Sharing Hint Hash" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="10" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastSharedByUser" ma:index="11" nillable="true" ma:displayName="Last Shared By User" ma:description="" ma:internalName="LastSharedByUser" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastSharedByTime" ma:index="12" nillable="true" ma:displayName="Last Shared By Time" ma:description="" ma:internalName="LastSharedByTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="26" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{973caeba-2f6e-4377-9853-72725798a959}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="361d4f7d-a938-4275-8fcb-42d4143832a1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="13" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="14" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="20" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="21" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="25" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="ba7e76ad-b1d6-47d4-8d36-3cc9679ac96f" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="27" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="28" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D31577A-01B4-4631-8F0C-D8D5DB59688F}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2E89E69-F9C9-4727-B0BC-4B94DDA0BB9F}"/>
 </file>
</xml_diff>

<commit_message>
Vendor size including nontraditional
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/NPS2024/DoD_2024_NPS.xlsx
+++ b/Output/AcqTrends/NPS2024/DoD_2024_NPS.xlsx
@@ -3,7 +3,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t xml:space="preserve">source</t>
   </si>
@@ -353,6 +353,24 @@
   <si>
     <t xml:space="preserve">multiyearcontract</t>
   </si>
+  <si>
+    <t xml:space="preserve">VendorSize.NTDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Five</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Traditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium or Large Non-Traditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium Traditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small</t>
+  </si>
 </sst>
 </file>
 
@@ -362,7 +380,7 @@
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="170" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="213" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="218" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="219" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="175" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="178" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="183" formatCode="0.00,,,&quot;B&quot;"/>
@@ -374,7 +392,7 @@
     <numFmt numFmtId="193" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="189" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="192" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="219" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="220" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -416,7 +434,7 @@
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="213" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="218" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="219" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="183" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -428,7 +446,7 @@
     <xf numFmtId="193" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="189" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="192" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="219" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="220" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9457,7 +9475,7 @@
         <f>L1</f>
       </c>
       <c r="L1" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="M1" t="s">
         <v>2</v>
@@ -9567,109 +9585,109 @@
         <f>L2</f>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="M2" s="17" t="n">
-        <v>120350129405</v>
+        <v>29993312707</v>
       </c>
       <c r="N2" s="17" t="n">
-        <v>136154193844</v>
+        <v>31945138023</v>
       </c>
       <c r="O2" s="17" t="n">
-        <v>123406660550</v>
+        <v>29753069568</v>
       </c>
       <c r="P2" s="17" t="n">
-        <v>121373382142</v>
+        <v>30346592157</v>
       </c>
       <c r="Q2" s="17" t="n">
-        <v>117161902725</v>
+        <v>31747329388</v>
       </c>
       <c r="R2" s="17" t="n">
-        <v>116592014868</v>
+        <v>28791249139</v>
       </c>
       <c r="S2" s="17" t="n">
-        <v>118448779098</v>
+        <v>32842967690</v>
       </c>
       <c r="T2" s="17" t="n">
-        <v>115982151879</v>
+        <v>34627617203</v>
       </c>
       <c r="U2" s="17" t="n">
-        <v>116965882167</v>
+        <v>37288669184</v>
       </c>
       <c r="V2" s="17" t="n">
-        <v>122185036488</v>
+        <v>39481622310</v>
       </c>
       <c r="W2" s="17" t="n">
-        <v>5236358155.9916</v>
+        <v>42902822546.2254</v>
       </c>
       <c r="X2" s="17" t="n">
-        <v>5491432009.7286</v>
+        <v>45999287165.102</v>
       </c>
       <c r="Y2" s="17" t="n">
-        <v>6587487263.1819</v>
+        <v>60247822851.393</v>
       </c>
       <c r="Z2" s="17" t="n">
-        <v>6976292471.2142</v>
+        <v>70112736203.1276</v>
       </c>
       <c r="AA2" s="17" t="n">
-        <v>9469780522.9719</v>
+        <v>72882060944.0123</v>
       </c>
       <c r="AB2" s="17" t="n">
-        <v>15314661031.4702</v>
+        <v>73955064380.7206</v>
       </c>
       <c r="AC2" s="17" t="n">
-        <v>13690206159.2622</v>
+        <v>88529377435.8539</v>
       </c>
       <c r="AD2" s="17" t="n">
-        <v>8188109934.3742</v>
+        <v>99100586147.3638</v>
       </c>
       <c r="AE2" s="17" t="n">
-        <v>10574055160.1785</v>
+        <v>105266669700.67</v>
       </c>
       <c r="AF2" s="17" t="n">
-        <v>6764981953.2342</v>
+        <v>107245503547.368</v>
       </c>
       <c r="AG2" s="17" t="n">
-        <v>5104291491.3231</v>
+        <v>96939369086.5759</v>
       </c>
       <c r="AH2" s="17" t="n">
-        <v>4330718826.8533</v>
+        <v>109468302700.962</v>
       </c>
       <c r="AI2" s="17" t="n">
-        <v>3082990599.5089</v>
+        <v>105499463138.199</v>
       </c>
       <c r="AJ2" s="17" t="n">
-        <v>1609033568.5028</v>
+        <v>96995856740.5779</v>
       </c>
       <c r="AK2" s="17" t="n">
-        <v>680453391.7032</v>
+        <v>82026660480.1835</v>
       </c>
       <c r="AL2" s="17" t="n">
-        <v>566899218.0891</v>
+        <v>82093613281.8144</v>
       </c>
       <c r="AM2" s="17" t="n">
-        <v>766600193.2492</v>
+        <v>103132925805.592</v>
       </c>
       <c r="AN2" s="17" t="n">
-        <v>547517746.2317</v>
+        <v>112799135328.923</v>
       </c>
       <c r="AO2" s="17" t="n">
-        <v>240712405.9436</v>
+        <v>113078047450.629</v>
       </c>
       <c r="AP2" s="17" t="n">
-        <v>380518692.1141</v>
+        <v>123281118568.194</v>
       </c>
       <c r="AQ2" s="17" t="n">
-        <v>789032280.102</v>
+        <v>153210907310.412</v>
       </c>
       <c r="AR2" s="17" t="n">
-        <v>769670794.6879</v>
+        <v>114361655314.093</v>
       </c>
       <c r="AS2" s="17" t="n">
-        <v>285283811.2825</v>
+        <v>122304776861.729</v>
       </c>
       <c r="AT2" s="17" t="n">
-        <v>235044504.6941</v>
+        <v>84663692097.9125</v>
       </c>
       <c r="AU2" s="17"/>
       <c r="AV2" s="17"/>
@@ -9679,89 +9697,109 @@
         <f>L3</f>
       </c>
       <c r="L3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="M3" s="17" t="n">
+        <v>35960694888</v>
+      </c>
+      <c r="N3" s="17" t="n">
+        <v>37863506273</v>
+      </c>
+      <c r="O3" s="17" t="n">
+        <v>35092959873</v>
+      </c>
+      <c r="P3" s="17" t="n">
+        <v>33829226700</v>
+      </c>
+      <c r="Q3" s="17" t="n">
+        <v>31124696371</v>
+      </c>
+      <c r="R3" s="17" t="n">
+        <v>28535738215</v>
+      </c>
+      <c r="S3" s="17" t="n">
+        <v>30194170969</v>
+      </c>
+      <c r="T3" s="17" t="n">
+        <v>29073662056</v>
+      </c>
+      <c r="U3" s="17" t="n">
+        <v>28130482737</v>
+      </c>
+      <c r="V3" s="17" t="n">
+        <v>29677352211</v>
+      </c>
       <c r="W3" s="17" t="n">
-        <v>1329220610.9815</v>
+        <v>24339685706.4517</v>
       </c>
       <c r="X3" s="17" t="n">
-        <v>1064745085.42</v>
+        <v>25668062870.6387</v>
       </c>
       <c r="Y3" s="17" t="n">
-        <v>1807184389.3146</v>
+        <v>32788951053.1231</v>
       </c>
       <c r="Z3" s="17" t="n">
-        <v>1921193307.4043</v>
+        <v>47830922262.423</v>
       </c>
       <c r="AA3" s="17" t="n">
-        <v>2648920884.8399</v>
+        <v>58825443576.2251</v>
       </c>
       <c r="AB3" s="17" t="n">
-        <v>3794008336.1995</v>
+        <v>65108861243.7038</v>
       </c>
       <c r="AC3" s="17" t="n">
-        <v>9741097914.2115</v>
+        <v>68516071349.0288</v>
       </c>
       <c r="AD3" s="17" t="n">
-        <v>12868195666.4892</v>
+        <v>82810086269.79</v>
       </c>
       <c r="AE3" s="17" t="n">
-        <v>16499453100.5148</v>
+        <v>101935552219.899</v>
       </c>
       <c r="AF3" s="17" t="n">
-        <v>20075739480.5829</v>
+        <v>91082000212.6408</v>
       </c>
       <c r="AG3" s="17" t="n">
-        <v>22679836748.4971</v>
+        <v>106725389754.146</v>
       </c>
       <c r="AH3" s="17" t="n">
-        <v>19753164985.6706</v>
+        <v>103383013784.238</v>
       </c>
       <c r="AI3" s="17" t="n">
-        <v>18705132716.5269</v>
+        <v>98265166220.3349</v>
       </c>
       <c r="AJ3" s="17" t="n">
-        <v>18039454964.6385</v>
+        <v>86438880967.1992</v>
       </c>
       <c r="AK3" s="17" t="n">
-        <v>12582856811.9378</v>
+        <v>77207039866.9569</v>
       </c>
       <c r="AL3" s="17" t="n">
-        <v>10809719855.91</v>
+        <v>71996639966.4858</v>
       </c>
       <c r="AM3" s="17" t="n">
-        <v>9825055376.308</v>
+        <v>71551510997.6919</v>
       </c>
       <c r="AN3" s="17" t="n">
-        <v>9874481423.791</v>
+        <v>76631880839.9451</v>
       </c>
       <c r="AO3" s="17" t="n">
-        <v>11566748983.7809</v>
+        <v>88698325243.6305</v>
       </c>
       <c r="AP3" s="17" t="n">
-        <v>11431443200.7392</v>
+        <v>92762373993.5141</v>
       </c>
       <c r="AQ3" s="17" t="n">
-        <v>10618049742.5667</v>
+        <v>98398389839.8272</v>
       </c>
       <c r="AR3" s="17" t="n">
-        <v>10617066974.1711</v>
+        <v>90770167372.218</v>
       </c>
       <c r="AS3" s="17" t="n">
-        <v>14696330210.8885</v>
+        <v>99021129618.9242</v>
       </c>
       <c r="AT3" s="17" t="n">
-        <v>6690070397.66</v>
+        <v>48591295833.2184</v>
       </c>
       <c r="AU3" s="17"/>
       <c r="AV3" s="17"/>
@@ -9771,7 +9809,7 @@
         <f>L4</f>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
@@ -9784,76 +9822,76 @@
       <c r="U4" s="17"/>
       <c r="V4" s="17"/>
       <c r="W4" s="17" t="n">
-        <v>42550348684.2254</v>
+        <v>30879636954.9954</v>
       </c>
       <c r="X4" s="17" t="n">
-        <v>45917051459.0678</v>
+        <v>28990916270.223</v>
       </c>
       <c r="Y4" s="17" t="n">
-        <v>60117240828.9049</v>
+        <v>30113227132.5393</v>
       </c>
       <c r="Z4" s="17" t="n">
-        <v>70050048326.1247</v>
+        <v>35201492871.434</v>
       </c>
       <c r="AA4" s="17" t="n">
-        <v>72695496311.2301</v>
+        <v>35241294858.2151</v>
       </c>
       <c r="AB4" s="17" t="n">
-        <v>73850346664.7419</v>
+        <v>41875695732.6547</v>
       </c>
       <c r="AC4" s="17" t="n">
-        <v>88459373239.3844</v>
+        <v>49185549119.2547</v>
       </c>
       <c r="AD4" s="17" t="n">
-        <v>98609321172.6504</v>
+        <v>46279650071.9425</v>
       </c>
       <c r="AE4" s="17" t="n">
-        <v>104453708239.205</v>
+        <v>54012288564.5049</v>
       </c>
       <c r="AF4" s="17" t="n">
-        <v>106806901294.444</v>
+        <v>47688602187.0404</v>
       </c>
       <c r="AG4" s="17" t="n">
-        <v>95972949166.2754</v>
+        <v>39399834017.7615</v>
       </c>
       <c r="AH4" s="17" t="n">
-        <v>108581856624.386</v>
+        <v>38073802839.4699</v>
       </c>
       <c r="AI4" s="17" t="n">
-        <v>105059996799.245</v>
+        <v>42291049655.6658</v>
       </c>
       <c r="AJ4" s="17" t="n">
-        <v>96262274718.1229</v>
+        <v>32247405087.1344</v>
       </c>
       <c r="AK4" s="17" t="n">
-        <v>81791269260.1643</v>
+        <v>31296907203.1947</v>
       </c>
       <c r="AL4" s="17" t="n">
-        <v>81079398578.4434</v>
+        <v>28506482015.0489</v>
       </c>
       <c r="AM4" s="17" t="n">
-        <v>102613616343.317</v>
+        <v>26784143602.9829</v>
       </c>
       <c r="AN4" s="17" t="n">
-        <v>112269920603.578</v>
+        <v>29083589497.9641</v>
       </c>
       <c r="AO4" s="17" t="n">
-        <v>112777911380.805</v>
+        <v>33837415345.756</v>
       </c>
       <c r="AP4" s="17" t="n">
-        <v>123162121122.305</v>
+        <v>35835726921.9774</v>
       </c>
       <c r="AQ4" s="17" t="n">
-        <v>152100850792.38</v>
+        <v>34006207873.992</v>
       </c>
       <c r="AR4" s="17" t="n">
-        <v>113891441901.645</v>
+        <v>52156510661.3755</v>
       </c>
       <c r="AS4" s="17" t="n">
-        <v>121494516261.001</v>
+        <v>50741258836.9179</v>
       </c>
       <c r="AT4" s="17" t="n">
-        <v>84206478607.0139</v>
+        <v>20342650358.8622</v>
       </c>
       <c r="AU4" s="17"/>
       <c r="AV4" s="17"/>
@@ -9863,89 +9901,109 @@
         <f>L5</f>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
-      </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
+        <v>120</v>
+      </c>
+      <c r="M5" s="17" t="n">
+        <v>28304563806</v>
+      </c>
+      <c r="N5" s="17" t="n">
+        <v>41243339793</v>
+      </c>
+      <c r="O5" s="17" t="n">
+        <v>34954992394</v>
+      </c>
+      <c r="P5" s="17" t="n">
+        <v>33954732784</v>
+      </c>
+      <c r="Q5" s="17" t="n">
+        <v>32186662449</v>
+      </c>
+      <c r="R5" s="17" t="n">
+        <v>35189234715</v>
+      </c>
+      <c r="S5" s="17" t="n">
+        <v>30275743132</v>
+      </c>
+      <c r="T5" s="17" t="n">
+        <v>30248655247</v>
+      </c>
+      <c r="U5" s="17" t="n">
+        <v>30401001630</v>
+      </c>
+      <c r="V5" s="17" t="n">
+        <v>32561216997</v>
+      </c>
       <c r="W5" s="17" t="n">
-        <v>34771960308.124</v>
+        <v>12561996255.8882</v>
       </c>
       <c r="X5" s="17" t="n">
-        <v>34505522327.9598</v>
+        <v>20376379119.5963</v>
       </c>
       <c r="Y5" s="17" t="n">
-        <v>39749055232.3268</v>
+        <v>19098314585.8526</v>
       </c>
       <c r="Z5" s="17" t="n">
-        <v>57603373075.2766</v>
+        <v>25174152975.356</v>
       </c>
       <c r="AA5" s="17" t="n">
-        <v>68106048145.708</v>
+        <v>26390491632.9557</v>
       </c>
       <c r="AB5" s="17" t="n">
-        <v>77903401149.8159</v>
+        <v>34314078131.7759</v>
       </c>
       <c r="AC5" s="17" t="n">
-        <v>85116776817.2881</v>
+        <v>36302990528.4341</v>
       </c>
       <c r="AD5" s="17" t="n">
-        <v>99651450297.1159</v>
+        <v>43285772133.7758</v>
       </c>
       <c r="AE5" s="17" t="n">
-        <v>122895484993.633</v>
+        <v>52322135708.5164</v>
       </c>
       <c r="AF5" s="17" t="n">
-        <v>115392227736.743</v>
+        <v>56439625804.5077</v>
       </c>
       <c r="AG5" s="17" t="n">
-        <v>112773841229.609</v>
+        <v>56543203658.8858</v>
       </c>
       <c r="AH5" s="17" t="n">
-        <v>112002045671.281</v>
+        <v>57356213929.8226</v>
       </c>
       <c r="AI5" s="17" t="n">
-        <v>112706301394.788</v>
+        <v>52731495692.821</v>
       </c>
       <c r="AJ5" s="17" t="n">
-        <v>92009456672.6568</v>
+        <v>43802955073.4203</v>
       </c>
       <c r="AK5" s="17" t="n">
-        <v>87683491745.7842</v>
+        <v>38918110176.3577</v>
       </c>
       <c r="AL5" s="17" t="n">
-        <v>82490216234.141</v>
+        <v>38302470301.744</v>
       </c>
       <c r="AM5" s="17" t="n">
-        <v>81735528122.8488</v>
+        <v>39722090100.4181</v>
       </c>
       <c r="AN5" s="17" t="n">
-        <v>86483132759.9886</v>
+        <v>43597259051.7596</v>
       </c>
       <c r="AO5" s="17" t="n">
-        <v>102597589171.143</v>
+        <v>51940589519.8209</v>
       </c>
       <c r="AP5" s="17" t="n">
-        <v>106177490090.298</v>
+        <v>57640239173.7832</v>
       </c>
       <c r="AQ5" s="17" t="n">
-        <v>109077960637.558</v>
+        <v>60573407783.3784</v>
       </c>
       <c r="AR5" s="17" t="n">
-        <v>118928831895.369</v>
+        <v>55378049713.2556</v>
       </c>
       <c r="AS5" s="17" t="n">
-        <v>120230112251.207</v>
+        <v>39014152184.0631</v>
       </c>
       <c r="AT5" s="17" t="n">
-        <v>53200181316.3679</v>
+        <v>17449481642.3526</v>
       </c>
       <c r="AU5" s="17"/>
       <c r="AV5" s="17"/>
@@ -9955,89 +10013,109 @@
         <f>L6</f>
       </c>
       <c r="L6" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
+        <v>121</v>
+      </c>
+      <c r="M6" s="17" t="n">
+        <v>13434401635</v>
+      </c>
+      <c r="N6" s="17" t="n">
+        <v>19369182588</v>
+      </c>
+      <c r="O6" s="17" t="n">
+        <v>17619229930</v>
+      </c>
+      <c r="P6" s="17" t="n">
+        <v>17645725767</v>
+      </c>
+      <c r="Q6" s="17" t="n">
+        <v>18075942350</v>
+      </c>
+      <c r="R6" s="17" t="n">
+        <v>19041220687</v>
+      </c>
+      <c r="S6" s="17" t="n">
+        <v>19347390330</v>
+      </c>
+      <c r="T6" s="17" t="n">
+        <v>17934428738</v>
+      </c>
+      <c r="U6" s="17" t="n">
+        <v>17288342573</v>
+      </c>
+      <c r="V6" s="17" t="n">
+        <v>19013150234</v>
+      </c>
       <c r="W6" s="17" t="n">
-        <v>27694622520.5188</v>
+        <v>20597636512.8267</v>
       </c>
       <c r="X6" s="17" t="n">
-        <v>35321226116.5173</v>
+        <v>21626410588.6674</v>
       </c>
       <c r="Y6" s="17" t="n">
-        <v>35479100087.3137</v>
+        <v>25988398540.367</v>
       </c>
       <c r="Z6" s="17" t="n">
-        <v>42482595240.0615</v>
+        <v>32503996698.2746</v>
       </c>
       <c r="AA6" s="17" t="n">
-        <v>42241259511.0147</v>
+        <v>34598872059.718</v>
       </c>
       <c r="AB6" s="17" t="n">
-        <v>51515737177.5681</v>
+        <v>43335587798.781</v>
       </c>
       <c r="AC6" s="17" t="n">
-        <v>52686944659.3421</v>
+        <v>45538329543.2904</v>
       </c>
       <c r="AD6" s="17" t="n">
-        <v>59156529141.1112</v>
+        <v>49801473286.0533</v>
       </c>
       <c r="AE6" s="17" t="n">
-        <v>68785814990.9706</v>
+        <v>54964300849.7418</v>
       </c>
       <c r="AF6" s="17" t="n">
-        <v>73316171682.0021</v>
+        <v>59264807867.4139</v>
       </c>
       <c r="AG6" s="17" t="n">
-        <v>67896388549.7625</v>
+        <v>58277206632.2153</v>
       </c>
       <c r="AH6" s="17" t="n">
-        <v>67582752969.7274</v>
+        <v>56309134741.6547</v>
       </c>
       <c r="AI6" s="17" t="n">
-        <v>61772665022.7063</v>
+        <v>56266882362.0404</v>
       </c>
       <c r="AJ6" s="17" t="n">
-        <v>51521870959.8257</v>
+        <v>47418032358.0387</v>
       </c>
       <c r="AK6" s="17" t="n">
-        <v>47080827373.4356</v>
+        <v>53482722030.406</v>
       </c>
       <c r="AL6" s="17" t="n">
-        <v>46743111826.9035</v>
+        <v>52427120840.6328</v>
       </c>
       <c r="AM6" s="17" t="n">
-        <v>46913522999.3205</v>
+        <v>56461734363.4189</v>
       </c>
       <c r="AN6" s="17" t="n">
-        <v>52279423408.0778</v>
+        <v>59242049642.4755</v>
       </c>
       <c r="AO6" s="17" t="n">
-        <v>61590797753.2091</v>
+        <v>70266476117.5831</v>
       </c>
       <c r="AP6" s="17" t="n">
-        <v>69492927376.2443</v>
+        <v>73354518952.1936</v>
       </c>
       <c r="AQ6" s="17" t="n">
-        <v>74295272089.9873</v>
+        <v>75798633027.2083</v>
       </c>
       <c r="AR6" s="17" t="n">
-        <v>68774128716.5469</v>
+        <v>74294234511.4505</v>
       </c>
       <c r="AS6" s="17" t="n">
-        <v>76336782621.0928</v>
+        <v>81672645182.5426</v>
       </c>
       <c r="AT6" s="17" t="n">
-        <v>38965329412.2745</v>
+        <v>32808828005.7754</v>
       </c>
       <c r="AU6" s="17"/>
       <c r="AV6" s="17"/>
@@ -10046,90 +10124,108 @@
       <c r="A7" t="str">
         <f>L7</f>
       </c>
-      <c r="L7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
+      <c r="L7"/>
+      <c r="M7" s="17" t="n">
+        <v>12657156369</v>
+      </c>
+      <c r="N7" s="17" t="n">
+        <v>5733027167</v>
+      </c>
+      <c r="O7" s="17" t="n">
+        <v>5986408785</v>
+      </c>
+      <c r="P7" s="17" t="n">
+        <v>5597104734</v>
+      </c>
+      <c r="Q7" s="17" t="n">
+        <v>4027272167</v>
+      </c>
+      <c r="R7" s="17" t="n">
+        <v>5034572112</v>
+      </c>
+      <c r="S7" s="17" t="n">
+        <v>5788506977</v>
+      </c>
+      <c r="T7" s="17" t="n">
+        <v>4097788635</v>
+      </c>
+      <c r="U7" s="17" t="n">
+        <v>3857386043</v>
+      </c>
+      <c r="V7" s="17" t="n">
+        <v>1451694736</v>
+      </c>
       <c r="W7" s="17" t="n">
-        <v>20595976226.5461</v>
+        <v>896708530</v>
       </c>
       <c r="X7" s="17" t="n">
-        <v>21693661545.1428</v>
+        <v>1332582608.1</v>
       </c>
       <c r="Y7" s="17" t="n">
-        <v>26070453425.0865</v>
+        <v>1573806973.21</v>
       </c>
       <c r="Z7" s="17" t="n">
-        <v>32499585092.2557</v>
+        <v>709786293.2455</v>
       </c>
       <c r="AA7" s="17" t="n">
-        <v>34600451673.0244</v>
+        <v>1836868750.7889</v>
       </c>
       <c r="AB7" s="17" t="n">
-        <v>43285206666.0946</v>
+        <v>7075231414.8205</v>
       </c>
       <c r="AC7" s="17" t="n">
-        <v>45470779321.3648</v>
+        <v>7092868367.2559</v>
       </c>
       <c r="AD7" s="17" t="n">
-        <v>49679874369.1679</v>
+        <v>6876854944.5664</v>
       </c>
       <c r="AE7" s="17" t="n">
-        <v>54779583262.9025</v>
+        <v>9487139041.4969</v>
       </c>
       <c r="AF7" s="17" t="n">
-        <v>59199358639.9791</v>
+        <v>5929525859.4555</v>
       </c>
       <c r="AG7" s="17" t="n">
-        <v>57976561655.5411</v>
+        <v>4811342087.0799</v>
       </c>
       <c r="AH7" s="17" t="n">
-        <v>56315376883.2436</v>
+        <v>3973190873.3447</v>
       </c>
       <c r="AI7" s="17" t="n">
-        <v>56309344122.8112</v>
+        <v>2739247979.5661</v>
       </c>
       <c r="AJ7" s="17" t="n">
-        <v>47138961458.9347</v>
+        <v>1325283035.7596</v>
       </c>
       <c r="AK7" s="17" t="n">
-        <v>53465462041.4739</v>
+        <v>518098070.4508</v>
       </c>
       <c r="AL7" s="17" t="n">
-        <v>52495096053.1374</v>
+        <v>899913864.8209</v>
       </c>
       <c r="AM7" s="17" t="n">
-        <v>56507462593.3487</v>
+        <v>872368734.0903</v>
       </c>
       <c r="AN7" s="17" t="n">
-        <v>59161370863.6707</v>
+        <v>501162415.0376</v>
       </c>
       <c r="AO7" s="17" t="n">
-        <v>70182061058.5694</v>
+        <v>1009255457.355</v>
       </c>
       <c r="AP7" s="17" t="n">
-        <v>73210905668.2453</v>
+        <v>1101647733.6542</v>
       </c>
       <c r="AQ7" s="17" t="n">
-        <v>75720333560.9938</v>
+        <v>760098902.1179</v>
       </c>
       <c r="AR7" s="17" t="n">
-        <v>74082748315.2369</v>
+        <v>742455295.4319</v>
       </c>
       <c r="AS7" s="17" t="n">
-        <v>81277666893.7311</v>
+        <v>21741977737.9626</v>
       </c>
       <c r="AT7" s="17" t="n">
-        <v>32703442132.7152</v>
+        <v>13529156156.6481</v>
       </c>
       <c r="AU7" s="17"/>
       <c r="AV7" s="17"/>
@@ -10280,7 +10376,7 @@
         <f>"Share "&amp;AU11</f>
       </c>
       <c r="L11" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="M11" t="s">
         <v>2</v>
@@ -10417,109 +10513,109 @@
         <f>AU12/Sum(AU11:AU$17)</f>
       </c>
       <c r="L12" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="M12" s="17" t="n">
-        <v>248917998790.874</v>
+        <v>62034626909.3846</v>
       </c>
       <c r="N12" s="17" t="n">
-        <v>271885202720.129</v>
+        <v>63790986396.3299</v>
       </c>
       <c r="O12" s="17" t="n">
-        <v>240412560734.939</v>
+        <v>57962930142.4092</v>
       </c>
       <c r="P12" s="17" t="n">
-        <v>231031479111.987</v>
+        <v>57764049648.3606</v>
       </c>
       <c r="Q12" s="17" t="n">
-        <v>218250472650.085</v>
+        <v>59139272094.0376</v>
       </c>
       <c r="R12" s="17" t="n">
-        <v>212677633977.603</v>
+        <v>52518645921.6326</v>
       </c>
       <c r="S12" s="17" t="n">
-        <v>212071611328.834</v>
+        <v>58802303678.2549</v>
       </c>
       <c r="T12" s="17" t="n">
-        <v>204034317412.979</v>
+        <v>60916461069.1388</v>
       </c>
       <c r="U12" s="17" t="n">
-        <v>203216983313.484</v>
+        <v>64785480372.1977</v>
       </c>
       <c r="V12" s="17" t="n">
-        <v>209688280565.4</v>
+        <v>67756525136.607</v>
       </c>
       <c r="W12" s="17" t="n">
-        <v>8803225999.57178</v>
+        <v>72127083679.6732</v>
       </c>
       <c r="X12" s="17" t="n">
-        <v>9013568711.16042</v>
+        <v>75502662109.3571</v>
       </c>
       <c r="Y12" s="17" t="n">
-        <v>10645149198.6628</v>
+        <v>97358376194.8559</v>
       </c>
       <c r="Z12" s="17" t="n">
-        <v>11061125099.6622</v>
+        <v>111165887815.399</v>
       </c>
       <c r="AA12" s="17" t="n">
-        <v>14656727633.9458</v>
+        <v>112802246479.287</v>
       </c>
       <c r="AB12" s="17" t="n">
-        <v>23003084448.4049</v>
+        <v>111082745340.634</v>
       </c>
       <c r="AC12" s="17" t="n">
-        <v>19916141880.4905</v>
+        <v>128790145385.143</v>
       </c>
       <c r="AD12" s="17" t="n">
-        <v>11592699836.7935</v>
+        <v>140306292668.808</v>
       </c>
       <c r="AE12" s="17" t="n">
-        <v>14666230120.2202</v>
+        <v>146005026305.648</v>
       </c>
       <c r="AF12" s="17" t="n">
-        <v>9288059234.71007</v>
+        <v>147243938932.912</v>
       </c>
       <c r="AG12" s="17" t="n">
-        <v>6947824064.64581</v>
+        <v>131951257583.197</v>
       </c>
       <c r="AH12" s="17" t="n">
-        <v>5778868031.6165</v>
+        <v>146073411885.194</v>
       </c>
       <c r="AI12" s="17" t="n">
-        <v>4040591181.29977</v>
+        <v>138268407453.454</v>
       </c>
       <c r="AJ12" s="17" t="n">
-        <v>2071229860.17048</v>
+        <v>124858000930.857</v>
       </c>
       <c r="AK12" s="17" t="n">
-        <v>860221059.722463</v>
+        <v>103697125569.675</v>
       </c>
       <c r="AL12" s="17" t="n">
-        <v>709321315.610776</v>
+        <v>102717992754.661</v>
       </c>
       <c r="AM12" s="17" t="n">
-        <v>951585170.123587</v>
+        <v>128019486053.215</v>
       </c>
       <c r="AN12" s="17" t="n">
-        <v>668354912.953427</v>
+        <v>137693904522.467</v>
       </c>
       <c r="AO12" s="17" t="n">
-        <v>287456108.23233</v>
+        <v>135036560825.555</v>
       </c>
       <c r="AP12" s="17" t="n">
-        <v>446161913.029099</v>
+        <v>144548325327.103</v>
       </c>
       <c r="AQ12" s="17" t="n">
-        <v>913218644.332686</v>
+        <v>177324883403.893</v>
       </c>
       <c r="AR12" s="17" t="n">
-        <v>861170613.266858</v>
+        <v>127957170157.387</v>
       </c>
       <c r="AS12" s="17" t="n">
-        <v>298334574.177027</v>
+        <v>127899803920.975</v>
       </c>
       <c r="AT12" s="17" t="n">
-        <v>235044504.6941</v>
+        <v>84663692097.9125</v>
       </c>
       <c r="AU12" s="17"/>
       <c r="AV12" s="17"/>
@@ -10556,89 +10652,109 @@
         <f>AU13/Sum(AU11:AU$17)</f>
       </c>
       <c r="L13" t="s">
-        <v>72</v>
-      </c>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="M13" s="17" t="n">
+        <v>74376855686.8564</v>
+      </c>
+      <c r="N13" s="17" t="n">
+        <v>75609327836.971</v>
+      </c>
+      <c r="O13" s="17" t="n">
+        <v>68365745489.2242</v>
+      </c>
+      <c r="P13" s="17" t="n">
+        <v>64393165484.7675</v>
+      </c>
+      <c r="Q13" s="17" t="n">
+        <v>57979424506.3217</v>
+      </c>
+      <c r="R13" s="17" t="n">
+        <v>52052563756.1149</v>
+      </c>
+      <c r="S13" s="17" t="n">
+        <v>54059877517.4901</v>
+      </c>
+      <c r="T13" s="17" t="n">
+        <v>51146014246.0563</v>
+      </c>
+      <c r="U13" s="17" t="n">
+        <v>48874011250.5904</v>
+      </c>
+      <c r="V13" s="17" t="n">
+        <v>50930892486.7369</v>
+      </c>
       <c r="W13" s="17" t="n">
-        <v>2234650322.45166</v>
+        <v>40919231964.1599</v>
       </c>
       <c r="X13" s="17" t="n">
-        <v>1747659439.34137</v>
+        <v>42131241533.5398</v>
       </c>
       <c r="Y13" s="17" t="n">
-        <v>2920346815.88986</v>
+        <v>52985798997.8947</v>
       </c>
       <c r="Z13" s="17" t="n">
-        <v>3046110753.17119</v>
+        <v>75837390269.9635</v>
       </c>
       <c r="AA13" s="17" t="n">
-        <v>4099832286.3754</v>
+        <v>91046302747.067</v>
       </c>
       <c r="AB13" s="17" t="n">
-        <v>5698715366.68095</v>
+        <v>97795480451.7547</v>
       </c>
       <c r="AC13" s="17" t="n">
-        <v>14171085948.1784</v>
+        <v>99675328640.5298</v>
       </c>
       <c r="AD13" s="17" t="n">
-        <v>18218750236.4228</v>
+        <v>117242255084.356</v>
       </c>
       <c r="AE13" s="17" t="n">
-        <v>22884765812.5746</v>
+        <v>141384761441.279</v>
       </c>
       <c r="AF13" s="17" t="n">
-        <v>27563215802.389</v>
+        <v>125052072428.137</v>
       </c>
       <c r="AG13" s="17" t="n">
-        <v>30871182770.6769</v>
+        <v>145271725273.345</v>
       </c>
       <c r="AH13" s="17" t="n">
-        <v>26358426446.6969</v>
+        <v>137953263016.154</v>
       </c>
       <c r="AI13" s="17" t="n">
-        <v>24515090740.6204</v>
+        <v>128787082296.679</v>
       </c>
       <c r="AJ13" s="17" t="n">
-        <v>23221304089.216</v>
+        <v>111268524686.888</v>
       </c>
       <c r="AK13" s="17" t="n">
-        <v>15907097463.3666</v>
+        <v>97604218690.3479</v>
       </c>
       <c r="AL13" s="17" t="n">
-        <v>13525445908.0466</v>
+        <v>90084356709.3377</v>
       </c>
       <c r="AM13" s="17" t="n">
-        <v>12195896993.0738</v>
+        <v>88817296636.4034</v>
       </c>
       <c r="AN13" s="17" t="n">
-        <v>12053779476.3372</v>
+        <v>93544536959.2909</v>
       </c>
       <c r="AO13" s="17" t="n">
-        <v>13812884445.0043</v>
+        <v>105922564652.665</v>
       </c>
       <c r="AP13" s="17" t="n">
-        <v>13403479705.0021</v>
+        <v>108764796830.682</v>
       </c>
       <c r="AQ13" s="17" t="n">
-        <v>12289232311.3958</v>
+        <v>113885383957.206</v>
       </c>
       <c r="AR13" s="17" t="n">
-        <v>11879242580.524</v>
+        <v>101561084611.461</v>
       </c>
       <c r="AS13" s="17" t="n">
-        <v>15368637272.8972</v>
+        <v>103551009104.182</v>
       </c>
       <c r="AT13" s="17" t="n">
-        <v>6690070397.66</v>
+        <v>48591295833.2184</v>
       </c>
       <c r="AU13" s="17"/>
       <c r="AV13" s="17"/>
@@ -10675,7 +10791,7 @@
         <f>AU14/Sum(AU11:AU$17)</f>
       </c>
       <c r="L14" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -10688,76 +10804,76 @@
       <c r="U14" s="17"/>
       <c r="V14" s="17"/>
       <c r="W14" s="17" t="n">
-        <v>71534514001.723</v>
+        <v>51914023984.1129</v>
       </c>
       <c r="X14" s="17" t="n">
-        <v>75367681436.6406</v>
+        <v>47585332084.2751</v>
       </c>
       <c r="Y14" s="17" t="n">
-        <v>97147360210.0785</v>
+        <v>48661922653.0792</v>
       </c>
       <c r="Z14" s="17" t="n">
-        <v>111066494268.953</v>
+        <v>55813043669.3161</v>
       </c>
       <c r="AA14" s="17" t="n">
-        <v>112513493534.888</v>
+        <v>54544248301.3675</v>
       </c>
       <c r="AB14" s="17" t="n">
-        <v>110925456161.399</v>
+        <v>62898562579.644</v>
       </c>
       <c r="AC14" s="17" t="n">
-        <v>128688305172.3</v>
+        <v>71553807395.8195</v>
       </c>
       <c r="AD14" s="17" t="n">
-        <v>139610761290.037</v>
+        <v>65522580441.1321</v>
       </c>
       <c r="AE14" s="17" t="n">
-        <v>144877447558.223</v>
+        <v>74915123990.4629</v>
       </c>
       <c r="AF14" s="17" t="n">
-        <v>146641754960.537</v>
+        <v>65474611018.2892</v>
       </c>
       <c r="AG14" s="17" t="n">
-        <v>130635792823.743</v>
+        <v>53629992604.6535</v>
       </c>
       <c r="AH14" s="17" t="n">
-        <v>144890547077.183</v>
+        <v>50805302968.8263</v>
       </c>
       <c r="AI14" s="17" t="n">
-        <v>137692439491.068</v>
+        <v>55426974806.1554</v>
       </c>
       <c r="AJ14" s="17" t="n">
-        <v>123913696834.575</v>
+        <v>41510500238.7463</v>
       </c>
       <c r="AK14" s="17" t="n">
-        <v>103399546797.634</v>
+        <v>39565176702.2284</v>
       </c>
       <c r="AL14" s="17" t="n">
-        <v>101448976878.908</v>
+        <v>35668165841.7306</v>
       </c>
       <c r="AM14" s="17" t="n">
-        <v>127374864270.755</v>
+        <v>33247309446.9647</v>
       </c>
       <c r="AN14" s="17" t="n">
-        <v>137047892107.115</v>
+        <v>35502337706.9848</v>
       </c>
       <c r="AO14" s="17" t="n">
-        <v>134678141631.357</v>
+        <v>40408269319.5754</v>
       </c>
       <c r="AP14" s="17" t="n">
-        <v>144408799650.168</v>
+        <v>42017742648.7726</v>
       </c>
       <c r="AQ14" s="17" t="n">
-        <v>176040114283.422</v>
+        <v>39358469655.472</v>
       </c>
       <c r="AR14" s="17" t="n">
-        <v>127431056946.961</v>
+        <v>58356968436.524</v>
       </c>
       <c r="AS14" s="17" t="n">
-        <v>127052476656.93</v>
+        <v>53062498640.4436</v>
       </c>
       <c r="AT14" s="17" t="n">
-        <v>84206478607.0139</v>
+        <v>20342650358.8622</v>
       </c>
       <c r="AU14" s="17"/>
       <c r="AV14" s="17"/>
@@ -10794,89 +10910,109 @@
         <f>AU15/Sum(AU11:AU$17)</f>
       </c>
       <c r="L15" t="s">
-        <v>74</v>
-      </c>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
+        <v>120</v>
+      </c>
+      <c r="M15" s="17" t="n">
+        <v>58541818060.9403</v>
+      </c>
+      <c r="N15" s="17" t="n">
+        <v>82358489914.1844</v>
+      </c>
+      <c r="O15" s="17" t="n">
+        <v>68096966520.7576</v>
+      </c>
+      <c r="P15" s="17" t="n">
+        <v>64632063468.1008</v>
+      </c>
+      <c r="Q15" s="17" t="n">
+        <v>59957666520.7577</v>
+      </c>
+      <c r="R15" s="17" t="n">
+        <v>64189328824.463</v>
+      </c>
+      <c r="S15" s="17" t="n">
+        <v>54205924949.7956</v>
+      </c>
+      <c r="T15" s="17" t="n">
+        <v>53213047231.7927</v>
+      </c>
+      <c r="U15" s="17" t="n">
+        <v>52818819697.6635</v>
+      </c>
+      <c r="V15" s="17" t="n">
+        <v>55880047192.9175</v>
+      </c>
       <c r="W15" s="17" t="n">
-        <v>58457694436.027</v>
+        <v>21118893847.9738</v>
       </c>
       <c r="X15" s="17" t="n">
-        <v>56636938391.7615</v>
+        <v>33445537148.3718</v>
       </c>
       <c r="Y15" s="17" t="n">
-        <v>64233084110.6817</v>
+        <v>30862208925.3496</v>
       </c>
       <c r="Z15" s="17" t="n">
-        <v>91331909947.47</v>
+        <v>39914389553.9664</v>
       </c>
       <c r="AA15" s="17" t="n">
-        <v>105410235799.507</v>
+        <v>40845534598.3846</v>
       </c>
       <c r="AB15" s="17" t="n">
-        <v>117013266685.09</v>
+        <v>51540784050.8128</v>
       </c>
       <c r="AC15" s="17" t="n">
-        <v>123825586246.286</v>
+        <v>52812609367.5539</v>
       </c>
       <c r="AD15" s="17" t="n">
-        <v>141086204368.835</v>
+        <v>61283857639.0038</v>
       </c>
       <c r="AE15" s="17" t="n">
-        <v>170456219146.701</v>
+        <v>72570879483.6226</v>
       </c>
       <c r="AF15" s="17" t="n">
-        <v>158429076951.437</v>
+        <v>77489428838.2428</v>
       </c>
       <c r="AG15" s="17" t="n">
-        <v>153504714472.041</v>
+        <v>76965085505.2447</v>
       </c>
       <c r="AH15" s="17" t="n">
-        <v>149454413247.074</v>
+        <v>76535560110.3393</v>
       </c>
       <c r="AI15" s="17" t="n">
-        <v>147713745077.665</v>
+        <v>69110303647.0819</v>
       </c>
       <c r="AJ15" s="17" t="n">
-        <v>118439253107.563</v>
+        <v>56385392006.5785</v>
       </c>
       <c r="AK15" s="17" t="n">
-        <v>110848424167.491</v>
+        <v>49199810577.0402</v>
       </c>
       <c r="AL15" s="17" t="n">
-        <v>103214234271.57</v>
+        <v>47925200385.9804</v>
       </c>
       <c r="AM15" s="17" t="n">
-        <v>101458774885.332</v>
+        <v>49307255853.4869</v>
       </c>
       <c r="AN15" s="17" t="n">
-        <v>105569960180.398</v>
+        <v>53219174134.7063</v>
       </c>
       <c r="AO15" s="17" t="n">
-        <v>122520912794.443</v>
+        <v>62026880850.333</v>
       </c>
       <c r="AP15" s="17" t="n">
-        <v>124494152537.218</v>
+        <v>67583747947.7055</v>
       </c>
       <c r="AQ15" s="17" t="n">
-        <v>126245820167.367</v>
+        <v>70107100474.2631</v>
       </c>
       <c r="AR15" s="17" t="n">
-        <v>133067300728.198</v>
+        <v>61961489720.3226</v>
       </c>
       <c r="AS15" s="17" t="n">
-        <v>125730230469.339</v>
+        <v>40798916792.3185</v>
       </c>
       <c r="AT15" s="17" t="n">
-        <v>53200181316.3679</v>
+        <v>17449481642.3526</v>
       </c>
       <c r="AU15" s="17"/>
       <c r="AV15" s="17"/>
@@ -10913,89 +11049,109 @@
         <f>AU16/Sum(AU11:AU$17)</f>
       </c>
       <c r="L16" t="s">
-        <v>75</v>
-      </c>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="17"/>
-      <c r="V16" s="17"/>
+        <v>121</v>
+      </c>
+      <c r="M16" s="17" t="n">
+        <v>27786130239.0766</v>
+      </c>
+      <c r="N16" s="17" t="n">
+        <v>38678163233.7772</v>
+      </c>
+      <c r="O16" s="17" t="n">
+        <v>34324599391.722</v>
+      </c>
+      <c r="P16" s="17" t="n">
+        <v>33588238640.2068</v>
+      </c>
+      <c r="Q16" s="17" t="n">
+        <v>33672062929.3893</v>
+      </c>
+      <c r="R16" s="17" t="n">
+        <v>34733440093.1433</v>
+      </c>
+      <c r="S16" s="17" t="n">
+        <v>34639717467.2126</v>
+      </c>
+      <c r="T16" s="17" t="n">
+        <v>31550017536.8974</v>
+      </c>
+      <c r="U16" s="17" t="n">
+        <v>30036834323.6961</v>
+      </c>
+      <c r="V16" s="17" t="n">
+        <v>32629484716.7365</v>
+      </c>
       <c r="W16" s="17" t="n">
-        <v>46559462465.7199</v>
+        <v>34628198430.6147</v>
       </c>
       <c r="X16" s="17" t="n">
-        <v>57975824520.7514</v>
+        <v>35497323370.5492</v>
       </c>
       <c r="Y16" s="17" t="n">
-        <v>57332985822.1718</v>
+        <v>41996343802.0963</v>
       </c>
       <c r="Z16" s="17" t="n">
-        <v>67357454184.6651</v>
+        <v>51536080977.4146</v>
       </c>
       <c r="AA16" s="17" t="n">
-        <v>65378351068</v>
+        <v>53549946906.4653</v>
       </c>
       <c r="AB16" s="17" t="n">
-        <v>77378196636.6948</v>
+        <v>65091364654.3129</v>
       </c>
       <c r="AC16" s="17" t="n">
-        <v>76647542986.4204</v>
+        <v>66247930939.3818</v>
       </c>
       <c r="AD16" s="17" t="n">
-        <v>83753624611.2749</v>
+        <v>70508766475.1082</v>
       </c>
       <c r="AE16" s="17" t="n">
-        <v>95406026957.7255</v>
+        <v>76235566435.774</v>
       </c>
       <c r="AF16" s="17" t="n">
-        <v>100660275245.679</v>
+        <v>81368294817.5627</v>
       </c>
       <c r="AG16" s="17" t="n">
-        <v>92418734915.6078</v>
+        <v>79325363637.2335</v>
       </c>
       <c r="AH16" s="17" t="n">
-        <v>90181751861.542</v>
+        <v>75138348079.497</v>
       </c>
       <c r="AI16" s="17" t="n">
-        <v>80959729678.0246</v>
+        <v>73743808595.2994</v>
       </c>
       <c r="AJ16" s="17" t="n">
-        <v>66321573193.2417</v>
+        <v>61038903384.6493</v>
       </c>
       <c r="AK16" s="17" t="n">
-        <v>59519020273.2539</v>
+        <v>67612219121.5487</v>
       </c>
       <c r="AL16" s="17" t="n">
-        <v>58486384385.1513</v>
+        <v>65598387053.1957</v>
       </c>
       <c r="AM16" s="17" t="n">
-        <v>58234022320.2804</v>
+        <v>70086271269.9855</v>
       </c>
       <c r="AN16" s="17" t="n">
-        <v>63817492166.4999</v>
+        <v>72316770012.4619</v>
       </c>
       <c r="AO16" s="17" t="n">
-        <v>73551053406.0729</v>
+        <v>83911453108.4576</v>
       </c>
       <c r="AP16" s="17" t="n">
-        <v>81481141564.7365</v>
+        <v>86008895708.1413</v>
       </c>
       <c r="AQ16" s="17" t="n">
-        <v>85988658980.5621</v>
+        <v>87728634988.71</v>
       </c>
       <c r="AR16" s="17" t="n">
-        <v>76950118170.6376</v>
+        <v>83126463857.007</v>
       </c>
       <c r="AS16" s="17" t="n">
-        <v>79828930477.7842</v>
+        <v>85408890581.307</v>
       </c>
       <c r="AT16" s="17" t="n">
-        <v>38965329412.2745</v>
+        <v>32808828005.7754</v>
       </c>
       <c r="AU16" s="17"/>
       <c r="AV16" s="17"/>
@@ -11031,90 +11187,108 @@
       <c r="J17" s="1" t="str">
         <f>AU17/Sum(AU11:AU$17)</f>
       </c>
-      <c r="L17" t="s">
-        <v>76</v>
-      </c>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
+      <c r="L17"/>
+      <c r="M17" s="17" t="n">
+        <v>26178567894.6163</v>
+      </c>
+      <c r="N17" s="17" t="n">
+        <v>11448235338.8668</v>
+      </c>
+      <c r="O17" s="17" t="n">
+        <v>11662319190.8258</v>
+      </c>
+      <c r="P17" s="17" t="n">
+        <v>10653961870.5513</v>
+      </c>
+      <c r="Q17" s="17" t="n">
+        <v>7502046599.57892</v>
+      </c>
+      <c r="R17" s="17" t="n">
+        <v>9183655382.24917</v>
+      </c>
+      <c r="S17" s="17" t="n">
+        <v>10363787716.0805</v>
+      </c>
+      <c r="T17" s="17" t="n">
+        <v>7208777329.09415</v>
+      </c>
+      <c r="U17" s="17" t="n">
+        <v>6701837669.3367</v>
+      </c>
+      <c r="V17" s="17" t="n">
+        <v>2491331032.40164</v>
+      </c>
       <c r="W17" s="17" t="n">
-        <v>34625407201.4977</v>
+        <v>1507522520.45657</v>
       </c>
       <c r="X17" s="17" t="n">
-        <v>35607708260.3208</v>
+        <v>2187284642.71751</v>
       </c>
       <c r="Y17" s="17" t="n">
-        <v>42128941628.1597</v>
+        <v>2543217067.50809</v>
       </c>
       <c r="Z17" s="17" t="n">
-        <v>51529086241.1321</v>
+        <v>1125387878.44821</v>
       </c>
       <c r="AA17" s="17" t="n">
-        <v>53552391732.0811</v>
+        <v>2842989329.51089</v>
       </c>
       <c r="AB17" s="17" t="n">
-        <v>65015690667.9667</v>
+        <v>10627211754.3237</v>
       </c>
       <c r="AC17" s="17" t="n">
-        <v>66149660702.376</v>
+        <v>10318513183.6995</v>
       </c>
       <c r="AD17" s="17" t="n">
-        <v>70336607117.7925</v>
+        <v>9736229219.25512</v>
       </c>
       <c r="AE17" s="17" t="n">
-        <v>75979362870.0844</v>
+        <v>13158675858.7299</v>
       </c>
       <c r="AF17" s="17" t="n">
-        <v>81278435553.2686</v>
+        <v>8141010249.1165</v>
       </c>
       <c r="AG17" s="17" t="n">
-        <v>78916133794.5799</v>
+        <v>6549069227.86101</v>
       </c>
       <c r="AH17" s="17" t="n">
-        <v>75146677531.0082</v>
+        <v>5301786294.48572</v>
       </c>
       <c r="AI17" s="17" t="n">
-        <v>73799459305.4055</v>
+        <v>3590079460.95946</v>
       </c>
       <c r="AJ17" s="17" t="n">
-        <v>60679669127.115</v>
+        <v>1705971740.16503</v>
       </c>
       <c r="AK17" s="17" t="n">
-        <v>67590399249.459</v>
+        <v>654973399.55614</v>
       </c>
       <c r="AL17" s="17" t="n">
-        <v>65683439679.1726</v>
+        <v>1125999236.13021</v>
       </c>
       <c r="AM17" s="17" t="n">
-        <v>70143033981.2924</v>
+        <v>1082876260.07676</v>
       </c>
       <c r="AN17" s="17" t="n">
-        <v>72218285427.156</v>
+        <v>611768960.153919</v>
       </c>
       <c r="AO17" s="17" t="n">
-        <v>83810645573.2366</v>
+        <v>1205241769.09887</v>
       </c>
       <c r="AP17" s="17" t="n">
-        <v>85840507718.7188</v>
+        <v>1291692814.35443</v>
       </c>
       <c r="AQ17" s="17" t="n">
-        <v>87638011912.5804</v>
+        <v>879731420.951674</v>
       </c>
       <c r="AR17" s="17" t="n">
-        <v>82889835809.6032</v>
+        <v>830719687.564062</v>
       </c>
       <c r="AS17" s="17" t="n">
-        <v>84995843380.7946</v>
+        <v>22736599181.9227</v>
       </c>
       <c r="AT17" s="17" t="n">
-        <v>32703442132.7152</v>
+        <v>13529156156.6481</v>
       </c>
       <c r="AU17" s="17"/>
       <c r="AV17" s="17"/>

</xml_diff>

<commit_message>
Working through slide output.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/NPS2024/DoD_2024_NPS.xlsx
+++ b/Output/AcqTrends/NPS2024/DoD_2024_NPS.xlsx
@@ -380,7 +380,7 @@
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="170" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="213" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="219" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="220" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="175" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="178" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="183" formatCode="0.00,,,&quot;B&quot;"/>
@@ -389,10 +389,10 @@
     <numFmt numFmtId="204" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="209" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="215" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="193" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="222" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="189" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="192" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="220" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="223" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -434,7 +434,7 @@
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="213" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="219" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="220" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="183" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -443,10 +443,10 @@
     <xf numFmtId="204" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="209" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="215" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="193" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="222" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="189" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="192" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="220" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="223" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2332,71 +2332,71 @@
       <c r="N2" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="14"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="14" t="n">
-        <v>27766409244.5725</v>
-      </c>
-      <c r="AL2" s="14" t="n">
-        <v>20117589432.5252</v>
-      </c>
-      <c r="AM2" s="14" t="n">
-        <v>15814444285.1675</v>
-      </c>
-      <c r="AN2" s="14" t="n">
-        <v>24205301305.0384</v>
-      </c>
-      <c r="AO2" s="14" t="n">
-        <v>33686791345.6108</v>
-      </c>
-      <c r="AP2" s="14" t="n">
-        <v>31035471218.9151</v>
-      </c>
-      <c r="AQ2" s="14" t="n">
-        <v>34812921569.4345</v>
-      </c>
-      <c r="AR2" s="14" t="n">
-        <v>38372888881.5383</v>
-      </c>
-      <c r="AS2" s="14" t="n">
-        <v>50101609453.4146</v>
-      </c>
-      <c r="AT2" s="14" t="n">
-        <v>24784144858.8701</v>
-      </c>
-      <c r="AU2" s="14" t="n">
-        <v>38727720245.0645</v>
-      </c>
-      <c r="AV2" s="14" t="n">
-        <v>65793606575.0316</v>
-      </c>
-      <c r="AW2" s="14"/>
-      <c r="AX2" s="14"/>
-      <c r="AY2" s="14"/>
-      <c r="AZ2" s="14"/>
-      <c r="BA2" s="14"/>
-      <c r="BB2" s="14"/>
-      <c r="BC2" s="14"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17"/>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="n">
+        <v>27766499707.7925</v>
+      </c>
+      <c r="AL2" s="17" t="n">
+        <v>20370470402.3352</v>
+      </c>
+      <c r="AM2" s="17" t="n">
+        <v>15761273120.7975</v>
+      </c>
+      <c r="AN2" s="17" t="n">
+        <v>23354753347.4642</v>
+      </c>
+      <c r="AO2" s="17" t="n">
+        <v>33579323851.3433</v>
+      </c>
+      <c r="AP2" s="17" t="n">
+        <v>31744209582.4775</v>
+      </c>
+      <c r="AQ2" s="17" t="n">
+        <v>34798072386.1799</v>
+      </c>
+      <c r="AR2" s="17" t="n">
+        <v>38381428744.3879</v>
+      </c>
+      <c r="AS2" s="17" t="n">
+        <v>50194113808.9869</v>
+      </c>
+      <c r="AT2" s="17" t="n">
+        <v>24883846155.5851</v>
+      </c>
+      <c r="AU2" s="17" t="n">
+        <v>38749898900.9551</v>
+      </c>
+      <c r="AV2" s="17" t="n">
+        <v>65793606959.6752</v>
+      </c>
+      <c r="AW2" s="17"/>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="17"/>
+      <c r="AZ2" s="17"/>
+      <c r="BA2" s="17"/>
+      <c r="BB2" s="17"/>
+      <c r="BC2" s="17"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -2411,71 +2411,71 @@
       <c r="N3" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14" t="n">
-        <v>329870021411.014</v>
-      </c>
-      <c r="AL3" s="14" t="n">
-        <v>286463462910.156</v>
-      </c>
-      <c r="AM3" s="14" t="n">
-        <v>267469916339.332</v>
-      </c>
-      <c r="AN3" s="14" t="n">
-        <v>249972893535.921</v>
-      </c>
-      <c r="AO3" s="14" t="n">
-        <v>264674994282.781</v>
-      </c>
-      <c r="AP3" s="14" t="n">
-        <v>289580375586.423</v>
-      </c>
-      <c r="AQ3" s="14" t="n">
-        <v>324142899184.017</v>
-      </c>
-      <c r="AR3" s="14" t="n">
-        <v>345482517268.407</v>
-      </c>
-      <c r="AS3" s="14" t="n">
-        <v>372499943849.534</v>
-      </c>
-      <c r="AT3" s="14" t="n">
-        <v>362279784320.787</v>
-      </c>
-      <c r="AU3" s="14" t="n">
-        <v>375515873709.073</v>
-      </c>
-      <c r="AV3" s="14" t="n">
-        <v>390453368175.855</v>
-      </c>
-      <c r="AW3" s="14"/>
-      <c r="AX3" s="14"/>
-      <c r="AY3" s="14"/>
-      <c r="AZ3" s="14"/>
-      <c r="BA3" s="14"/>
-      <c r="BB3" s="14"/>
-      <c r="BC3" s="14"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="17"/>
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="17"/>
+      <c r="AI3" s="17"/>
+      <c r="AJ3" s="17"/>
+      <c r="AK3" s="17" t="n">
+        <v>330026805340.834</v>
+      </c>
+      <c r="AL3" s="17" t="n">
+        <v>287169645793.985</v>
+      </c>
+      <c r="AM3" s="17" t="n">
+        <v>267688247411.752</v>
+      </c>
+      <c r="AN3" s="17" t="n">
+        <v>182341674892.763</v>
+      </c>
+      <c r="AO3" s="17" t="n">
+        <v>264945449752.851</v>
+      </c>
+      <c r="AP3" s="17" t="n">
+        <v>290110867193.627</v>
+      </c>
+      <c r="AQ3" s="17" t="n">
+        <v>324032036748.594</v>
+      </c>
+      <c r="AR3" s="17" t="n">
+        <v>345594196598.929</v>
+      </c>
+      <c r="AS3" s="17" t="n">
+        <v>372553530927.949</v>
+      </c>
+      <c r="AT3" s="17" t="n">
+        <v>362819226712.24</v>
+      </c>
+      <c r="AU3" s="17" t="n">
+        <v>375746041521.185</v>
+      </c>
+      <c r="AV3" s="17" t="n">
+        <v>390453124911.284</v>
+      </c>
+      <c r="AW3" s="17"/>
+      <c r="AX3" s="17"/>
+      <c r="AY3" s="17"/>
+      <c r="AZ3" s="17"/>
+      <c r="BA3" s="17"/>
+      <c r="BB3" s="17"/>
+      <c r="BC3" s="17"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -2490,93 +2490,99 @@
       <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="14" t="n">
+      <c r="O4" s="17" t="n">
         <v>120350129405</v>
       </c>
-      <c r="P4" s="14" t="n">
+      <c r="P4" s="17" t="n">
         <v>136154193844</v>
       </c>
-      <c r="Q4" s="14" t="n">
+      <c r="Q4" s="17" t="n">
         <v>123406660550</v>
       </c>
-      <c r="R4" s="14" t="n">
+      <c r="R4" s="17" t="n">
         <v>121373382142</v>
       </c>
-      <c r="S4" s="14" t="n">
+      <c r="S4" s="17" t="n">
         <v>117161902725</v>
       </c>
-      <c r="T4" s="14" t="n">
+      <c r="T4" s="17" t="n">
         <v>116592014868</v>
       </c>
-      <c r="U4" s="14" t="n">
+      <c r="U4" s="17" t="n">
         <v>118448779098</v>
       </c>
-      <c r="V4" s="14" t="n">
+      <c r="V4" s="17" t="n">
         <v>115982151879</v>
       </c>
-      <c r="W4" s="14" t="n">
+      <c r="W4" s="17" t="n">
         <v>116965882167</v>
       </c>
-      <c r="X4" s="14" t="n">
+      <c r="X4" s="17" t="n">
         <v>122185036488</v>
       </c>
-      <c r="Y4" s="14" t="n">
+      <c r="Y4" s="17" t="n">
         <v>132178486506.387</v>
       </c>
-      <c r="Z4" s="14" t="n">
-        <v>143993638543.836</v>
-      </c>
-      <c r="AA4" s="14" t="n">
-        <v>169810521226.128</v>
-      </c>
-      <c r="AB4" s="14" t="n">
-        <v>211533087512.337</v>
-      </c>
-      <c r="AC4" s="14" t="n">
-        <v>229761957048.789</v>
-      </c>
-      <c r="AD4" s="14" t="n">
-        <v>265663361025.89</v>
-      </c>
-      <c r="AE4" s="14" t="n">
-        <v>295165178110.853</v>
-      </c>
-      <c r="AF4" s="14" t="n">
-        <v>328153480580.909</v>
-      </c>
-      <c r="AG4" s="14" t="n">
-        <v>377988099747.404</v>
-      </c>
-      <c r="AH4" s="14" t="n">
-        <v>381555380786.985</v>
-      </c>
-      <c r="AI4" s="14" t="n">
-        <v>362403868841.008</v>
-      </c>
-      <c r="AJ4" s="14" t="n">
-        <v>368565915961.162</v>
-      </c>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="14"/>
-      <c r="AN4" s="14" t="n">
-        <v>6246925.665</v>
-      </c>
-      <c r="AO4" s="14"/>
-      <c r="AP4" s="14"/>
-      <c r="AQ4" s="14"/>
-      <c r="AR4" s="14"/>
-      <c r="AS4" s="14"/>
-      <c r="AT4" s="14"/>
-      <c r="AU4" s="14"/>
-      <c r="AV4" s="14"/>
-      <c r="AW4" s="14"/>
-      <c r="AX4" s="14"/>
-      <c r="AY4" s="14"/>
-      <c r="AZ4" s="14"/>
-      <c r="BA4" s="14"/>
-      <c r="BB4" s="14"/>
-      <c r="BC4" s="14"/>
+      <c r="Z4" s="17" t="n">
+        <v>143993638622.327</v>
+      </c>
+      <c r="AA4" s="17" t="n">
+        <v>169810521136.485</v>
+      </c>
+      <c r="AB4" s="17" t="n">
+        <v>211533087303.861</v>
+      </c>
+      <c r="AC4" s="17" t="n">
+        <v>229775031821.915</v>
+      </c>
+      <c r="AD4" s="17" t="n">
+        <v>265664518702.457</v>
+      </c>
+      <c r="AE4" s="17" t="n">
+        <v>295165186343.118</v>
+      </c>
+      <c r="AF4" s="17" t="n">
+        <v>328154422853.492</v>
+      </c>
+      <c r="AG4" s="17" t="n">
+        <v>377988086084.829</v>
+      </c>
+      <c r="AH4" s="17" t="n">
+        <v>367650065478.427</v>
+      </c>
+      <c r="AI4" s="17" t="n">
+        <v>362696345236.665</v>
+      </c>
+      <c r="AJ4" s="17" t="n">
+        <v>368563658869.492</v>
+      </c>
+      <c r="AK4" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="17" t="n">
+        <v>688297065.81</v>
+      </c>
+      <c r="AM4" s="17" t="n">
+        <v>17295</v>
+      </c>
+      <c r="AN4" s="17" t="n">
+        <v>68529812030.32</v>
+      </c>
+      <c r="AO4" s="17"/>
+      <c r="AP4" s="17"/>
+      <c r="AQ4" s="17"/>
+      <c r="AR4" s="17"/>
+      <c r="AS4" s="17"/>
+      <c r="AT4" s="17"/>
+      <c r="AU4" s="17"/>
+      <c r="AV4" s="17"/>
+      <c r="AW4" s="17"/>
+      <c r="AX4" s="17"/>
+      <c r="AY4" s="17"/>
+      <c r="AZ4" s="17"/>
+      <c r="BA4" s="17"/>
+      <c r="BB4" s="17"/>
+      <c r="BC4" s="17"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -2591,127 +2597,127 @@
       <c r="N5" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="14" t="n">
+      <c r="O5" s="17" t="n">
         <v>289694000000</v>
       </c>
-      <c r="P5" s="14" t="n">
+      <c r="P5" s="17" t="n">
         <v>262324000000</v>
       </c>
-      <c r="Q5" s="14" t="n">
+      <c r="Q5" s="17" t="n">
         <v>286834000000</v>
       </c>
-      <c r="R5" s="14" t="n">
+      <c r="R5" s="17" t="n">
         <v>278497000000</v>
       </c>
-      <c r="S5" s="14" t="n">
+      <c r="S5" s="17" t="n">
         <v>268553000000</v>
       </c>
-      <c r="T5" s="14" t="n">
+      <c r="T5" s="17" t="n">
         <v>259373000000</v>
       </c>
-      <c r="U5" s="14" t="n">
+      <c r="U5" s="17" t="n">
         <v>253130000000</v>
       </c>
-      <c r="V5" s="14" t="n">
+      <c r="V5" s="17" t="n">
         <v>258251000000</v>
       </c>
-      <c r="W5" s="14" t="n">
+      <c r="W5" s="17" t="n">
         <v>255793000000</v>
       </c>
-      <c r="X5" s="14" t="n">
+      <c r="X5" s="17" t="n">
         <v>261198000000</v>
       </c>
-      <c r="Y5" s="14" t="n">
+      <c r="Y5" s="17" t="n">
         <v>281029000000</v>
       </c>
-      <c r="Z5" s="14" t="n">
+      <c r="Z5" s="17" t="n">
         <v>290185000000</v>
       </c>
-      <c r="AA5" s="14" t="n">
+      <c r="AA5" s="17" t="n">
         <v>331845000000</v>
       </c>
-      <c r="AB5" s="14" t="n">
+      <c r="AB5" s="17" t="n">
         <v>387136000000</v>
       </c>
-      <c r="AC5" s="14" t="n">
+      <c r="AC5" s="17" t="n">
         <v>436439000000</v>
       </c>
-      <c r="AD5" s="14" t="n">
+      <c r="AD5" s="17" t="n">
         <v>474071000000</v>
       </c>
-      <c r="AE5" s="14" t="n">
+      <c r="AE5" s="17" t="n">
         <v>499297000000</v>
       </c>
-      <c r="AF5" s="14" t="n">
+      <c r="AF5" s="17" t="n">
         <v>528548000000</v>
       </c>
-      <c r="AG5" s="14" t="n">
+      <c r="AG5" s="17" t="n">
         <v>594632000000</v>
       </c>
-      <c r="AH5" s="14" t="n">
+      <c r="AH5" s="17" t="n">
         <v>636742000000</v>
       </c>
-      <c r="AI5" s="14" t="n">
+      <c r="AI5" s="17" t="n">
         <v>666703000000</v>
       </c>
-      <c r="AJ5" s="14" t="n">
+      <c r="AJ5" s="17" t="n">
         <v>678064000000</v>
       </c>
-      <c r="AK5" s="14" t="n">
+      <c r="AK5" s="17" t="n">
         <v>650851000000</v>
       </c>
-      <c r="AL5" s="14" t="n">
+      <c r="AL5" s="17" t="n">
         <v>607795000000</v>
       </c>
-      <c r="AM5" s="14" t="n">
+      <c r="AM5" s="17" t="n">
         <v>577897000000</v>
       </c>
-      <c r="AN5" s="14" t="n">
+      <c r="AN5" s="17" t="n">
         <v>562499000000</v>
       </c>
-      <c r="AO5" s="14" t="n">
+      <c r="AO5" s="17" t="n">
         <v>565370000000</v>
       </c>
-      <c r="AP5" s="14" t="n">
+      <c r="AP5" s="17" t="n">
         <v>568897000000</v>
       </c>
-      <c r="AQ5" s="14" t="n">
+      <c r="AQ5" s="17" t="n">
         <v>600804000000</v>
       </c>
-      <c r="AR5" s="14" t="n">
+      <c r="AR5" s="17" t="n">
         <v>653690000000</v>
       </c>
-      <c r="AS5" s="14" t="n">
+      <c r="AS5" s="17" t="n">
         <v>690363000000</v>
       </c>
-      <c r="AT5" s="14" t="n">
+      <c r="AT5" s="17" t="n">
         <v>717577000000</v>
       </c>
-      <c r="AU5" s="14" t="n">
+      <c r="AU5" s="17" t="n">
         <v>726458000000</v>
       </c>
-      <c r="AV5" s="14" t="n">
+      <c r="AV5" s="17" t="n">
         <v>775874000000</v>
       </c>
-      <c r="AW5" s="14" t="n">
+      <c r="AW5" s="17" t="n">
         <v>859539000000</v>
       </c>
-      <c r="AX5" s="14" t="n">
+      <c r="AX5" s="17" t="n">
         <v>878467000000</v>
       </c>
-      <c r="AY5" s="14" t="n">
+      <c r="AY5" s="17" t="n">
         <v>883218000000</v>
       </c>
-      <c r="AZ5" s="14" t="n">
+      <c r="AZ5" s="17" t="n">
         <v>895811000000</v>
       </c>
-      <c r="BA5" s="14" t="n">
+      <c r="BA5" s="17" t="n">
         <v>914366000000</v>
       </c>
-      <c r="BB5" s="14" t="n">
+      <c r="BB5" s="17" t="n">
         <v>934814000000</v>
       </c>
-      <c r="BC5" s="14"/>
+      <c r="BC5" s="17"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -2726,127 +2732,127 @@
       <c r="N6" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="14" t="str">
+      <c r="O6" s="17" t="str">
         <f>Sum(O2:O5)</f>
       </c>
-      <c r="P6" s="14" t="str">
+      <c r="P6" s="17" t="str">
         <f>Sum(P2:P5)</f>
       </c>
-      <c r="Q6" s="14" t="str">
+      <c r="Q6" s="17" t="str">
         <f>Sum(Q2:Q5)</f>
       </c>
-      <c r="R6" s="14" t="str">
+      <c r="R6" s="17" t="str">
         <f>Sum(R2:R5)</f>
       </c>
-      <c r="S6" s="14" t="str">
+      <c r="S6" s="17" t="str">
         <f>Sum(S2:S5)</f>
       </c>
-      <c r="T6" s="14" t="str">
+      <c r="T6" s="17" t="str">
         <f>Sum(T2:T5)</f>
       </c>
-      <c r="U6" s="14" t="str">
+      <c r="U6" s="17" t="str">
         <f>Sum(U2:U5)</f>
       </c>
-      <c r="V6" s="14" t="str">
+      <c r="V6" s="17" t="str">
         <f>Sum(V2:V5)</f>
       </c>
-      <c r="W6" s="14" t="str">
+      <c r="W6" s="17" t="str">
         <f>Sum(W2:W5)</f>
       </c>
-      <c r="X6" s="14" t="str">
+      <c r="X6" s="17" t="str">
         <f>Sum(X2:X5)</f>
       </c>
-      <c r="Y6" s="14" t="str">
+      <c r="Y6" s="17" t="str">
         <f>Sum(Y2:Y5)</f>
       </c>
-      <c r="Z6" s="14" t="str">
+      <c r="Z6" s="17" t="str">
         <f>Sum(Z2:Z5)</f>
       </c>
-      <c r="AA6" s="14" t="str">
+      <c r="AA6" s="17" t="str">
         <f>Sum(AA2:AA5)</f>
       </c>
-      <c r="AB6" s="14" t="str">
+      <c r="AB6" s="17" t="str">
         <f>Sum(AB2:AB5)</f>
       </c>
-      <c r="AC6" s="14" t="str">
+      <c r="AC6" s="17" t="str">
         <f>Sum(AC2:AC5)</f>
       </c>
-      <c r="AD6" s="14" t="str">
+      <c r="AD6" s="17" t="str">
         <f>Sum(AD2:AD5)</f>
       </c>
-      <c r="AE6" s="14" t="str">
+      <c r="AE6" s="17" t="str">
         <f>Sum(AE2:AE5)</f>
       </c>
-      <c r="AF6" s="14" t="str">
+      <c r="AF6" s="17" t="str">
         <f>Sum(AF2:AF5)</f>
       </c>
-      <c r="AG6" s="14" t="str">
+      <c r="AG6" s="17" t="str">
         <f>Sum(AG2:AG5)</f>
       </c>
-      <c r="AH6" s="14" t="str">
+      <c r="AH6" s="17" t="str">
         <f>Sum(AH2:AH5)</f>
       </c>
-      <c r="AI6" s="14" t="str">
+      <c r="AI6" s="17" t="str">
         <f>Sum(AI2:AI5)</f>
       </c>
-      <c r="AJ6" s="14" t="str">
+      <c r="AJ6" s="17" t="str">
         <f>Sum(AJ2:AJ5)</f>
       </c>
-      <c r="AK6" s="14" t="str">
+      <c r="AK6" s="17" t="str">
         <f>Sum(AK2:AK5)</f>
       </c>
-      <c r="AL6" s="14" t="str">
+      <c r="AL6" s="17" t="str">
         <f>Sum(AL2:AL5)</f>
       </c>
-      <c r="AM6" s="14" t="str">
+      <c r="AM6" s="17" t="str">
         <f>Sum(AM2:AM5)</f>
       </c>
-      <c r="AN6" s="14" t="str">
+      <c r="AN6" s="17" t="str">
         <f>Sum(AN2:AN5)</f>
       </c>
-      <c r="AO6" s="14" t="str">
+      <c r="AO6" s="17" t="str">
         <f>Sum(AO2:AO5)</f>
       </c>
-      <c r="AP6" s="14" t="str">
+      <c r="AP6" s="17" t="str">
         <f>Sum(AP2:AP5)</f>
       </c>
-      <c r="AQ6" s="14" t="str">
+      <c r="AQ6" s="17" t="str">
         <f>Sum(AQ2:AQ5)</f>
       </c>
-      <c r="AR6" s="14" t="str">
+      <c r="AR6" s="17" t="str">
         <f>Sum(AR2:AR5)</f>
       </c>
-      <c r="AS6" s="14" t="str">
+      <c r="AS6" s="17" t="str">
         <f>Sum(AS2:AS5)</f>
       </c>
-      <c r="AT6" s="14" t="str">
+      <c r="AT6" s="17" t="str">
         <f>Sum(AT2:AT5)</f>
       </c>
-      <c r="AU6" s="14" t="str">
+      <c r="AU6" s="17" t="str">
         <f>Sum(AU2:AU5)</f>
       </c>
-      <c r="AV6" s="14" t="str">
+      <c r="AV6" s="17" t="str">
         <f>Sum(AV2:AV5)</f>
       </c>
-      <c r="AW6" s="14" t="str">
+      <c r="AW6" s="17" t="str">
         <f>Sum(AW2:AW5)</f>
       </c>
-      <c r="AX6" s="14" t="str">
+      <c r="AX6" s="17" t="str">
         <f>Sum(AX2:AX5)</f>
       </c>
-      <c r="AY6" s="14" t="str">
+      <c r="AY6" s="17" t="str">
         <f>Sum(AY2:AY5)</f>
       </c>
-      <c r="AZ6" s="14" t="str">
+      <c r="AZ6" s="17" t="str">
         <f>Sum(AZ2:AZ5)</f>
       </c>
-      <c r="BA6" s="14" t="str">
+      <c r="BA6" s="17" t="str">
         <f>Sum(BA2:BA5)</f>
       </c>
-      <c r="BB6" s="14" t="str">
+      <c r="BB6" s="17" t="str">
         <f>Sum(BB2:BB5)</f>
       </c>
-      <c r="BC6" s="14"/>
+      <c r="BC6" s="17"/>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -3007,16 +3013,16 @@
       <c r="B10" t="str">
         <f>N10</f>
       </c>
-      <c r="C10" s="14" t="str">
+      <c r="C10" s="17" t="str">
         <f>AS10</f>
       </c>
-      <c r="D10" s="14" t="str">
+      <c r="D10" s="17" t="str">
         <f>AU10</f>
       </c>
-      <c r="E10" s="14" t="str">
+      <c r="E10" s="17" t="str">
         <f>AV10</f>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="1" t="str">
         <f>AV10/AU10-1</f>
       </c>
@@ -3034,71 +3040,71 @@
       <c r="N10" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="14"/>
-      <c r="AG10" s="14"/>
-      <c r="AH10" s="14"/>
-      <c r="AI10" s="14"/>
-      <c r="AJ10" s="14"/>
-      <c r="AK10" s="14" t="n">
-        <v>36390869420.0532</v>
-      </c>
-      <c r="AL10" s="14" t="n">
-        <v>25896384490.0193</v>
-      </c>
-      <c r="AM10" s="14" t="n">
-        <v>19992431792.9514</v>
-      </c>
-      <c r="AN10" s="14" t="n">
-        <v>30286399449.1285</v>
-      </c>
-      <c r="AO10" s="14" t="n">
-        <v>41815605260.499</v>
-      </c>
-      <c r="AP10" s="14" t="n">
-        <v>37884999724.2074</v>
-      </c>
-      <c r="AQ10" s="14" t="n">
-        <v>41573208124.9344</v>
-      </c>
-      <c r="AR10" s="14" t="n">
-        <v>44992590026.8429</v>
-      </c>
-      <c r="AS10" s="14" t="n">
-        <v>57987138191.6318</v>
-      </c>
-      <c r="AT10" s="14" t="n">
-        <v>27730527616.1122</v>
-      </c>
-      <c r="AU10" s="14" t="n">
-        <v>40499381567.492</v>
-      </c>
-      <c r="AV10" s="14" t="n">
-        <v>65793606575.0316</v>
-      </c>
-      <c r="AW10" s="14"/>
-      <c r="AX10" s="14"/>
-      <c r="AY10" s="14"/>
-      <c r="AZ10" s="14"/>
-      <c r="BA10" s="14"/>
-      <c r="BB10" s="14"/>
-      <c r="BC10" s="14"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="17"/>
+      <c r="AG10" s="17"/>
+      <c r="AH10" s="17"/>
+      <c r="AI10" s="17"/>
+      <c r="AJ10" s="17"/>
+      <c r="AK10" s="17" t="n">
+        <v>36390987981.8448</v>
+      </c>
+      <c r="AL10" s="17" t="n">
+        <v>26221905738.2968</v>
+      </c>
+      <c r="AM10" s="17" t="n">
+        <v>19925213441.3071</v>
+      </c>
+      <c r="AN10" s="17" t="n">
+        <v>29222168317.7287</v>
+      </c>
+      <c r="AO10" s="17" t="n">
+        <v>41682205250.0166</v>
+      </c>
+      <c r="AP10" s="17" t="n">
+        <v>38750156644.7742</v>
+      </c>
+      <c r="AQ10" s="17" t="n">
+        <v>41555475393.5778</v>
+      </c>
+      <c r="AR10" s="17" t="n">
+        <v>45002603100.1161</v>
+      </c>
+      <c r="AS10" s="17" t="n">
+        <v>58094201874.9828</v>
+      </c>
+      <c r="AT10" s="17" t="n">
+        <v>27842081578.4401</v>
+      </c>
+      <c r="AU10" s="17" t="n">
+        <v>40522574821.365</v>
+      </c>
+      <c r="AV10" s="17" t="n">
+        <v>65793606959.6752</v>
+      </c>
+      <c r="AW10" s="17"/>
+      <c r="AX10" s="17"/>
+      <c r="AY10" s="17"/>
+      <c r="AZ10" s="17"/>
+      <c r="BA10" s="17"/>
+      <c r="BB10" s="17"/>
+      <c r="BC10" s="17"/>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -3107,16 +3113,16 @@
       <c r="B11" t="str">
         <f>N11</f>
       </c>
-      <c r="C11" s="14" t="str">
+      <c r="C11" s="17" t="str">
         <f>AS11</f>
       </c>
-      <c r="D11" s="14" t="str">
+      <c r="D11" s="17" t="str">
         <f>AU11</f>
       </c>
-      <c r="E11" s="14" t="str">
+      <c r="E11" s="17" t="str">
         <f>AV11</f>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="1" t="str">
         <f>AV11/AU11-1</f>
       </c>
@@ -3134,71 +3140,71 @@
       <c r="N11" t="s">
         <v>43</v>
       </c>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="14"/>
-      <c r="AH11" s="14"/>
-      <c r="AI11" s="14"/>
-      <c r="AJ11" s="14"/>
-      <c r="AK11" s="14" t="n">
-        <v>432330186054.03</v>
-      </c>
-      <c r="AL11" s="14" t="n">
-        <v>368750341721.862</v>
-      </c>
-      <c r="AM11" s="14" t="n">
-        <v>338132277217.976</v>
-      </c>
-      <c r="AN11" s="14" t="n">
-        <v>312773586648.454</v>
-      </c>
-      <c r="AO11" s="14" t="n">
-        <v>328542572360.358</v>
-      </c>
-      <c r="AP11" s="14" t="n">
-        <v>353490764546.252</v>
-      </c>
-      <c r="AQ11" s="14" t="n">
-        <v>387087885833.412</v>
-      </c>
-      <c r="AR11" s="14" t="n">
-        <v>405081653062.029</v>
-      </c>
-      <c r="AS11" s="14" t="n">
-        <v>431127980837.866</v>
-      </c>
-      <c r="AT11" s="14" t="n">
-        <v>405348242639.538</v>
-      </c>
-      <c r="AU11" s="14" t="n">
-        <v>392694446194.055</v>
-      </c>
-      <c r="AV11" s="14" t="n">
-        <v>390453368175.855</v>
-      </c>
-      <c r="AW11" s="14"/>
-      <c r="AX11" s="14"/>
-      <c r="AY11" s="14"/>
-      <c r="AZ11" s="14"/>
-      <c r="BA11" s="14"/>
-      <c r="BB11" s="14"/>
-      <c r="BC11" s="14"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="17"/>
+      <c r="AI11" s="17"/>
+      <c r="AJ11" s="17"/>
+      <c r="AK11" s="17" t="n">
+        <v>432535668277.784</v>
+      </c>
+      <c r="AL11" s="17" t="n">
+        <v>369659376253.123</v>
+      </c>
+      <c r="AM11" s="17" t="n">
+        <v>338408288754.957</v>
+      </c>
+      <c r="AN11" s="17" t="n">
+        <v>228151376115.108</v>
+      </c>
+      <c r="AO11" s="17" t="n">
+        <v>328878290270.115</v>
+      </c>
+      <c r="AP11" s="17" t="n">
+        <v>354138335651.29</v>
+      </c>
+      <c r="AQ11" s="17" t="n">
+        <v>386955495132.106</v>
+      </c>
+      <c r="AR11" s="17" t="n">
+        <v>405212598176.643</v>
+      </c>
+      <c r="AS11" s="17" t="n">
+        <v>431190002025.514</v>
+      </c>
+      <c r="AT11" s="17" t="n">
+        <v>405951814891.826</v>
+      </c>
+      <c r="AU11" s="17" t="n">
+        <v>392935143399.785</v>
+      </c>
+      <c r="AV11" s="17" t="n">
+        <v>390453124911.284</v>
+      </c>
+      <c r="AW11" s="17"/>
+      <c r="AX11" s="17"/>
+      <c r="AY11" s="17"/>
+      <c r="AZ11" s="17"/>
+      <c r="BA11" s="17"/>
+      <c r="BB11" s="17"/>
+      <c r="BC11" s="17"/>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -3207,16 +3213,16 @@
       <c r="B12" t="str">
         <f>N12</f>
       </c>
-      <c r="C12" s="14" t="str">
+      <c r="C12" s="17" t="str">
         <f>AS12</f>
       </c>
-      <c r="D12" s="14" t="str">
+      <c r="D12" s="17" t="str">
         <f>AU12</f>
       </c>
-      <c r="E12" s="14" t="str">
+      <c r="E12" s="17" t="str">
         <f>AV12</f>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="1" t="str">
         <f>AV12/AU12-1</f>
       </c>
@@ -3234,93 +3240,99 @@
       <c r="N12" t="s">
         <v>44</v>
       </c>
-      <c r="O12" s="14" t="n">
+      <c r="O12" s="17" t="n">
         <v>248917998790.874</v>
       </c>
-      <c r="P12" s="14" t="n">
+      <c r="P12" s="17" t="n">
         <v>271885202720.129</v>
       </c>
-      <c r="Q12" s="14" t="n">
+      <c r="Q12" s="17" t="n">
         <v>240412560734.939</v>
       </c>
-      <c r="R12" s="14" t="n">
+      <c r="R12" s="17" t="n">
         <v>231031479111.987</v>
       </c>
-      <c r="S12" s="14" t="n">
+      <c r="S12" s="17" t="n">
         <v>218250472650.085</v>
       </c>
-      <c r="T12" s="14" t="n">
+      <c r="T12" s="17" t="n">
         <v>212677633977.603</v>
       </c>
-      <c r="U12" s="14" t="n">
+      <c r="U12" s="17" t="n">
         <v>212071611328.834</v>
       </c>
-      <c r="V12" s="14" t="n">
+      <c r="V12" s="17" t="n">
         <v>204034317412.979</v>
       </c>
-      <c r="W12" s="14" t="n">
+      <c r="W12" s="17" t="n">
         <v>203216983313.484</v>
       </c>
-      <c r="X12" s="14" t="n">
+      <c r="X12" s="17" t="n">
         <v>209688280565.4</v>
       </c>
-      <c r="Y12" s="14" t="n">
+      <c r="Y12" s="17" t="n">
         <v>222214954426.99</v>
       </c>
-      <c r="Z12" s="14" t="n">
-        <v>236349380759.976</v>
-      </c>
-      <c r="AA12" s="14" t="n">
-        <v>274407867785.644</v>
-      </c>
-      <c r="AB12" s="14" t="n">
-        <v>335392180495.053</v>
-      </c>
-      <c r="AC12" s="14" t="n">
-        <v>355611032054.797</v>
-      </c>
-      <c r="AD12" s="14" t="n">
-        <v>399034409966.236</v>
-      </c>
-      <c r="AE12" s="14" t="n">
-        <v>429398322936.051</v>
-      </c>
-      <c r="AF12" s="14" t="n">
-        <v>464598647461.156</v>
-      </c>
-      <c r="AG12" s="14" t="n">
-        <v>524270052465.528</v>
-      </c>
-      <c r="AH12" s="14" t="n">
-        <v>523860817748.021</v>
-      </c>
-      <c r="AI12" s="14" t="n">
-        <v>493294382841.294</v>
-      </c>
-      <c r="AJ12" s="14" t="n">
-        <v>491810684195.121</v>
-      </c>
-      <c r="AK12" s="14"/>
-      <c r="AL12" s="14"/>
-      <c r="AM12" s="14"/>
-      <c r="AN12" s="14" t="n">
-        <v>7816340.87652611</v>
-      </c>
-      <c r="AO12" s="14"/>
-      <c r="AP12" s="14"/>
-      <c r="AQ12" s="14"/>
-      <c r="AR12" s="14"/>
-      <c r="AS12" s="14"/>
-      <c r="AT12" s="14"/>
-      <c r="AU12" s="14"/>
-      <c r="AV12" s="14"/>
-      <c r="AW12" s="14"/>
-      <c r="AX12" s="14"/>
-      <c r="AY12" s="14"/>
-      <c r="AZ12" s="14"/>
-      <c r="BA12" s="14"/>
-      <c r="BB12" s="14"/>
-      <c r="BC12" s="14"/>
+      <c r="Z12" s="17" t="n">
+        <v>236349380888.81</v>
+      </c>
+      <c r="AA12" s="17" t="n">
+        <v>274407867640.784</v>
+      </c>
+      <c r="AB12" s="17" t="n">
+        <v>335392180164.508</v>
+      </c>
+      <c r="AC12" s="17" t="n">
+        <v>355631268362.082</v>
+      </c>
+      <c r="AD12" s="17" t="n">
+        <v>399036148831.483</v>
+      </c>
+      <c r="AE12" s="17" t="n">
+        <v>429398334912.128</v>
+      </c>
+      <c r="AF12" s="17" t="n">
+        <v>464599981527.663</v>
+      </c>
+      <c r="AG12" s="17" t="n">
+        <v>524270033515.516</v>
+      </c>
+      <c r="AH12" s="17" t="n">
+        <v>504769356284.26</v>
+      </c>
+      <c r="AI12" s="17" t="n">
+        <v>493692493831.535</v>
+      </c>
+      <c r="AJ12" s="17" t="n">
+        <v>491807672354.496</v>
+      </c>
+      <c r="AK12" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="17" t="n">
+        <v>886010996.464129</v>
+      </c>
+      <c r="AM12" s="17" t="n">
+        <v>21864.1326640477</v>
+      </c>
+      <c r="AN12" s="17" t="n">
+        <v>85746557548.1986</v>
+      </c>
+      <c r="AO12" s="17"/>
+      <c r="AP12" s="17"/>
+      <c r="AQ12" s="17"/>
+      <c r="AR12" s="17"/>
+      <c r="AS12" s="17"/>
+      <c r="AT12" s="17"/>
+      <c r="AU12" s="17"/>
+      <c r="AV12" s="17"/>
+      <c r="AW12" s="17"/>
+      <c r="AX12" s="17"/>
+      <c r="AY12" s="17"/>
+      <c r="AZ12" s="17"/>
+      <c r="BA12" s="17"/>
+      <c r="BB12" s="17"/>
+      <c r="BC12" s="17"/>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -3329,16 +3341,16 @@
       <c r="B13" t="str">
         <f>N13</f>
       </c>
-      <c r="C13" s="14" t="str">
+      <c r="C13" s="17" t="str">
         <f>AS13</f>
       </c>
-      <c r="D13" s="14" t="str">
+      <c r="D13" s="17" t="str">
         <f>AU13</f>
       </c>
-      <c r="E13" s="14" t="str">
+      <c r="E13" s="17" t="str">
         <f>AV13</f>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="1" t="str">
         <f>AV13/AU13-1</f>
       </c>
@@ -3356,127 +3368,127 @@
       <c r="N13" t="s">
         <v>43</v>
       </c>
-      <c r="O13" s="14" t="n">
+      <c r="O13" s="17" t="n">
         <v>599168867522.029</v>
       </c>
-      <c r="P13" s="14" t="n">
+      <c r="P13" s="17" t="n">
         <v>523832662841.61</v>
       </c>
-      <c r="Q13" s="14" t="n">
+      <c r="Q13" s="17" t="n">
         <v>558790717928.113</v>
       </c>
-      <c r="R13" s="14" t="n">
+      <c r="R13" s="17" t="n">
         <v>530112720785.642</v>
       </c>
-      <c r="S13" s="14" t="n">
+      <c r="S13" s="17" t="n">
         <v>500263462937.87</v>
       </c>
-      <c r="T13" s="14" t="n">
+      <c r="T13" s="17" t="n">
         <v>473127049224.817</v>
       </c>
-      <c r="U13" s="14" t="n">
+      <c r="U13" s="17" t="n">
         <v>453205912162.704</v>
       </c>
-      <c r="V13" s="14" t="n">
+      <c r="V13" s="17" t="n">
         <v>454311854475.601</v>
       </c>
-      <c r="W13" s="14" t="n">
+      <c r="W13" s="17" t="n">
         <v>444415763380.374</v>
       </c>
-      <c r="X13" s="14" t="n">
+      <c r="X13" s="17" t="n">
         <v>448255867341.827</v>
       </c>
-      <c r="Y13" s="14" t="n">
+      <c r="Y13" s="17" t="n">
         <v>472458477005.221</v>
       </c>
-      <c r="Z13" s="14" t="n">
+      <c r="Z13" s="17" t="n">
         <v>476306076778.206</v>
       </c>
-      <c r="AA13" s="14" t="n">
+      <c r="AA13" s="17" t="n">
         <v>536249922724.551</v>
       </c>
-      <c r="AB13" s="14" t="n">
+      <c r="AB13" s="17" t="n">
         <v>613815969478.346</v>
       </c>
-      <c r="AC13" s="14" t="n">
+      <c r="AC13" s="17" t="n">
         <v>675492693448.842</v>
       </c>
-      <c r="AD13" s="14" t="n">
+      <c r="AD13" s="17" t="n">
         <v>712068992263.739</v>
       </c>
-      <c r="AE13" s="14" t="n">
+      <c r="AE13" s="17" t="n">
         <v>726363779830.702</v>
       </c>
-      <c r="AF13" s="14" t="n">
+      <c r="AF13" s="17" t="n">
         <v>748316566637.036</v>
       </c>
-      <c r="AG13" s="14" t="n">
+      <c r="AG13" s="17" t="n">
         <v>824755462000.025</v>
       </c>
-      <c r="AH13" s="14" t="n">
+      <c r="AH13" s="17" t="n">
         <v>874222201051.157</v>
       </c>
-      <c r="AI13" s="14" t="n">
+      <c r="AI13" s="17" t="n">
         <v>907498162133.927</v>
       </c>
-      <c r="AJ13" s="14" t="n">
+      <c r="AJ13" s="17" t="n">
         <v>904801842293.038</v>
       </c>
-      <c r="AK13" s="14" t="n">
+      <c r="AK13" s="17" t="n">
         <v>853010324247.841</v>
       </c>
-      <c r="AL13" s="14" t="n">
+      <c r="AL13" s="17" t="n">
         <v>782384642250.63</v>
       </c>
-      <c r="AM13" s="14" t="n">
+      <c r="AM13" s="17" t="n">
         <v>730570492868.181</v>
       </c>
-      <c r="AN13" s="14" t="n">
+      <c r="AN13" s="17" t="n">
         <v>703815630677.12</v>
       </c>
-      <c r="AO13" s="14" t="n">
+      <c r="AO13" s="17" t="n">
         <v>701796989317.852</v>
       </c>
-      <c r="AP13" s="14" t="n">
+      <c r="AP13" s="17" t="n">
         <v>694452568033.404</v>
       </c>
-      <c r="AQ13" s="14" t="n">
+      <c r="AQ13" s="17" t="n">
         <v>717473530179.755</v>
       </c>
-      <c r="AR13" s="14" t="n">
+      <c r="AR13" s="17" t="n">
         <v>766457961125.701</v>
       </c>
-      <c r="AS13" s="14" t="n">
+      <c r="AS13" s="17" t="n">
         <v>799019734497.993</v>
       </c>
-      <c r="AT13" s="14" t="n">
+      <c r="AT13" s="17" t="n">
         <v>802883816589.107</v>
       </c>
-      <c r="AU13" s="14" t="n">
+      <c r="AU13" s="17" t="n">
         <v>759690979706.108</v>
       </c>
-      <c r="AV13" s="14" t="n">
+      <c r="AV13" s="17" t="n">
         <v>775874000000</v>
       </c>
-      <c r="AW13" s="14" t="n">
+      <c r="AW13" s="17" t="n">
         <v>837181247646.527</v>
       </c>
-      <c r="AX13" s="14" t="n">
+      <c r="AX13" s="17" t="n">
         <v>837245992301.702</v>
       </c>
-      <c r="AY13" s="14" t="n">
+      <c r="AY13" s="17" t="n">
         <v>824647554246.88</v>
       </c>
-      <c r="AZ13" s="14" t="n">
+      <c r="AZ13" s="17" t="n">
         <v>819236206162.472</v>
       </c>
-      <c r="BA13" s="14" t="n">
+      <c r="BA13" s="17" t="n">
         <v>819144705553.104</v>
       </c>
-      <c r="BB13" s="14" t="n">
+      <c r="BB13" s="17" t="n">
         <v>820305837219.535</v>
       </c>
-      <c r="BC13" s="14"/>
+      <c r="BC13" s="17"/>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -3485,16 +3497,16 @@
       <c r="B14" t="str">
         <f>N14</f>
       </c>
-      <c r="C14" s="14" t="str">
+      <c r="C14" s="17" t="str">
         <f>AS14</f>
       </c>
-      <c r="D14" s="14" t="str">
+      <c r="D14" s="17" t="str">
         <f>AU14</f>
       </c>
-      <c r="E14" s="14" t="str">
+      <c r="E14" s="17" t="str">
         <f>AV14</f>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="1" t="str">
         <f>AV14/AU14-1</f>
       </c>
@@ -3512,127 +3524,127 @@
       <c r="N14" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="14" t="str">
+      <c r="O14" s="17" t="str">
         <f>Sum(O10:O13)</f>
       </c>
-      <c r="P14" s="14" t="str">
+      <c r="P14" s="17" t="str">
         <f>Sum(P10:P13)</f>
       </c>
-      <c r="Q14" s="14" t="str">
+      <c r="Q14" s="17" t="str">
         <f>Sum(Q10:Q13)</f>
       </c>
-      <c r="R14" s="14" t="str">
+      <c r="R14" s="17" t="str">
         <f>Sum(R10:R13)</f>
       </c>
-      <c r="S14" s="14" t="str">
+      <c r="S14" s="17" t="str">
         <f>Sum(S10:S13)</f>
       </c>
-      <c r="T14" s="14" t="str">
+      <c r="T14" s="17" t="str">
         <f>Sum(T10:T13)</f>
       </c>
-      <c r="U14" s="14" t="str">
+      <c r="U14" s="17" t="str">
         <f>Sum(U10:U13)</f>
       </c>
-      <c r="V14" s="14" t="str">
+      <c r="V14" s="17" t="str">
         <f>Sum(V10:V13)</f>
       </c>
-      <c r="W14" s="14" t="str">
+      <c r="W14" s="17" t="str">
         <f>Sum(W10:W13)</f>
       </c>
-      <c r="X14" s="14" t="str">
+      <c r="X14" s="17" t="str">
         <f>Sum(X10:X13)</f>
       </c>
-      <c r="Y14" s="14" t="str">
+      <c r="Y14" s="17" t="str">
         <f>Sum(Y10:Y13)</f>
       </c>
-      <c r="Z14" s="14" t="str">
+      <c r="Z14" s="17" t="str">
         <f>Sum(Z10:Z13)</f>
       </c>
-      <c r="AA14" s="14" t="str">
+      <c r="AA14" s="17" t="str">
         <f>Sum(AA10:AA13)</f>
       </c>
-      <c r="AB14" s="14" t="str">
+      <c r="AB14" s="17" t="str">
         <f>Sum(AB10:AB13)</f>
       </c>
-      <c r="AC14" s="14" t="str">
+      <c r="AC14" s="17" t="str">
         <f>Sum(AC10:AC13)</f>
       </c>
-      <c r="AD14" s="14" t="str">
+      <c r="AD14" s="17" t="str">
         <f>Sum(AD10:AD13)</f>
       </c>
-      <c r="AE14" s="14" t="str">
+      <c r="AE14" s="17" t="str">
         <f>Sum(AE10:AE13)</f>
       </c>
-      <c r="AF14" s="14" t="str">
+      <c r="AF14" s="17" t="str">
         <f>Sum(AF10:AF13)</f>
       </c>
-      <c r="AG14" s="14" t="str">
+      <c r="AG14" s="17" t="str">
         <f>Sum(AG10:AG13)</f>
       </c>
-      <c r="AH14" s="14" t="str">
+      <c r="AH14" s="17" t="str">
         <f>Sum(AH10:AH13)</f>
       </c>
-      <c r="AI14" s="14" t="str">
+      <c r="AI14" s="17" t="str">
         <f>Sum(AI10:AI13)</f>
       </c>
-      <c r="AJ14" s="14" t="str">
+      <c r="AJ14" s="17" t="str">
         <f>Sum(AJ10:AJ13)</f>
       </c>
-      <c r="AK14" s="14" t="str">
+      <c r="AK14" s="17" t="str">
         <f>Sum(AK10:AK13)</f>
       </c>
-      <c r="AL14" s="14" t="str">
+      <c r="AL14" s="17" t="str">
         <f>Sum(AL10:AL13)</f>
       </c>
-      <c r="AM14" s="14" t="str">
+      <c r="AM14" s="17" t="str">
         <f>Sum(AM10:AM13)</f>
       </c>
-      <c r="AN14" s="14" t="str">
+      <c r="AN14" s="17" t="str">
         <f>Sum(AN10:AN13)</f>
       </c>
-      <c r="AO14" s="14" t="str">
+      <c r="AO14" s="17" t="str">
         <f>Sum(AO10:AO13)</f>
       </c>
-      <c r="AP14" s="14" t="str">
+      <c r="AP14" s="17" t="str">
         <f>Sum(AP10:AP13)</f>
       </c>
-      <c r="AQ14" s="14" t="str">
+      <c r="AQ14" s="17" t="str">
         <f>Sum(AQ10:AQ13)</f>
       </c>
-      <c r="AR14" s="14" t="str">
+      <c r="AR14" s="17" t="str">
         <f>Sum(AR10:AR13)</f>
       </c>
-      <c r="AS14" s="14" t="str">
+      <c r="AS14" s="17" t="str">
         <f>Sum(AS10:AS13)</f>
       </c>
-      <c r="AT14" s="14" t="str">
+      <c r="AT14" s="17" t="str">
         <f>Sum(AT10:AT13)</f>
       </c>
-      <c r="AU14" s="14" t="str">
+      <c r="AU14" s="17" t="str">
         <f>Sum(AU10:AU13)</f>
       </c>
-      <c r="AV14" s="14" t="str">
+      <c r="AV14" s="17" t="str">
         <f>Sum(AV10:AV13)</f>
       </c>
-      <c r="AW14" s="14" t="str">
+      <c r="AW14" s="17" t="str">
         <f>Sum(AW10:AW13)</f>
       </c>
-      <c r="AX14" s="14" t="str">
+      <c r="AX14" s="17" t="str">
         <f>Sum(AX10:AX13)</f>
       </c>
-      <c r="AY14" s="14" t="str">
+      <c r="AY14" s="17" t="str">
         <f>Sum(AY10:AY13)</f>
       </c>
-      <c r="AZ14" s="14" t="str">
+      <c r="AZ14" s="17" t="str">
         <f>Sum(AZ10:AZ13)</f>
       </c>
-      <c r="BA14" s="14" t="str">
+      <c r="BA14" s="17" t="str">
         <f>Sum(BA10:BA13)</f>
       </c>
-      <c r="BB14" s="14" t="str">
+      <c r="BB14" s="17" t="str">
         <f>Sum(BB10:BB13)</f>
       </c>
-      <c r="BC14" s="14"/>
+      <c r="BC14" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9587,110 +9599,110 @@
       <c r="L2" t="s">
         <v>117</v>
       </c>
-      <c r="M2" s="17" t="n">
+      <c r="M2" s="5" t="n">
         <v>29993312707</v>
       </c>
-      <c r="N2" s="17" t="n">
+      <c r="N2" s="5" t="n">
         <v>31945138023</v>
       </c>
-      <c r="O2" s="17" t="n">
+      <c r="O2" s="5" t="n">
         <v>29753069568</v>
       </c>
-      <c r="P2" s="17" t="n">
+      <c r="P2" s="5" t="n">
         <v>30346592157</v>
       </c>
-      <c r="Q2" s="17" t="n">
+      <c r="Q2" s="5" t="n">
         <v>31747329388</v>
       </c>
-      <c r="R2" s="17" t="n">
+      <c r="R2" s="5" t="n">
         <v>28791249139</v>
       </c>
-      <c r="S2" s="17" t="n">
+      <c r="S2" s="5" t="n">
         <v>32842967690</v>
       </c>
-      <c r="T2" s="17" t="n">
+      <c r="T2" s="5" t="n">
         <v>34627617203</v>
       </c>
-      <c r="U2" s="17" t="n">
+      <c r="U2" s="5" t="n">
         <v>37288669184</v>
       </c>
-      <c r="V2" s="17" t="n">
+      <c r="V2" s="5" t="n">
         <v>39481622310</v>
       </c>
-      <c r="W2" s="17" t="n">
+      <c r="W2" s="5" t="n">
         <v>42902822546.2254</v>
       </c>
-      <c r="X2" s="17" t="n">
+      <c r="X2" s="5" t="n">
         <v>45999287165.102</v>
       </c>
-      <c r="Y2" s="17" t="n">
+      <c r="Y2" s="5" t="n">
         <v>60247822851.393</v>
       </c>
-      <c r="Z2" s="17" t="n">
+      <c r="Z2" s="5" t="n">
         <v>70112736203.1276</v>
       </c>
-      <c r="AA2" s="17" t="n">
+      <c r="AA2" s="5" t="n">
         <v>72882060944.0123</v>
       </c>
-      <c r="AB2" s="17" t="n">
+      <c r="AB2" s="5" t="n">
         <v>73955064380.7206</v>
       </c>
-      <c r="AC2" s="17" t="n">
+      <c r="AC2" s="5" t="n">
         <v>88529377435.8539</v>
       </c>
-      <c r="AD2" s="17" t="n">
+      <c r="AD2" s="5" t="n">
         <v>99100586147.3638</v>
       </c>
-      <c r="AE2" s="17" t="n">
+      <c r="AE2" s="5" t="n">
         <v>105266669700.67</v>
       </c>
-      <c r="AF2" s="17" t="n">
+      <c r="AF2" s="5" t="n">
         <v>107245503547.368</v>
       </c>
-      <c r="AG2" s="17" t="n">
+      <c r="AG2" s="5" t="n">
         <v>96939369086.5759</v>
       </c>
-      <c r="AH2" s="17" t="n">
+      <c r="AH2" s="5" t="n">
         <v>109468302700.962</v>
       </c>
-      <c r="AI2" s="17" t="n">
+      <c r="AI2" s="5" t="n">
         <v>105499463138.199</v>
       </c>
-      <c r="AJ2" s="17" t="n">
+      <c r="AJ2" s="5" t="n">
         <v>96995856740.5779</v>
       </c>
-      <c r="AK2" s="17" t="n">
+      <c r="AK2" s="5" t="n">
         <v>82026660480.1835</v>
       </c>
-      <c r="AL2" s="17" t="n">
+      <c r="AL2" s="5" t="n">
         <v>82093613281.8144</v>
       </c>
-      <c r="AM2" s="17" t="n">
+      <c r="AM2" s="5" t="n">
         <v>103132925805.592</v>
       </c>
-      <c r="AN2" s="17" t="n">
+      <c r="AN2" s="5" t="n">
         <v>112799135328.923</v>
       </c>
-      <c r="AO2" s="17" t="n">
+      <c r="AO2" s="5" t="n">
         <v>113078047450.629</v>
       </c>
-      <c r="AP2" s="17" t="n">
+      <c r="AP2" s="5" t="n">
         <v>123281118568.194</v>
       </c>
-      <c r="AQ2" s="17" t="n">
+      <c r="AQ2" s="5" t="n">
         <v>153210907310.412</v>
       </c>
-      <c r="AR2" s="17" t="n">
+      <c r="AR2" s="5" t="n">
         <v>114361655314.093</v>
       </c>
-      <c r="AS2" s="17" t="n">
+      <c r="AS2" s="5" t="n">
         <v>122304776861.729</v>
       </c>
-      <c r="AT2" s="17" t="n">
+      <c r="AT2" s="5" t="n">
         <v>84663692097.9125</v>
       </c>
-      <c r="AU2" s="17"/>
-      <c r="AV2" s="17"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -9699,110 +9711,110 @@
       <c r="L3" t="s">
         <v>118</v>
       </c>
-      <c r="M3" s="17" t="n">
+      <c r="M3" s="5" t="n">
         <v>35960694888</v>
       </c>
-      <c r="N3" s="17" t="n">
+      <c r="N3" s="5" t="n">
         <v>37863506273</v>
       </c>
-      <c r="O3" s="17" t="n">
+      <c r="O3" s="5" t="n">
         <v>35092959873</v>
       </c>
-      <c r="P3" s="17" t="n">
+      <c r="P3" s="5" t="n">
         <v>33829226700</v>
       </c>
-      <c r="Q3" s="17" t="n">
+      <c r="Q3" s="5" t="n">
         <v>31124696371</v>
       </c>
-      <c r="R3" s="17" t="n">
+      <c r="R3" s="5" t="n">
         <v>28535738215</v>
       </c>
-      <c r="S3" s="17" t="n">
+      <c r="S3" s="5" t="n">
         <v>30194170969</v>
       </c>
-      <c r="T3" s="17" t="n">
+      <c r="T3" s="5" t="n">
         <v>29073662056</v>
       </c>
-      <c r="U3" s="17" t="n">
+      <c r="U3" s="5" t="n">
         <v>28130482737</v>
       </c>
-      <c r="V3" s="17" t="n">
+      <c r="V3" s="5" t="n">
         <v>29677352211</v>
       </c>
-      <c r="W3" s="17" t="n">
+      <c r="W3" s="5" t="n">
         <v>24339685706.4517</v>
       </c>
-      <c r="X3" s="17" t="n">
+      <c r="X3" s="5" t="n">
         <v>25668062870.6387</v>
       </c>
-      <c r="Y3" s="17" t="n">
+      <c r="Y3" s="5" t="n">
         <v>32788951053.1231</v>
       </c>
-      <c r="Z3" s="17" t="n">
+      <c r="Z3" s="5" t="n">
         <v>47830922262.423</v>
       </c>
-      <c r="AA3" s="17" t="n">
+      <c r="AA3" s="5" t="n">
         <v>58825443576.2251</v>
       </c>
-      <c r="AB3" s="17" t="n">
+      <c r="AB3" s="5" t="n">
         <v>65108861243.7038</v>
       </c>
-      <c r="AC3" s="17" t="n">
+      <c r="AC3" s="5" t="n">
         <v>68516071349.0288</v>
       </c>
-      <c r="AD3" s="17" t="n">
+      <c r="AD3" s="5" t="n">
         <v>82810086269.79</v>
       </c>
-      <c r="AE3" s="17" t="n">
+      <c r="AE3" s="5" t="n">
         <v>101935552219.899</v>
       </c>
-      <c r="AF3" s="17" t="n">
+      <c r="AF3" s="5" t="n">
         <v>91082000212.6408</v>
       </c>
-      <c r="AG3" s="17" t="n">
+      <c r="AG3" s="5" t="n">
         <v>106725389754.146</v>
       </c>
-      <c r="AH3" s="17" t="n">
+      <c r="AH3" s="5" t="n">
         <v>103383013784.238</v>
       </c>
-      <c r="AI3" s="17" t="n">
+      <c r="AI3" s="5" t="n">
         <v>98265166220.3349</v>
       </c>
-      <c r="AJ3" s="17" t="n">
+      <c r="AJ3" s="5" t="n">
         <v>86438880967.1992</v>
       </c>
-      <c r="AK3" s="17" t="n">
+      <c r="AK3" s="5" t="n">
         <v>77207039866.9569</v>
       </c>
-      <c r="AL3" s="17" t="n">
+      <c r="AL3" s="5" t="n">
         <v>71996639966.4858</v>
       </c>
-      <c r="AM3" s="17" t="n">
+      <c r="AM3" s="5" t="n">
         <v>71551510997.6919</v>
       </c>
-      <c r="AN3" s="17" t="n">
+      <c r="AN3" s="5" t="n">
         <v>76631880839.9451</v>
       </c>
-      <c r="AO3" s="17" t="n">
+      <c r="AO3" s="5" t="n">
         <v>88698325243.6305</v>
       </c>
-      <c r="AP3" s="17" t="n">
+      <c r="AP3" s="5" t="n">
         <v>92762373993.5141</v>
       </c>
-      <c r="AQ3" s="17" t="n">
+      <c r="AQ3" s="5" t="n">
         <v>98398389839.8272</v>
       </c>
-      <c r="AR3" s="17" t="n">
+      <c r="AR3" s="5" t="n">
         <v>90770167372.218</v>
       </c>
-      <c r="AS3" s="17" t="n">
+      <c r="AS3" s="5" t="n">
         <v>99021129618.9242</v>
       </c>
-      <c r="AT3" s="17" t="n">
+      <c r="AT3" s="5" t="n">
         <v>48591295833.2184</v>
       </c>
-      <c r="AU3" s="17"/>
-      <c r="AV3" s="17"/>
+      <c r="AU3" s="5"/>
+      <c r="AV3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -9811,90 +9823,90 @@
       <c r="L4" t="s">
         <v>119</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17" t="n">
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5" t="n">
         <v>30879636954.9954</v>
       </c>
-      <c r="X4" s="17" t="n">
+      <c r="X4" s="5" t="n">
         <v>28990916270.223</v>
       </c>
-      <c r="Y4" s="17" t="n">
+      <c r="Y4" s="5" t="n">
         <v>30113227132.5393</v>
       </c>
-      <c r="Z4" s="17" t="n">
+      <c r="Z4" s="5" t="n">
         <v>35201492871.434</v>
       </c>
-      <c r="AA4" s="17" t="n">
+      <c r="AA4" s="5" t="n">
         <v>35241294858.2151</v>
       </c>
-      <c r="AB4" s="17" t="n">
+      <c r="AB4" s="5" t="n">
         <v>41875695732.6547</v>
       </c>
-      <c r="AC4" s="17" t="n">
+      <c r="AC4" s="5" t="n">
         <v>49185549119.2547</v>
       </c>
-      <c r="AD4" s="17" t="n">
+      <c r="AD4" s="5" t="n">
         <v>46279650071.9425</v>
       </c>
-      <c r="AE4" s="17" t="n">
+      <c r="AE4" s="5" t="n">
         <v>54012288564.5049</v>
       </c>
-      <c r="AF4" s="17" t="n">
+      <c r="AF4" s="5" t="n">
         <v>47688602187.0404</v>
       </c>
-      <c r="AG4" s="17" t="n">
+      <c r="AG4" s="5" t="n">
         <v>39399834017.7615</v>
       </c>
-      <c r="AH4" s="17" t="n">
+      <c r="AH4" s="5" t="n">
         <v>38073802839.4699</v>
       </c>
-      <c r="AI4" s="17" t="n">
+      <c r="AI4" s="5" t="n">
         <v>42291049655.6658</v>
       </c>
-      <c r="AJ4" s="17" t="n">
+      <c r="AJ4" s="5" t="n">
         <v>32247405087.1344</v>
       </c>
-      <c r="AK4" s="17" t="n">
+      <c r="AK4" s="5" t="n">
         <v>31296907203.1947</v>
       </c>
-      <c r="AL4" s="17" t="n">
+      <c r="AL4" s="5" t="n">
         <v>28506482015.0489</v>
       </c>
-      <c r="AM4" s="17" t="n">
+      <c r="AM4" s="5" t="n">
         <v>26784143602.9829</v>
       </c>
-      <c r="AN4" s="17" t="n">
+      <c r="AN4" s="5" t="n">
         <v>29083589497.9641</v>
       </c>
-      <c r="AO4" s="17" t="n">
+      <c r="AO4" s="5" t="n">
         <v>33837415345.756</v>
       </c>
-      <c r="AP4" s="17" t="n">
+      <c r="AP4" s="5" t="n">
         <v>35835726921.9774</v>
       </c>
-      <c r="AQ4" s="17" t="n">
+      <c r="AQ4" s="5" t="n">
         <v>34006207873.992</v>
       </c>
-      <c r="AR4" s="17" t="n">
+      <c r="AR4" s="5" t="n">
         <v>52156510661.3755</v>
       </c>
-      <c r="AS4" s="17" t="n">
+      <c r="AS4" s="5" t="n">
         <v>50741258836.9179</v>
       </c>
-      <c r="AT4" s="17" t="n">
+      <c r="AT4" s="5" t="n">
         <v>20342650358.8622</v>
       </c>
-      <c r="AU4" s="17"/>
-      <c r="AV4" s="17"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -9903,110 +9915,110 @@
       <c r="L5" t="s">
         <v>120</v>
       </c>
-      <c r="M5" s="17" t="n">
+      <c r="M5" s="5" t="n">
         <v>28304563806</v>
       </c>
-      <c r="N5" s="17" t="n">
+      <c r="N5" s="5" t="n">
         <v>41243339793</v>
       </c>
-      <c r="O5" s="17" t="n">
+      <c r="O5" s="5" t="n">
         <v>34954992394</v>
       </c>
-      <c r="P5" s="17" t="n">
+      <c r="P5" s="5" t="n">
         <v>33954732784</v>
       </c>
-      <c r="Q5" s="17" t="n">
+      <c r="Q5" s="5" t="n">
         <v>32186662449</v>
       </c>
-      <c r="R5" s="17" t="n">
+      <c r="R5" s="5" t="n">
         <v>35189234715</v>
       </c>
-      <c r="S5" s="17" t="n">
+      <c r="S5" s="5" t="n">
         <v>30275743132</v>
       </c>
-      <c r="T5" s="17" t="n">
+      <c r="T5" s="5" t="n">
         <v>30248655247</v>
       </c>
-      <c r="U5" s="17" t="n">
+      <c r="U5" s="5" t="n">
         <v>30401001630</v>
       </c>
-      <c r="V5" s="17" t="n">
+      <c r="V5" s="5" t="n">
         <v>32561216997</v>
       </c>
-      <c r="W5" s="17" t="n">
+      <c r="W5" s="5" t="n">
         <v>12561996255.8882</v>
       </c>
-      <c r="X5" s="17" t="n">
+      <c r="X5" s="5" t="n">
         <v>20376379119.5963</v>
       </c>
-      <c r="Y5" s="17" t="n">
+      <c r="Y5" s="5" t="n">
         <v>19098314585.8526</v>
       </c>
-      <c r="Z5" s="17" t="n">
+      <c r="Z5" s="5" t="n">
         <v>25174152975.356</v>
       </c>
-      <c r="AA5" s="17" t="n">
+      <c r="AA5" s="5" t="n">
         <v>26390491632.9557</v>
       </c>
-      <c r="AB5" s="17" t="n">
+      <c r="AB5" s="5" t="n">
         <v>34314078131.7759</v>
       </c>
-      <c r="AC5" s="17" t="n">
+      <c r="AC5" s="5" t="n">
         <v>36302990528.4341</v>
       </c>
-      <c r="AD5" s="17" t="n">
+      <c r="AD5" s="5" t="n">
         <v>43285772133.7758</v>
       </c>
-      <c r="AE5" s="17" t="n">
+      <c r="AE5" s="5" t="n">
         <v>52322135708.5164</v>
       </c>
-      <c r="AF5" s="17" t="n">
+      <c r="AF5" s="5" t="n">
         <v>56439625804.5077</v>
       </c>
-      <c r="AG5" s="17" t="n">
+      <c r="AG5" s="5" t="n">
         <v>56543203658.8858</v>
       </c>
-      <c r="AH5" s="17" t="n">
+      <c r="AH5" s="5" t="n">
         <v>57356213929.8226</v>
       </c>
-      <c r="AI5" s="17" t="n">
+      <c r="AI5" s="5" t="n">
         <v>52731495692.821</v>
       </c>
-      <c r="AJ5" s="17" t="n">
+      <c r="AJ5" s="5" t="n">
         <v>43802955073.4203</v>
       </c>
-      <c r="AK5" s="17" t="n">
+      <c r="AK5" s="5" t="n">
         <v>38918110176.3577</v>
       </c>
-      <c r="AL5" s="17" t="n">
+      <c r="AL5" s="5" t="n">
         <v>38302470301.744</v>
       </c>
-      <c r="AM5" s="17" t="n">
+      <c r="AM5" s="5" t="n">
         <v>39722090100.4181</v>
       </c>
-      <c r="AN5" s="17" t="n">
+      <c r="AN5" s="5" t="n">
         <v>43597259051.7596</v>
       </c>
-      <c r="AO5" s="17" t="n">
+      <c r="AO5" s="5" t="n">
         <v>51940589519.8209</v>
       </c>
-      <c r="AP5" s="17" t="n">
+      <c r="AP5" s="5" t="n">
         <v>57640239173.7832</v>
       </c>
-      <c r="AQ5" s="17" t="n">
+      <c r="AQ5" s="5" t="n">
         <v>60573407783.3784</v>
       </c>
-      <c r="AR5" s="17" t="n">
+      <c r="AR5" s="5" t="n">
         <v>55378049713.2556</v>
       </c>
-      <c r="AS5" s="17" t="n">
+      <c r="AS5" s="5" t="n">
         <v>39014152184.0631</v>
       </c>
-      <c r="AT5" s="17" t="n">
+      <c r="AT5" s="5" t="n">
         <v>17449481642.3526</v>
       </c>
-      <c r="AU5" s="17"/>
-      <c r="AV5" s="17"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -10015,220 +10027,220 @@
       <c r="L6" t="s">
         <v>121</v>
       </c>
-      <c r="M6" s="17" t="n">
+      <c r="M6" s="5" t="n">
         <v>13434401635</v>
       </c>
-      <c r="N6" s="17" t="n">
+      <c r="N6" s="5" t="n">
         <v>19369182588</v>
       </c>
-      <c r="O6" s="17" t="n">
+      <c r="O6" s="5" t="n">
         <v>17619229930</v>
       </c>
-      <c r="P6" s="17" t="n">
+      <c r="P6" s="5" t="n">
         <v>17645725767</v>
       </c>
-      <c r="Q6" s="17" t="n">
+      <c r="Q6" s="5" t="n">
         <v>18075942350</v>
       </c>
-      <c r="R6" s="17" t="n">
+      <c r="R6" s="5" t="n">
         <v>19041220687</v>
       </c>
-      <c r="S6" s="17" t="n">
+      <c r="S6" s="5" t="n">
         <v>19347390330</v>
       </c>
-      <c r="T6" s="17" t="n">
+      <c r="T6" s="5" t="n">
         <v>17934428738</v>
       </c>
-      <c r="U6" s="17" t="n">
+      <c r="U6" s="5" t="n">
         <v>17288342573</v>
       </c>
-      <c r="V6" s="17" t="n">
+      <c r="V6" s="5" t="n">
         <v>19013150234</v>
       </c>
-      <c r="W6" s="17" t="n">
+      <c r="W6" s="5" t="n">
         <v>20597636512.8267</v>
       </c>
-      <c r="X6" s="17" t="n">
+      <c r="X6" s="5" t="n">
         <v>21626410588.6674</v>
       </c>
-      <c r="Y6" s="17" t="n">
+      <c r="Y6" s="5" t="n">
         <v>25988398540.367</v>
       </c>
-      <c r="Z6" s="17" t="n">
+      <c r="Z6" s="5" t="n">
         <v>32503996698.2746</v>
       </c>
-      <c r="AA6" s="17" t="n">
+      <c r="AA6" s="5" t="n">
         <v>34598872059.718</v>
       </c>
-      <c r="AB6" s="17" t="n">
+      <c r="AB6" s="5" t="n">
         <v>43335587798.781</v>
       </c>
-      <c r="AC6" s="17" t="n">
+      <c r="AC6" s="5" t="n">
         <v>45538329543.2904</v>
       </c>
-      <c r="AD6" s="17" t="n">
+      <c r="AD6" s="5" t="n">
         <v>49801473286.0533</v>
       </c>
-      <c r="AE6" s="17" t="n">
+      <c r="AE6" s="5" t="n">
         <v>54964300849.7418</v>
       </c>
-      <c r="AF6" s="17" t="n">
+      <c r="AF6" s="5" t="n">
         <v>59264807867.4139</v>
       </c>
-      <c r="AG6" s="17" t="n">
+      <c r="AG6" s="5" t="n">
         <v>58277206632.2153</v>
       </c>
-      <c r="AH6" s="17" t="n">
+      <c r="AH6" s="5" t="n">
         <v>56309134741.6547</v>
       </c>
-      <c r="AI6" s="17" t="n">
+      <c r="AI6" s="5" t="n">
         <v>56266882362.0404</v>
       </c>
-      <c r="AJ6" s="17" t="n">
+      <c r="AJ6" s="5" t="n">
         <v>47418032358.0387</v>
       </c>
-      <c r="AK6" s="17" t="n">
+      <c r="AK6" s="5" t="n">
         <v>53482722030.406</v>
       </c>
-      <c r="AL6" s="17" t="n">
+      <c r="AL6" s="5" t="n">
         <v>52427120840.6328</v>
       </c>
-      <c r="AM6" s="17" t="n">
+      <c r="AM6" s="5" t="n">
         <v>56461734363.4189</v>
       </c>
-      <c r="AN6" s="17" t="n">
+      <c r="AN6" s="5" t="n">
         <v>59242049642.4755</v>
       </c>
-      <c r="AO6" s="17" t="n">
+      <c r="AO6" s="5" t="n">
         <v>70266476117.5831</v>
       </c>
-      <c r="AP6" s="17" t="n">
+      <c r="AP6" s="5" t="n">
         <v>73354518952.1936</v>
       </c>
-      <c r="AQ6" s="17" t="n">
+      <c r="AQ6" s="5" t="n">
         <v>75798633027.2083</v>
       </c>
-      <c r="AR6" s="17" t="n">
+      <c r="AR6" s="5" t="n">
         <v>74294234511.4505</v>
       </c>
-      <c r="AS6" s="17" t="n">
+      <c r="AS6" s="5" t="n">
         <v>81672645182.5426</v>
       </c>
-      <c r="AT6" s="17" t="n">
+      <c r="AT6" s="5" t="n">
         <v>32808828005.7754</v>
       </c>
-      <c r="AU6" s="17"/>
-      <c r="AV6" s="17"/>
+      <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <f>L7</f>
       </c>
       <c r="L7"/>
-      <c r="M7" s="17" t="n">
+      <c r="M7" s="5" t="n">
         <v>12657156369</v>
       </c>
-      <c r="N7" s="17" t="n">
+      <c r="N7" s="5" t="n">
         <v>5733027167</v>
       </c>
-      <c r="O7" s="17" t="n">
+      <c r="O7" s="5" t="n">
         <v>5986408785</v>
       </c>
-      <c r="P7" s="17" t="n">
+      <c r="P7" s="5" t="n">
         <v>5597104734</v>
       </c>
-      <c r="Q7" s="17" t="n">
+      <c r="Q7" s="5" t="n">
         <v>4027272167</v>
       </c>
-      <c r="R7" s="17" t="n">
+      <c r="R7" s="5" t="n">
         <v>5034572112</v>
       </c>
-      <c r="S7" s="17" t="n">
+      <c r="S7" s="5" t="n">
         <v>5788506977</v>
       </c>
-      <c r="T7" s="17" t="n">
+      <c r="T7" s="5" t="n">
         <v>4097788635</v>
       </c>
-      <c r="U7" s="17" t="n">
+      <c r="U7" s="5" t="n">
         <v>3857386043</v>
       </c>
-      <c r="V7" s="17" t="n">
+      <c r="V7" s="5" t="n">
         <v>1451694736</v>
       </c>
-      <c r="W7" s="17" t="n">
+      <c r="W7" s="5" t="n">
         <v>896708530</v>
       </c>
-      <c r="X7" s="17" t="n">
+      <c r="X7" s="5" t="n">
         <v>1332582608.1</v>
       </c>
-      <c r="Y7" s="17" t="n">
+      <c r="Y7" s="5" t="n">
         <v>1573806973.21</v>
       </c>
-      <c r="Z7" s="17" t="n">
+      <c r="Z7" s="5" t="n">
         <v>709786293.2455</v>
       </c>
-      <c r="AA7" s="17" t="n">
+      <c r="AA7" s="5" t="n">
         <v>1836868750.7889</v>
       </c>
-      <c r="AB7" s="17" t="n">
+      <c r="AB7" s="5" t="n">
         <v>7075231414.8205</v>
       </c>
-      <c r="AC7" s="17" t="n">
+      <c r="AC7" s="5" t="n">
         <v>7092868367.2559</v>
       </c>
-      <c r="AD7" s="17" t="n">
+      <c r="AD7" s="5" t="n">
         <v>6876854944.5664</v>
       </c>
-      <c r="AE7" s="17" t="n">
+      <c r="AE7" s="5" t="n">
         <v>9487139041.4969</v>
       </c>
-      <c r="AF7" s="17" t="n">
+      <c r="AF7" s="5" t="n">
         <v>5929525859.4555</v>
       </c>
-      <c r="AG7" s="17" t="n">
+      <c r="AG7" s="5" t="n">
         <v>4811342087.0799</v>
       </c>
-      <c r="AH7" s="17" t="n">
+      <c r="AH7" s="5" t="n">
         <v>3973190873.3447</v>
       </c>
-      <c r="AI7" s="17" t="n">
+      <c r="AI7" s="5" t="n">
         <v>2739247979.5661</v>
       </c>
-      <c r="AJ7" s="17" t="n">
+      <c r="AJ7" s="5" t="n">
         <v>1325283035.7596</v>
       </c>
-      <c r="AK7" s="17" t="n">
+      <c r="AK7" s="5" t="n">
         <v>518098070.4508</v>
       </c>
-      <c r="AL7" s="17" t="n">
+      <c r="AL7" s="5" t="n">
         <v>899913864.8209</v>
       </c>
-      <c r="AM7" s="17" t="n">
+      <c r="AM7" s="5" t="n">
         <v>872368734.0903</v>
       </c>
-      <c r="AN7" s="17" t="n">
+      <c r="AN7" s="5" t="n">
         <v>501162415.0376</v>
       </c>
-      <c r="AO7" s="17" t="n">
+      <c r="AO7" s="5" t="n">
         <v>1009255457.355</v>
       </c>
-      <c r="AP7" s="17" t="n">
+      <c r="AP7" s="5" t="n">
         <v>1101647733.6542</v>
       </c>
-      <c r="AQ7" s="17" t="n">
+      <c r="AQ7" s="5" t="n">
         <v>760098902.1179</v>
       </c>
-      <c r="AR7" s="17" t="n">
+      <c r="AR7" s="5" t="n">
         <v>742455295.4319</v>
       </c>
-      <c r="AS7" s="17" t="n">
+      <c r="AS7" s="5" t="n">
         <v>21741977737.9626</v>
       </c>
-      <c r="AT7" s="17" t="n">
+      <c r="AT7" s="5" t="n">
         <v>13529156156.6481</v>
       </c>
-      <c r="AU7" s="17"/>
-      <c r="AV7" s="17"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -10237,112 +10249,112 @@
       <c r="L8" t="s">
         <v>46</v>
       </c>
-      <c r="M8" s="17" t="str">
+      <c r="M8" s="5" t="str">
         <f>Sum(M2:M7)</f>
       </c>
-      <c r="N8" s="17" t="str">
+      <c r="N8" s="5" t="str">
         <f>Sum(N2:N7)</f>
       </c>
-      <c r="O8" s="17" t="str">
+      <c r="O8" s="5" t="str">
         <f>Sum(O2:O7)</f>
       </c>
-      <c r="P8" s="17" t="str">
+      <c r="P8" s="5" t="str">
         <f>Sum(P2:P7)</f>
       </c>
-      <c r="Q8" s="17" t="str">
+      <c r="Q8" s="5" t="str">
         <f>Sum(Q2:Q7)</f>
       </c>
-      <c r="R8" s="17" t="str">
+      <c r="R8" s="5" t="str">
         <f>Sum(R2:R7)</f>
       </c>
-      <c r="S8" s="17" t="str">
+      <c r="S8" s="5" t="str">
         <f>Sum(S2:S7)</f>
       </c>
-      <c r="T8" s="17" t="str">
+      <c r="T8" s="5" t="str">
         <f>Sum(T2:T7)</f>
       </c>
-      <c r="U8" s="17" t="str">
+      <c r="U8" s="5" t="str">
         <f>Sum(U2:U7)</f>
       </c>
-      <c r="V8" s="17" t="str">
+      <c r="V8" s="5" t="str">
         <f>Sum(V2:V7)</f>
       </c>
-      <c r="W8" s="17" t="str">
+      <c r="W8" s="5" t="str">
         <f>Sum(W2:W7)</f>
       </c>
-      <c r="X8" s="17" t="str">
+      <c r="X8" s="5" t="str">
         <f>Sum(X2:X7)</f>
       </c>
-      <c r="Y8" s="17" t="str">
+      <c r="Y8" s="5" t="str">
         <f>Sum(Y2:Y7)</f>
       </c>
-      <c r="Z8" s="17" t="str">
+      <c r="Z8" s="5" t="str">
         <f>Sum(Z2:Z7)</f>
       </c>
-      <c r="AA8" s="17" t="str">
+      <c r="AA8" s="5" t="str">
         <f>Sum(AA2:AA7)</f>
       </c>
-      <c r="AB8" s="17" t="str">
+      <c r="AB8" s="5" t="str">
         <f>Sum(AB2:AB7)</f>
       </c>
-      <c r="AC8" s="17" t="str">
+      <c r="AC8" s="5" t="str">
         <f>Sum(AC2:AC7)</f>
       </c>
-      <c r="AD8" s="17" t="str">
+      <c r="AD8" s="5" t="str">
         <f>Sum(AD2:AD7)</f>
       </c>
-      <c r="AE8" s="17" t="str">
+      <c r="AE8" s="5" t="str">
         <f>Sum(AE2:AE7)</f>
       </c>
-      <c r="AF8" s="17" t="str">
+      <c r="AF8" s="5" t="str">
         <f>Sum(AF2:AF7)</f>
       </c>
-      <c r="AG8" s="17" t="str">
+      <c r="AG8" s="5" t="str">
         <f>Sum(AG2:AG7)</f>
       </c>
-      <c r="AH8" s="17" t="str">
+      <c r="AH8" s="5" t="str">
         <f>Sum(AH2:AH7)</f>
       </c>
-      <c r="AI8" s="17" t="str">
+      <c r="AI8" s="5" t="str">
         <f>Sum(AI2:AI7)</f>
       </c>
-      <c r="AJ8" s="17" t="str">
+      <c r="AJ8" s="5" t="str">
         <f>Sum(AJ2:AJ7)</f>
       </c>
-      <c r="AK8" s="17" t="str">
+      <c r="AK8" s="5" t="str">
         <f>Sum(AK2:AK7)</f>
       </c>
-      <c r="AL8" s="17" t="str">
+      <c r="AL8" s="5" t="str">
         <f>Sum(AL2:AL7)</f>
       </c>
-      <c r="AM8" s="17" t="str">
+      <c r="AM8" s="5" t="str">
         <f>Sum(AM2:AM7)</f>
       </c>
-      <c r="AN8" s="17" t="str">
+      <c r="AN8" s="5" t="str">
         <f>Sum(AN2:AN7)</f>
       </c>
-      <c r="AO8" s="17" t="str">
+      <c r="AO8" s="5" t="str">
         <f>Sum(AO2:AO7)</f>
       </c>
-      <c r="AP8" s="17" t="str">
+      <c r="AP8" s="5" t="str">
         <f>Sum(AP2:AP7)</f>
       </c>
-      <c r="AQ8" s="17" t="str">
+      <c r="AQ8" s="5" t="str">
         <f>Sum(AQ2:AQ7)</f>
       </c>
-      <c r="AR8" s="17" t="str">
+      <c r="AR8" s="5" t="str">
         <f>Sum(AR2:AR7)</f>
       </c>
-      <c r="AS8" s="17" t="str">
+      <c r="AS8" s="5" t="str">
         <f>Sum(AS2:AS7)</f>
       </c>
-      <c r="AT8" s="17" t="str">
+      <c r="AT8" s="5" t="str">
         <f>Sum(AT2:AT7)</f>
       </c>
-      <c r="AU8" s="17" t="str">
+      <c r="AU8" s="5" t="str">
         <f>Sum(AU2:AU7)</f>
       </c>
-      <c r="AV8" s="17"/>
+      <c r="AV8" s="5"/>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -10485,16 +10497,16 @@
       <c r="A12" t="str">
         <f>L12</f>
       </c>
-      <c r="B12" s="17" t="str">
+      <c r="B12" s="5" t="str">
         <f>AQ12</f>
       </c>
-      <c r="C12" s="17" t="str">
+      <c r="C12" s="5" t="str">
         <f>AS12</f>
       </c>
-      <c r="D12" s="17" t="str">
+      <c r="D12" s="5" t="str">
         <f>AT12</f>
       </c>
-      <c r="E12" s="17" t="str">
+      <c r="E12" s="5" t="str">
         <f>AU12</f>
       </c>
       <c r="F12" s="1" t="str">
@@ -10515,125 +10527,125 @@
       <c r="L12" t="s">
         <v>117</v>
       </c>
-      <c r="M12" s="17" t="n">
+      <c r="M12" s="5" t="n">
         <v>62034626909.3846</v>
       </c>
-      <c r="N12" s="17" t="n">
+      <c r="N12" s="5" t="n">
         <v>63790986396.3299</v>
       </c>
-      <c r="O12" s="17" t="n">
+      <c r="O12" s="5" t="n">
         <v>57962930142.4092</v>
       </c>
-      <c r="P12" s="17" t="n">
+      <c r="P12" s="5" t="n">
         <v>57764049648.3606</v>
       </c>
-      <c r="Q12" s="17" t="n">
+      <c r="Q12" s="5" t="n">
         <v>59139272094.0376</v>
       </c>
-      <c r="R12" s="17" t="n">
+      <c r="R12" s="5" t="n">
         <v>52518645921.6326</v>
       </c>
-      <c r="S12" s="17" t="n">
+      <c r="S12" s="5" t="n">
         <v>58802303678.2549</v>
       </c>
-      <c r="T12" s="17" t="n">
+      <c r="T12" s="5" t="n">
         <v>60916461069.1388</v>
       </c>
-      <c r="U12" s="17" t="n">
+      <c r="U12" s="5" t="n">
         <v>64785480372.1977</v>
       </c>
-      <c r="V12" s="17" t="n">
+      <c r="V12" s="5" t="n">
         <v>67756525136.607</v>
       </c>
-      <c r="W12" s="17" t="n">
+      <c r="W12" s="5" t="n">
         <v>72127083679.6732</v>
       </c>
-      <c r="X12" s="17" t="n">
+      <c r="X12" s="5" t="n">
         <v>75502662109.3571</v>
       </c>
-      <c r="Y12" s="17" t="n">
+      <c r="Y12" s="5" t="n">
         <v>97358376194.8559</v>
       </c>
-      <c r="Z12" s="17" t="n">
+      <c r="Z12" s="5" t="n">
         <v>111165887815.399</v>
       </c>
-      <c r="AA12" s="17" t="n">
+      <c r="AA12" s="5" t="n">
         <v>112802246479.287</v>
       </c>
-      <c r="AB12" s="17" t="n">
+      <c r="AB12" s="5" t="n">
         <v>111082745340.634</v>
       </c>
-      <c r="AC12" s="17" t="n">
+      <c r="AC12" s="5" t="n">
         <v>128790145385.143</v>
       </c>
-      <c r="AD12" s="17" t="n">
+      <c r="AD12" s="5" t="n">
         <v>140306292668.808</v>
       </c>
-      <c r="AE12" s="17" t="n">
+      <c r="AE12" s="5" t="n">
         <v>146005026305.648</v>
       </c>
-      <c r="AF12" s="17" t="n">
+      <c r="AF12" s="5" t="n">
         <v>147243938932.912</v>
       </c>
-      <c r="AG12" s="17" t="n">
+      <c r="AG12" s="5" t="n">
         <v>131951257583.197</v>
       </c>
-      <c r="AH12" s="17" t="n">
+      <c r="AH12" s="5" t="n">
         <v>146073411885.194</v>
       </c>
-      <c r="AI12" s="17" t="n">
+      <c r="AI12" s="5" t="n">
         <v>138268407453.454</v>
       </c>
-      <c r="AJ12" s="17" t="n">
+      <c r="AJ12" s="5" t="n">
         <v>124858000930.857</v>
       </c>
-      <c r="AK12" s="17" t="n">
+      <c r="AK12" s="5" t="n">
         <v>103697125569.675</v>
       </c>
-      <c r="AL12" s="17" t="n">
+      <c r="AL12" s="5" t="n">
         <v>102717992754.661</v>
       </c>
-      <c r="AM12" s="17" t="n">
+      <c r="AM12" s="5" t="n">
         <v>128019486053.215</v>
       </c>
-      <c r="AN12" s="17" t="n">
+      <c r="AN12" s="5" t="n">
         <v>137693904522.467</v>
       </c>
-      <c r="AO12" s="17" t="n">
+      <c r="AO12" s="5" t="n">
         <v>135036560825.555</v>
       </c>
-      <c r="AP12" s="17" t="n">
+      <c r="AP12" s="5" t="n">
         <v>144548325327.103</v>
       </c>
-      <c r="AQ12" s="17" t="n">
+      <c r="AQ12" s="5" t="n">
         <v>177324883403.893</v>
       </c>
-      <c r="AR12" s="17" t="n">
+      <c r="AR12" s="5" t="n">
         <v>127957170157.387</v>
       </c>
-      <c r="AS12" s="17" t="n">
+      <c r="AS12" s="5" t="n">
         <v>127899803920.975</v>
       </c>
-      <c r="AT12" s="17" t="n">
+      <c r="AT12" s="5" t="n">
         <v>84663692097.9125</v>
       </c>
-      <c r="AU12" s="17"/>
-      <c r="AV12" s="17"/>
+      <c r="AU12" s="5"/>
+      <c r="AV12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" t="str">
         <f>L13</f>
       </c>
-      <c r="B13" s="17" t="str">
+      <c r="B13" s="5" t="str">
         <f>AQ13</f>
       </c>
-      <c r="C13" s="17" t="str">
+      <c r="C13" s="5" t="str">
         <f>AS13</f>
       </c>
-      <c r="D13" s="17" t="str">
+      <c r="D13" s="5" t="str">
         <f>AT13</f>
       </c>
-      <c r="E13" s="17" t="str">
+      <c r="E13" s="5" t="str">
         <f>AU13</f>
       </c>
       <c r="F13" s="1" t="str">
@@ -10654,125 +10666,125 @@
       <c r="L13" t="s">
         <v>118</v>
       </c>
-      <c r="M13" s="17" t="n">
+      <c r="M13" s="5" t="n">
         <v>74376855686.8564</v>
       </c>
-      <c r="N13" s="17" t="n">
+      <c r="N13" s="5" t="n">
         <v>75609327836.971</v>
       </c>
-      <c r="O13" s="17" t="n">
+      <c r="O13" s="5" t="n">
         <v>68365745489.2242</v>
       </c>
-      <c r="P13" s="17" t="n">
+      <c r="P13" s="5" t="n">
         <v>64393165484.7675</v>
       </c>
-      <c r="Q13" s="17" t="n">
+      <c r="Q13" s="5" t="n">
         <v>57979424506.3217</v>
       </c>
-      <c r="R13" s="17" t="n">
+      <c r="R13" s="5" t="n">
         <v>52052563756.1149</v>
       </c>
-      <c r="S13" s="17" t="n">
+      <c r="S13" s="5" t="n">
         <v>54059877517.4901</v>
       </c>
-      <c r="T13" s="17" t="n">
+      <c r="T13" s="5" t="n">
         <v>51146014246.0563</v>
       </c>
-      <c r="U13" s="17" t="n">
+      <c r="U13" s="5" t="n">
         <v>48874011250.5904</v>
       </c>
-      <c r="V13" s="17" t="n">
+      <c r="V13" s="5" t="n">
         <v>50930892486.7369</v>
       </c>
-      <c r="W13" s="17" t="n">
+      <c r="W13" s="5" t="n">
         <v>40919231964.1599</v>
       </c>
-      <c r="X13" s="17" t="n">
+      <c r="X13" s="5" t="n">
         <v>42131241533.5398</v>
       </c>
-      <c r="Y13" s="17" t="n">
+      <c r="Y13" s="5" t="n">
         <v>52985798997.8947</v>
       </c>
-      <c r="Z13" s="17" t="n">
+      <c r="Z13" s="5" t="n">
         <v>75837390269.9635</v>
       </c>
-      <c r="AA13" s="17" t="n">
+      <c r="AA13" s="5" t="n">
         <v>91046302747.067</v>
       </c>
-      <c r="AB13" s="17" t="n">
+      <c r="AB13" s="5" t="n">
         <v>97795480451.7547</v>
       </c>
-      <c r="AC13" s="17" t="n">
+      <c r="AC13" s="5" t="n">
         <v>99675328640.5298</v>
       </c>
-      <c r="AD13" s="17" t="n">
+      <c r="AD13" s="5" t="n">
         <v>117242255084.356</v>
       </c>
-      <c r="AE13" s="17" t="n">
+      <c r="AE13" s="5" t="n">
         <v>141384761441.279</v>
       </c>
-      <c r="AF13" s="17" t="n">
+      <c r="AF13" s="5" t="n">
         <v>125052072428.137</v>
       </c>
-      <c r="AG13" s="17" t="n">
+      <c r="AG13" s="5" t="n">
         <v>145271725273.345</v>
       </c>
-      <c r="AH13" s="17" t="n">
+      <c r="AH13" s="5" t="n">
         <v>137953263016.154</v>
       </c>
-      <c r="AI13" s="17" t="n">
+      <c r="AI13" s="5" t="n">
         <v>128787082296.679</v>
       </c>
-      <c r="AJ13" s="17" t="n">
+      <c r="AJ13" s="5" t="n">
         <v>111268524686.888</v>
       </c>
-      <c r="AK13" s="17" t="n">
+      <c r="AK13" s="5" t="n">
         <v>97604218690.3479</v>
       </c>
-      <c r="AL13" s="17" t="n">
+      <c r="AL13" s="5" t="n">
         <v>90084356709.3377</v>
       </c>
-      <c r="AM13" s="17" t="n">
+      <c r="AM13" s="5" t="n">
         <v>88817296636.4034</v>
       </c>
-      <c r="AN13" s="17" t="n">
+      <c r="AN13" s="5" t="n">
         <v>93544536959.2909</v>
       </c>
-      <c r="AO13" s="17" t="n">
+      <c r="AO13" s="5" t="n">
         <v>105922564652.665</v>
       </c>
-      <c r="AP13" s="17" t="n">
+      <c r="AP13" s="5" t="n">
         <v>108764796830.682</v>
       </c>
-      <c r="AQ13" s="17" t="n">
+      <c r="AQ13" s="5" t="n">
         <v>113885383957.206</v>
       </c>
-      <c r="AR13" s="17" t="n">
+      <c r="AR13" s="5" t="n">
         <v>101561084611.461</v>
       </c>
-      <c r="AS13" s="17" t="n">
+      <c r="AS13" s="5" t="n">
         <v>103551009104.182</v>
       </c>
-      <c r="AT13" s="17" t="n">
+      <c r="AT13" s="5" t="n">
         <v>48591295833.2184</v>
       </c>
-      <c r="AU13" s="17"/>
-      <c r="AV13" s="17"/>
+      <c r="AU13" s="5"/>
+      <c r="AV13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" t="str">
         <f>L14</f>
       </c>
-      <c r="B14" s="17" t="str">
+      <c r="B14" s="5" t="str">
         <f>AQ14</f>
       </c>
-      <c r="C14" s="17" t="str">
+      <c r="C14" s="5" t="str">
         <f>AS14</f>
       </c>
-      <c r="D14" s="17" t="str">
+      <c r="D14" s="5" t="str">
         <f>AT14</f>
       </c>
-      <c r="E14" s="17" t="str">
+      <c r="E14" s="5" t="str">
         <f>AU14</f>
       </c>
       <c r="F14" s="1" t="str">
@@ -10793,105 +10805,105 @@
       <c r="L14" t="s">
         <v>119</v>
       </c>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="17" t="n">
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5" t="n">
         <v>51914023984.1129</v>
       </c>
-      <c r="X14" s="17" t="n">
+      <c r="X14" s="5" t="n">
         <v>47585332084.2751</v>
       </c>
-      <c r="Y14" s="17" t="n">
+      <c r="Y14" s="5" t="n">
         <v>48661922653.0792</v>
       </c>
-      <c r="Z14" s="17" t="n">
+      <c r="Z14" s="5" t="n">
         <v>55813043669.3161</v>
       </c>
-      <c r="AA14" s="17" t="n">
+      <c r="AA14" s="5" t="n">
         <v>54544248301.3675</v>
       </c>
-      <c r="AB14" s="17" t="n">
+      <c r="AB14" s="5" t="n">
         <v>62898562579.644</v>
       </c>
-      <c r="AC14" s="17" t="n">
+      <c r="AC14" s="5" t="n">
         <v>71553807395.8195</v>
       </c>
-      <c r="AD14" s="17" t="n">
+      <c r="AD14" s="5" t="n">
         <v>65522580441.1321</v>
       </c>
-      <c r="AE14" s="17" t="n">
+      <c r="AE14" s="5" t="n">
         <v>74915123990.4629</v>
       </c>
-      <c r="AF14" s="17" t="n">
+      <c r="AF14" s="5" t="n">
         <v>65474611018.2892</v>
       </c>
-      <c r="AG14" s="17" t="n">
+      <c r="AG14" s="5" t="n">
         <v>53629992604.6535</v>
       </c>
-      <c r="AH14" s="17" t="n">
+      <c r="AH14" s="5" t="n">
         <v>50805302968.8263</v>
       </c>
-      <c r="AI14" s="17" t="n">
+      <c r="AI14" s="5" t="n">
         <v>55426974806.1554</v>
       </c>
-      <c r="AJ14" s="17" t="n">
+      <c r="AJ14" s="5" t="n">
         <v>41510500238.7463</v>
       </c>
-      <c r="AK14" s="17" t="n">
+      <c r="AK14" s="5" t="n">
         <v>39565176702.2284</v>
       </c>
-      <c r="AL14" s="17" t="n">
+      <c r="AL14" s="5" t="n">
         <v>35668165841.7306</v>
       </c>
-      <c r="AM14" s="17" t="n">
+      <c r="AM14" s="5" t="n">
         <v>33247309446.9647</v>
       </c>
-      <c r="AN14" s="17" t="n">
+      <c r="AN14" s="5" t="n">
         <v>35502337706.9848</v>
       </c>
-      <c r="AO14" s="17" t="n">
+      <c r="AO14" s="5" t="n">
         <v>40408269319.5754</v>
       </c>
-      <c r="AP14" s="17" t="n">
+      <c r="AP14" s="5" t="n">
         <v>42017742648.7726</v>
       </c>
-      <c r="AQ14" s="17" t="n">
+      <c r="AQ14" s="5" t="n">
         <v>39358469655.472</v>
       </c>
-      <c r="AR14" s="17" t="n">
+      <c r="AR14" s="5" t="n">
         <v>58356968436.524</v>
       </c>
-      <c r="AS14" s="17" t="n">
+      <c r="AS14" s="5" t="n">
         <v>53062498640.4436</v>
       </c>
-      <c r="AT14" s="17" t="n">
+      <c r="AT14" s="5" t="n">
         <v>20342650358.8622</v>
       </c>
-      <c r="AU14" s="17"/>
-      <c r="AV14" s="17"/>
+      <c r="AU14" s="5"/>
+      <c r="AV14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" t="str">
         <f>L15</f>
       </c>
-      <c r="B15" s="17" t="str">
+      <c r="B15" s="5" t="str">
         <f>AQ15</f>
       </c>
-      <c r="C15" s="17" t="str">
+      <c r="C15" s="5" t="str">
         <f>AS15</f>
       </c>
-      <c r="D15" s="17" t="str">
+      <c r="D15" s="5" t="str">
         <f>AT15</f>
       </c>
-      <c r="E15" s="17" t="str">
+      <c r="E15" s="5" t="str">
         <f>AU15</f>
       </c>
       <c r="F15" s="1" t="str">
@@ -10912,125 +10924,125 @@
       <c r="L15" t="s">
         <v>120</v>
       </c>
-      <c r="M15" s="17" t="n">
+      <c r="M15" s="5" t="n">
         <v>58541818060.9403</v>
       </c>
-      <c r="N15" s="17" t="n">
+      <c r="N15" s="5" t="n">
         <v>82358489914.1844</v>
       </c>
-      <c r="O15" s="17" t="n">
+      <c r="O15" s="5" t="n">
         <v>68096966520.7576</v>
       </c>
-      <c r="P15" s="17" t="n">
+      <c r="P15" s="5" t="n">
         <v>64632063468.1008</v>
       </c>
-      <c r="Q15" s="17" t="n">
+      <c r="Q15" s="5" t="n">
         <v>59957666520.7577</v>
       </c>
-      <c r="R15" s="17" t="n">
+      <c r="R15" s="5" t="n">
         <v>64189328824.463</v>
       </c>
-      <c r="S15" s="17" t="n">
+      <c r="S15" s="5" t="n">
         <v>54205924949.7956</v>
       </c>
-      <c r="T15" s="17" t="n">
+      <c r="T15" s="5" t="n">
         <v>53213047231.7927</v>
       </c>
-      <c r="U15" s="17" t="n">
+      <c r="U15" s="5" t="n">
         <v>52818819697.6635</v>
       </c>
-      <c r="V15" s="17" t="n">
+      <c r="V15" s="5" t="n">
         <v>55880047192.9175</v>
       </c>
-      <c r="W15" s="17" t="n">
+      <c r="W15" s="5" t="n">
         <v>21118893847.9738</v>
       </c>
-      <c r="X15" s="17" t="n">
+      <c r="X15" s="5" t="n">
         <v>33445537148.3718</v>
       </c>
-      <c r="Y15" s="17" t="n">
+      <c r="Y15" s="5" t="n">
         <v>30862208925.3496</v>
       </c>
-      <c r="Z15" s="17" t="n">
+      <c r="Z15" s="5" t="n">
         <v>39914389553.9664</v>
       </c>
-      <c r="AA15" s="17" t="n">
+      <c r="AA15" s="5" t="n">
         <v>40845534598.3846</v>
       </c>
-      <c r="AB15" s="17" t="n">
+      <c r="AB15" s="5" t="n">
         <v>51540784050.8128</v>
       </c>
-      <c r="AC15" s="17" t="n">
+      <c r="AC15" s="5" t="n">
         <v>52812609367.5539</v>
       </c>
-      <c r="AD15" s="17" t="n">
+      <c r="AD15" s="5" t="n">
         <v>61283857639.0038</v>
       </c>
-      <c r="AE15" s="17" t="n">
+      <c r="AE15" s="5" t="n">
         <v>72570879483.6226</v>
       </c>
-      <c r="AF15" s="17" t="n">
+      <c r="AF15" s="5" t="n">
         <v>77489428838.2428</v>
       </c>
-      <c r="AG15" s="17" t="n">
+      <c r="AG15" s="5" t="n">
         <v>76965085505.2447</v>
       </c>
-      <c r="AH15" s="17" t="n">
+      <c r="AH15" s="5" t="n">
         <v>76535560110.3393</v>
       </c>
-      <c r="AI15" s="17" t="n">
+      <c r="AI15" s="5" t="n">
         <v>69110303647.0819</v>
       </c>
-      <c r="AJ15" s="17" t="n">
+      <c r="AJ15" s="5" t="n">
         <v>56385392006.5785</v>
       </c>
-      <c r="AK15" s="17" t="n">
+      <c r="AK15" s="5" t="n">
         <v>49199810577.0402</v>
       </c>
-      <c r="AL15" s="17" t="n">
+      <c r="AL15" s="5" t="n">
         <v>47925200385.9804</v>
       </c>
-      <c r="AM15" s="17" t="n">
+      <c r="AM15" s="5" t="n">
         <v>49307255853.4869</v>
       </c>
-      <c r="AN15" s="17" t="n">
+      <c r="AN15" s="5" t="n">
         <v>53219174134.7063</v>
       </c>
-      <c r="AO15" s="17" t="n">
+      <c r="AO15" s="5" t="n">
         <v>62026880850.333</v>
       </c>
-      <c r="AP15" s="17" t="n">
+      <c r="AP15" s="5" t="n">
         <v>67583747947.7055</v>
       </c>
-      <c r="AQ15" s="17" t="n">
+      <c r="AQ15" s="5" t="n">
         <v>70107100474.2631</v>
       </c>
-      <c r="AR15" s="17" t="n">
+      <c r="AR15" s="5" t="n">
         <v>61961489720.3226</v>
       </c>
-      <c r="AS15" s="17" t="n">
+      <c r="AS15" s="5" t="n">
         <v>40798916792.3185</v>
       </c>
-      <c r="AT15" s="17" t="n">
+      <c r="AT15" s="5" t="n">
         <v>17449481642.3526</v>
       </c>
-      <c r="AU15" s="17"/>
-      <c r="AV15" s="17"/>
+      <c r="AU15" s="5"/>
+      <c r="AV15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" t="str">
         <f>L16</f>
       </c>
-      <c r="B16" s="17" t="str">
+      <c r="B16" s="5" t="str">
         <f>AQ16</f>
       </c>
-      <c r="C16" s="17" t="str">
+      <c r="C16" s="5" t="str">
         <f>AS16</f>
       </c>
-      <c r="D16" s="17" t="str">
+      <c r="D16" s="5" t="str">
         <f>AT16</f>
       </c>
-      <c r="E16" s="17" t="str">
+      <c r="E16" s="5" t="str">
         <f>AU16</f>
       </c>
       <c r="F16" s="1" t="str">
@@ -11051,125 +11063,125 @@
       <c r="L16" t="s">
         <v>121</v>
       </c>
-      <c r="M16" s="17" t="n">
+      <c r="M16" s="5" t="n">
         <v>27786130239.0766</v>
       </c>
-      <c r="N16" s="17" t="n">
+      <c r="N16" s="5" t="n">
         <v>38678163233.7772</v>
       </c>
-      <c r="O16" s="17" t="n">
+      <c r="O16" s="5" t="n">
         <v>34324599391.722</v>
       </c>
-      <c r="P16" s="17" t="n">
+      <c r="P16" s="5" t="n">
         <v>33588238640.2068</v>
       </c>
-      <c r="Q16" s="17" t="n">
+      <c r="Q16" s="5" t="n">
         <v>33672062929.3893</v>
       </c>
-      <c r="R16" s="17" t="n">
+      <c r="R16" s="5" t="n">
         <v>34733440093.1433</v>
       </c>
-      <c r="S16" s="17" t="n">
+      <c r="S16" s="5" t="n">
         <v>34639717467.2126</v>
       </c>
-      <c r="T16" s="17" t="n">
+      <c r="T16" s="5" t="n">
         <v>31550017536.8974</v>
       </c>
-      <c r="U16" s="17" t="n">
+      <c r="U16" s="5" t="n">
         <v>30036834323.6961</v>
       </c>
-      <c r="V16" s="17" t="n">
+      <c r="V16" s="5" t="n">
         <v>32629484716.7365</v>
       </c>
-      <c r="W16" s="17" t="n">
+      <c r="W16" s="5" t="n">
         <v>34628198430.6147</v>
       </c>
-      <c r="X16" s="17" t="n">
+      <c r="X16" s="5" t="n">
         <v>35497323370.5492</v>
       </c>
-      <c r="Y16" s="17" t="n">
+      <c r="Y16" s="5" t="n">
         <v>41996343802.0963</v>
       </c>
-      <c r="Z16" s="17" t="n">
+      <c r="Z16" s="5" t="n">
         <v>51536080977.4146</v>
       </c>
-      <c r="AA16" s="17" t="n">
+      <c r="AA16" s="5" t="n">
         <v>53549946906.4653</v>
       </c>
-      <c r="AB16" s="17" t="n">
+      <c r="AB16" s="5" t="n">
         <v>65091364654.3129</v>
       </c>
-      <c r="AC16" s="17" t="n">
+      <c r="AC16" s="5" t="n">
         <v>66247930939.3818</v>
       </c>
-      <c r="AD16" s="17" t="n">
+      <c r="AD16" s="5" t="n">
         <v>70508766475.1082</v>
       </c>
-      <c r="AE16" s="17" t="n">
+      <c r="AE16" s="5" t="n">
         <v>76235566435.774</v>
       </c>
-      <c r="AF16" s="17" t="n">
+      <c r="AF16" s="5" t="n">
         <v>81368294817.5627</v>
       </c>
-      <c r="AG16" s="17" t="n">
+      <c r="AG16" s="5" t="n">
         <v>79325363637.2335</v>
       </c>
-      <c r="AH16" s="17" t="n">
+      <c r="AH16" s="5" t="n">
         <v>75138348079.497</v>
       </c>
-      <c r="AI16" s="17" t="n">
+      <c r="AI16" s="5" t="n">
         <v>73743808595.2994</v>
       </c>
-      <c r="AJ16" s="17" t="n">
+      <c r="AJ16" s="5" t="n">
         <v>61038903384.6493</v>
       </c>
-      <c r="AK16" s="17" t="n">
+      <c r="AK16" s="5" t="n">
         <v>67612219121.5487</v>
       </c>
-      <c r="AL16" s="17" t="n">
+      <c r="AL16" s="5" t="n">
         <v>65598387053.1957</v>
       </c>
-      <c r="AM16" s="17" t="n">
+      <c r="AM16" s="5" t="n">
         <v>70086271269.9855</v>
       </c>
-      <c r="AN16" s="17" t="n">
+      <c r="AN16" s="5" t="n">
         <v>72316770012.4619</v>
       </c>
-      <c r="AO16" s="17" t="n">
+      <c r="AO16" s="5" t="n">
         <v>83911453108.4576</v>
       </c>
-      <c r="AP16" s="17" t="n">
+      <c r="AP16" s="5" t="n">
         <v>86008895708.1413</v>
       </c>
-      <c r="AQ16" s="17" t="n">
+      <c r="AQ16" s="5" t="n">
         <v>87728634988.71</v>
       </c>
-      <c r="AR16" s="17" t="n">
+      <c r="AR16" s="5" t="n">
         <v>83126463857.007</v>
       </c>
-      <c r="AS16" s="17" t="n">
+      <c r="AS16" s="5" t="n">
         <v>85408890581.307</v>
       </c>
-      <c r="AT16" s="17" t="n">
+      <c r="AT16" s="5" t="n">
         <v>32808828005.7754</v>
       </c>
-      <c r="AU16" s="17"/>
-      <c r="AV16" s="17"/>
+      <c r="AU16" s="5"/>
+      <c r="AV16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" t="str">
         <f>L17</f>
       </c>
-      <c r="B17" s="17" t="str">
+      <c r="B17" s="5" t="str">
         <f>AQ17</f>
       </c>
-      <c r="C17" s="17" t="str">
+      <c r="C17" s="5" t="str">
         <f>AS17</f>
       </c>
-      <c r="D17" s="17" t="str">
+      <c r="D17" s="5" t="str">
         <f>AT17</f>
       </c>
-      <c r="E17" s="17" t="str">
+      <c r="E17" s="5" t="str">
         <f>AU17</f>
       </c>
       <c r="F17" s="1" t="str">
@@ -11188,125 +11200,125 @@
         <f>AU17/Sum(AU11:AU$17)</f>
       </c>
       <c r="L17"/>
-      <c r="M17" s="17" t="n">
+      <c r="M17" s="5" t="n">
         <v>26178567894.6163</v>
       </c>
-      <c r="N17" s="17" t="n">
+      <c r="N17" s="5" t="n">
         <v>11448235338.8668</v>
       </c>
-      <c r="O17" s="17" t="n">
+      <c r="O17" s="5" t="n">
         <v>11662319190.8258</v>
       </c>
-      <c r="P17" s="17" t="n">
+      <c r="P17" s="5" t="n">
         <v>10653961870.5513</v>
       </c>
-      <c r="Q17" s="17" t="n">
+      <c r="Q17" s="5" t="n">
         <v>7502046599.57892</v>
       </c>
-      <c r="R17" s="17" t="n">
+      <c r="R17" s="5" t="n">
         <v>9183655382.24917</v>
       </c>
-      <c r="S17" s="17" t="n">
+      <c r="S17" s="5" t="n">
         <v>10363787716.0805</v>
       </c>
-      <c r="T17" s="17" t="n">
+      <c r="T17" s="5" t="n">
         <v>7208777329.09415</v>
       </c>
-      <c r="U17" s="17" t="n">
+      <c r="U17" s="5" t="n">
         <v>6701837669.3367</v>
       </c>
-      <c r="V17" s="17" t="n">
+      <c r="V17" s="5" t="n">
         <v>2491331032.40164</v>
       </c>
-      <c r="W17" s="17" t="n">
+      <c r="W17" s="5" t="n">
         <v>1507522520.45657</v>
       </c>
-      <c r="X17" s="17" t="n">
+      <c r="X17" s="5" t="n">
         <v>2187284642.71751</v>
       </c>
-      <c r="Y17" s="17" t="n">
+      <c r="Y17" s="5" t="n">
         <v>2543217067.50809</v>
       </c>
-      <c r="Z17" s="17" t="n">
+      <c r="Z17" s="5" t="n">
         <v>1125387878.44821</v>
       </c>
-      <c r="AA17" s="17" t="n">
+      <c r="AA17" s="5" t="n">
         <v>2842989329.51089</v>
       </c>
-      <c r="AB17" s="17" t="n">
+      <c r="AB17" s="5" t="n">
         <v>10627211754.3237</v>
       </c>
-      <c r="AC17" s="17" t="n">
+      <c r="AC17" s="5" t="n">
         <v>10318513183.6995</v>
       </c>
-      <c r="AD17" s="17" t="n">
+      <c r="AD17" s="5" t="n">
         <v>9736229219.25512</v>
       </c>
-      <c r="AE17" s="17" t="n">
+      <c r="AE17" s="5" t="n">
         <v>13158675858.7299</v>
       </c>
-      <c r="AF17" s="17" t="n">
+      <c r="AF17" s="5" t="n">
         <v>8141010249.1165</v>
       </c>
-      <c r="AG17" s="17" t="n">
+      <c r="AG17" s="5" t="n">
         <v>6549069227.86101</v>
       </c>
-      <c r="AH17" s="17" t="n">
+      <c r="AH17" s="5" t="n">
         <v>5301786294.48572</v>
       </c>
-      <c r="AI17" s="17" t="n">
+      <c r="AI17" s="5" t="n">
         <v>3590079460.95946</v>
       </c>
-      <c r="AJ17" s="17" t="n">
+      <c r="AJ17" s="5" t="n">
         <v>1705971740.16503</v>
       </c>
-      <c r="AK17" s="17" t="n">
+      <c r="AK17" s="5" t="n">
         <v>654973399.55614</v>
       </c>
-      <c r="AL17" s="17" t="n">
+      <c r="AL17" s="5" t="n">
         <v>1125999236.13021</v>
       </c>
-      <c r="AM17" s="17" t="n">
+      <c r="AM17" s="5" t="n">
         <v>1082876260.07676</v>
       </c>
-      <c r="AN17" s="17" t="n">
+      <c r="AN17" s="5" t="n">
         <v>611768960.153919</v>
       </c>
-      <c r="AO17" s="17" t="n">
+      <c r="AO17" s="5" t="n">
         <v>1205241769.09887</v>
       </c>
-      <c r="AP17" s="17" t="n">
+      <c r="AP17" s="5" t="n">
         <v>1291692814.35443</v>
       </c>
-      <c r="AQ17" s="17" t="n">
+      <c r="AQ17" s="5" t="n">
         <v>879731420.951674</v>
       </c>
-      <c r="AR17" s="17" t="n">
+      <c r="AR17" s="5" t="n">
         <v>830719687.564062</v>
       </c>
-      <c r="AS17" s="17" t="n">
+      <c r="AS17" s="5" t="n">
         <v>22736599181.9227</v>
       </c>
-      <c r="AT17" s="17" t="n">
+      <c r="AT17" s="5" t="n">
         <v>13529156156.6481</v>
       </c>
-      <c r="AU17" s="17"/>
-      <c r="AV17" s="17"/>
+      <c r="AU17" s="5"/>
+      <c r="AV17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" t="str">
         <f>L18</f>
       </c>
-      <c r="B18" s="17" t="str">
+      <c r="B18" s="5" t="str">
         <f>AQ18</f>
       </c>
-      <c r="C18" s="17" t="str">
+      <c r="C18" s="5" t="str">
         <f>AS18</f>
       </c>
-      <c r="D18" s="17" t="str">
+      <c r="D18" s="5" t="str">
         <f>AT18</f>
       </c>
-      <c r="E18" s="17" t="str">
+      <c r="E18" s="5" t="str">
         <f>AU18</f>
       </c>
       <c r="F18" s="1" t="str">
@@ -11327,112 +11339,112 @@
       <c r="L18" t="s">
         <v>46</v>
       </c>
-      <c r="M18" s="17" t="str">
+      <c r="M18" s="5" t="str">
         <f>Sum(M12:M17)</f>
       </c>
-      <c r="N18" s="17" t="str">
+      <c r="N18" s="5" t="str">
         <f>Sum(N12:N17)</f>
       </c>
-      <c r="O18" s="17" t="str">
+      <c r="O18" s="5" t="str">
         <f>Sum(O12:O17)</f>
       </c>
-      <c r="P18" s="17" t="str">
+      <c r="P18" s="5" t="str">
         <f>Sum(P12:P17)</f>
       </c>
-      <c r="Q18" s="17" t="str">
+      <c r="Q18" s="5" t="str">
         <f>Sum(Q12:Q17)</f>
       </c>
-      <c r="R18" s="17" t="str">
+      <c r="R18" s="5" t="str">
         <f>Sum(R12:R17)</f>
       </c>
-      <c r="S18" s="17" t="str">
+      <c r="S18" s="5" t="str">
         <f>Sum(S12:S17)</f>
       </c>
-      <c r="T18" s="17" t="str">
+      <c r="T18" s="5" t="str">
         <f>Sum(T12:T17)</f>
       </c>
-      <c r="U18" s="17" t="str">
+      <c r="U18" s="5" t="str">
         <f>Sum(U12:U17)</f>
       </c>
-      <c r="V18" s="17" t="str">
+      <c r="V18" s="5" t="str">
         <f>Sum(V12:V17)</f>
       </c>
-      <c r="W18" s="17" t="str">
+      <c r="W18" s="5" t="str">
         <f>Sum(W12:W17)</f>
       </c>
-      <c r="X18" s="17" t="str">
+      <c r="X18" s="5" t="str">
         <f>Sum(X12:X17)</f>
       </c>
-      <c r="Y18" s="17" t="str">
+      <c r="Y18" s="5" t="str">
         <f>Sum(Y12:Y17)</f>
       </c>
-      <c r="Z18" s="17" t="str">
+      <c r="Z18" s="5" t="str">
         <f>Sum(Z12:Z17)</f>
       </c>
-      <c r="AA18" s="17" t="str">
+      <c r="AA18" s="5" t="str">
         <f>Sum(AA12:AA17)</f>
       </c>
-      <c r="AB18" s="17" t="str">
+      <c r="AB18" s="5" t="str">
         <f>Sum(AB12:AB17)</f>
       </c>
-      <c r="AC18" s="17" t="str">
+      <c r="AC18" s="5" t="str">
         <f>Sum(AC12:AC17)</f>
       </c>
-      <c r="AD18" s="17" t="str">
+      <c r="AD18" s="5" t="str">
         <f>Sum(AD12:AD17)</f>
       </c>
-      <c r="AE18" s="17" t="str">
+      <c r="AE18" s="5" t="str">
         <f>Sum(AE12:AE17)</f>
       </c>
-      <c r="AF18" s="17" t="str">
+      <c r="AF18" s="5" t="str">
         <f>Sum(AF12:AF17)</f>
       </c>
-      <c r="AG18" s="17" t="str">
+      <c r="AG18" s="5" t="str">
         <f>Sum(AG12:AG17)</f>
       </c>
-      <c r="AH18" s="17" t="str">
+      <c r="AH18" s="5" t="str">
         <f>Sum(AH12:AH17)</f>
       </c>
-      <c r="AI18" s="17" t="str">
+      <c r="AI18" s="5" t="str">
         <f>Sum(AI12:AI17)</f>
       </c>
-      <c r="AJ18" s="17" t="str">
+      <c r="AJ18" s="5" t="str">
         <f>Sum(AJ12:AJ17)</f>
       </c>
-      <c r="AK18" s="17" t="str">
+      <c r="AK18" s="5" t="str">
         <f>Sum(AK12:AK17)</f>
       </c>
-      <c r="AL18" s="17" t="str">
+      <c r="AL18" s="5" t="str">
         <f>Sum(AL12:AL17)</f>
       </c>
-      <c r="AM18" s="17" t="str">
+      <c r="AM18" s="5" t="str">
         <f>Sum(AM12:AM17)</f>
       </c>
-      <c r="AN18" s="17" t="str">
+      <c r="AN18" s="5" t="str">
         <f>Sum(AN12:AN17)</f>
       </c>
-      <c r="AO18" s="17" t="str">
+      <c r="AO18" s="5" t="str">
         <f>Sum(AO12:AO17)</f>
       </c>
-      <c r="AP18" s="17" t="str">
+      <c r="AP18" s="5" t="str">
         <f>Sum(AP12:AP17)</f>
       </c>
-      <c r="AQ18" s="17" t="str">
+      <c r="AQ18" s="5" t="str">
         <f>Sum(AQ12:AQ17)</f>
       </c>
-      <c r="AR18" s="17" t="str">
+      <c r="AR18" s="5" t="str">
         <f>Sum(AR12:AR17)</f>
       </c>
-      <c r="AS18" s="17" t="str">
+      <c r="AS18" s="5" t="str">
         <f>Sum(AS12:AS17)</f>
       </c>
-      <c r="AT18" s="17" t="str">
+      <c r="AT18" s="5" t="str">
         <f>Sum(AT12:AT17)</f>
       </c>
-      <c r="AU18" s="17" t="str">
+      <c r="AU18" s="5" t="str">
         <f>Sum(AU12:AU17)</f>
       </c>
-      <c r="AV18" s="17"/>
+      <c r="AV18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>